<commit_message>
Fix little issues and a few warnings(?)
</commit_message>
<xml_diff>
--- a/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
+++ b/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="Workbook_______"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Common\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Domain\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06E7FA3-575E-4F77-8736-6CAA3373E33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722F7443-E9EB-4212-898D-CA8458B1C560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="FIELD_NUMBER_NAMES" localSheetId="0">Відомість!$B$20</definedName>
-    <definedName name="FIELD_RANGE_0" localSheetId="0">Відомість!$F$4</definedName>
+    <definedName name="FIELD_RANGE_0" localSheetId="0">Відомість!$C$4</definedName>
     <definedName name="FIELD_RANGE_1" localSheetId="0">Відомість!$A$3</definedName>
     <definedName name="FIELD_RANGE_10" localSheetId="0">Відомість!$J$38</definedName>
     <definedName name="FIELD_RANGE_11" localSheetId="0">Відомість!$C$39</definedName>
@@ -311,9 +311,6 @@
     <t>[COMMANDER_RANK]</t>
   </si>
   <si>
-    <t>визначення залишкової вартості майна [SERVICE_NAME] станом на ___.___.20___ року</t>
-  </si>
-  <si>
     <t>визначила залишкову вартість майна [SERVICE_NAME]</t>
   </si>
   <si>
@@ -342,6 +339,9 @@
   </si>
   <si>
     <t>[UNIT_EDRPOU]</t>
+  </si>
+  <si>
+    <t>визначення залишкової вартості майна [SERVICE_NAME] станом на [REPORT_DATE] року</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -848,11 +848,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -877,9 +903,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -993,68 +1016,46 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1087,40 +1088,72 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1896,8 +1929,8 @@
   </sheetPr>
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1977,13 +2010,13 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="72"/>
+      <c r="B3" s="80"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="E3" s="100"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -2007,16 +2040,15 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="10" t="s">
-        <v>61</v>
+      <c r="B4" s="80"/>
+      <c r="C4" s="98" t="s">
+        <v>60</v>
       </c>
+      <c r="D4" s="99"/>
+      <c r="E4" s="101"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2043,7 +2075,7 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="E5" s="100"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -2067,292 +2099,292 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" spans="1:26" ht="18" customHeight="1">
-      <c r="A6" s="74"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="52" t="s">
+      <c r="A6" s="82"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="18" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="J7" s="52" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="J7" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="18" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="J8" s="53" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="J8" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="54" t="s">
+      <c r="K8" s="83"/>
+      <c r="L8" s="83"/>
+      <c r="M8" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
+      <c r="N8" s="84"/>
+      <c r="O8" s="84"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="24.75" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="J9" s="52" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="J9" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
     </row>
     <row r="10" spans="1:26" ht="18" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="8"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="18" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
     </row>
     <row r="12" spans="1:26" ht="18" customHeight="1">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="90" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="90"/>
+      <c r="O12" s="90"/>
+      <c r="Q12" s="11"/>
+    </row>
+    <row r="13" spans="1:26" ht="18" customHeight="1">
+      <c r="A13" s="91" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="91"/>
+      <c r="M13" s="91"/>
+      <c r="N13" s="91"/>
+      <c r="O13" s="91"/>
+      <c r="Q13" s="11"/>
+    </row>
+    <row r="14" spans="1:26" ht="18" customHeight="1">
+      <c r="A14" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
-      <c r="Q12" s="12"/>
-    </row>
-    <row r="13" spans="1:26" ht="18" customHeight="1">
-      <c r="A13" s="62" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-      <c r="Q13" s="12"/>
-    </row>
-    <row r="14" spans="1:26" ht="18" customHeight="1">
-      <c r="A14" s="69" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="69"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="70"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="12"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="96"/>
+      <c r="N14" s="96"/>
+      <c r="O14" s="97"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:26" ht="81.75" customHeight="1">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="63" t="s">
+      <c r="F15" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="63" t="s">
+      <c r="G15" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="55" t="s">
+      <c r="H15" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="66" t="s">
+      <c r="I15" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="63" t="s">
+      <c r="J15" s="94"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="57" t="s">
+      <c r="N15" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="O15" s="59" t="s">
+      <c r="O15" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="P15" s="14"/>
+      <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="24" customHeight="1">
-      <c r="A16" s="64"/>
-      <c r="B16" s="64"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="92"/>
       <c r="C16" s="65"/>
       <c r="D16" s="65"/>
       <c r="E16" s="65"/>
       <c r="F16" s="65"/>
       <c r="G16" s="65"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="15" t="s">
+      <c r="H16" s="86"/>
+      <c r="I16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="14" t="s">
         <v>15</v>
       </c>
       <c r="M16" s="65"/>
-      <c r="N16" s="58"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="14"/>
+      <c r="N16" s="88"/>
+      <c r="O16" s="89"/>
+      <c r="P16" s="13"/>
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1">
       <c r="A17" s="4">
@@ -2379,22 +2411,22 @@
       <c r="H17" s="4">
         <v>8</v>
       </c>
-      <c r="I17" s="92">
+      <c r="I17" s="53">
         <v>9</v>
       </c>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="94"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="55"/>
       <c r="M17" s="4">
         <v>10</v>
       </c>
       <c r="N17" s="4">
         <v>11</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17" s="15">
         <v>12</v>
       </c>
-      <c r="P17" s="17"/>
+      <c r="P17" s="16"/>
     </row>
     <row r="18" spans="1:26" ht="49.5" hidden="1" customHeight="1">
       <c r="A18" s="2" t="s">
@@ -2445,8 +2477,8 @@
     </row>
     <row r="19" spans="1:26" ht="15.5">
       <c r="A19" s="2"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
       <c r="F19" s="4"/>
@@ -2471,13 +2503,13 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
       <c r="A20" s="4"/>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="18"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
       <c r="I20" s="6"/>
@@ -2485,197 +2517,197 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="51">
+      <c r="N20" s="50">
         <f>SUM(N19:N19)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="19"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="11"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="1:26" ht="15" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="25"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="24"/>
       <c r="Q21" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="12"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="11"/>
     </row>
     <row r="24" spans="1:26" ht="18.5" thickBot="1">
-      <c r="A24" s="79"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="29"/>
+      <c r="A24" s="70"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="28"/>
       <c r="Q24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="18">
-      <c r="A25" s="89" t="s">
+      <c r="A25" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="91" t="s">
+      <c r="B25" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91" t="s">
+      <c r="C25" s="51"/>
+      <c r="D25" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91" t="s">
+      <c r="E25" s="51"/>
+      <c r="F25" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="76" t="s">
+      <c r="G25" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="29"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="28"/>
       <c r="Q25" s="8"/>
     </row>
     <row r="26" spans="1:26" ht="18">
-      <c r="A26" s="90"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="29"/>
+      <c r="A26" s="78"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="28"/>
       <c r="Q26" s="8"/>
     </row>
     <row r="27" spans="1:26" ht="18">
-      <c r="A27" s="90"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="29"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="28"/>
       <c r="Q27" s="8"/>
     </row>
     <row r="28" spans="1:26" ht="18">
-      <c r="A28" s="90"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="27"/>
+      <c r="A28" s="78"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="26"/>
       <c r="Q28" s="8"/>
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
-      <c r="A29" s="44"/>
-      <c r="B29" s="83" t="s">
+      <c r="A29" s="43"/>
+      <c r="B29" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="84"/>
-      <c r="D29" s="85"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
       <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
-      <c r="A30" s="46"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="87"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
@@ -2688,22 +2720,22 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A31" s="46"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="26"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
@@ -2716,27 +2748,27 @@
       <c r="Z31" s="8"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A32" s="48"/>
-      <c r="B32" s="96" t="s">
+      <c r="A32" s="47"/>
+      <c r="B32" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="97"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="50">
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="49">
         <f>SUM(G29:G31)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
@@ -2749,22 +2781,22 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
-      <c r="A33" s="21"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
@@ -2777,22 +2809,22 @@
       <c r="Z33" s="8"/>
     </row>
     <row r="34" spans="1:26" ht="18">
-      <c r="A34" s="28"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="Q34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="Q34" s="25"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
@@ -2804,25 +2836,25 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35" spans="1:26" ht="18">
-      <c r="A35" s="95" t="str">
+      <c r="A35" s="56" t="str">
         <f>_xlfn.CONCAT("        Висновки комісії: Залишкова вартість майна [SERVICE_NAME] визначалась з урахуванням технічного зносу згідно з Методикою визначення залишкової вартості майна ЗС України та інших військових формувань, та становить ",TEXT(FIELD_SUM, "0,00")," грн.")</f>
         <v xml:space="preserve">        Висновки комісії: Залишкова вартість майна [SERVICE_NAME] визначалась з урахуванням технічного зносу згідно з Методикою визначення залишкової вартості майна ЗС України та інших військових формувань, та становить 0,00 грн.</v>
       </c>
-      <c r="B35" s="95"/>
-      <c r="C35" s="95"/>
-      <c r="D35" s="95"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="95"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="95"/>
-      <c r="K35" s="95"/>
-      <c r="L35" s="95"/>
-      <c r="M35" s="95"/>
-      <c r="N35" s="95"/>
-      <c r="O35" s="95"/>
-      <c r="P35" s="26"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="25"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
@@ -2835,22 +2867,22 @@
       <c r="Z35" s="8"/>
     </row>
     <row r="36" spans="1:26" ht="18">
-      <c r="A36" s="95"/>
-      <c r="B36" s="95"/>
-      <c r="C36" s="95"/>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95"/>
-      <c r="I36" s="95"/>
-      <c r="J36" s="95"/>
-      <c r="K36" s="95"/>
-      <c r="L36" s="95"/>
-      <c r="M36" s="95"/>
-      <c r="N36" s="95"/>
-      <c r="O36" s="95"/>
-      <c r="P36" s="26"/>
+      <c r="A36" s="56"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="56"/>
+      <c r="L36" s="56"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="25"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
@@ -2863,22 +2895,22 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37" spans="1:26" ht="15.5" customHeight="1">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="27"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="25"/>
+      <c r="O37" s="25"/>
+      <c r="P37" s="26"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
@@ -2891,28 +2923,28 @@
       <c r="Z37" s="8"/>
     </row>
     <row r="38" spans="1:26" ht="18" customHeight="1">
-      <c r="A38" s="95" t="s">
+      <c r="A38" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="95"/>
-      <c r="C38" s="95" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="95"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="95" t="s">
+      <c r="B38" s="56"/>
+      <c r="C38" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="K38" s="95"/>
-      <c r="L38" s="95"/>
-      <c r="M38" s="95"/>
-      <c r="N38" s="95"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="27"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="K38" s="56"/>
+      <c r="L38" s="56"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="56"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="26"/>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
@@ -2925,173 +2957,173 @@
       <c r="Z38" s="8"/>
     </row>
     <row r="39" spans="1:26" ht="18" customHeight="1">
-      <c r="A39" s="95" t="s">
+      <c r="A39" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="95"/>
-      <c r="C39" s="95" t="s">
+      <c r="B39" s="56"/>
+      <c r="C39" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="56"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="K39" s="56"/>
+      <c r="L39" s="56"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="56"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+    </row>
+    <row r="40" spans="1:26" ht="18" customHeight="1">
+      <c r="A40" s="11"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="95"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="95" t="s">
+      <c r="D40" s="66"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="K39" s="95"/>
-      <c r="L39" s="95"/>
-      <c r="M39" s="95"/>
-      <c r="N39" s="95"/>
-      <c r="O39" s="26"/>
-      <c r="P39" s="26"/>
-      <c r="Q39" s="12"/>
-      <c r="R39" s="12"/>
-      <c r="S39" s="12"/>
-      <c r="T39" s="12"/>
-      <c r="U39" s="12"/>
-      <c r="V39" s="12"/>
-      <c r="W39" s="12"/>
-      <c r="X39" s="12"/>
-      <c r="Y39" s="12"/>
-      <c r="Z39" s="12"/>
-    </row>
-    <row r="40" spans="1:26" ht="18" customHeight="1">
-      <c r="A40" s="12"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="75" t="s">
+      <c r="K40" s="66"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="66"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
+    </row>
+    <row r="41" spans="1:26" ht="18" customHeight="1">
+      <c r="A41" s="11"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="75"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="75" t="s">
+      <c r="D41" s="66"/>
+      <c r="E41" s="28"/>
+      <c r="J41" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="K40" s="75"/>
-      <c r="L40" s="75"/>
-      <c r="M40" s="75"/>
-      <c r="N40" s="75"/>
-      <c r="O40" s="37"/>
-      <c r="P40" s="26"/>
-      <c r="Q40" s="12"/>
-      <c r="R40" s="12"/>
-      <c r="S40" s="12"/>
-      <c r="T40" s="12"/>
-      <c r="U40" s="12"/>
-      <c r="V40" s="12"/>
-      <c r="W40" s="12"/>
-      <c r="X40" s="12"/>
-      <c r="Y40" s="12"/>
-      <c r="Z40" s="12"/>
-    </row>
-    <row r="41" spans="1:26" ht="18" customHeight="1">
-      <c r="A41" s="12"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="75" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" s="75"/>
-      <c r="E41" s="29"/>
-      <c r="J41" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="75"/>
-      <c r="N41" s="75"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="S41" s="32"/>
-      <c r="T41" s="32"/>
-      <c r="U41" s="32"/>
-      <c r="V41" s="32"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="32"/>
-      <c r="Y41" s="32"/>
-      <c r="Z41" s="32"/>
+      <c r="K41" s="66"/>
+      <c r="L41" s="66"/>
+      <c r="M41" s="66"/>
+      <c r="N41" s="66"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
     </row>
     <row r="42" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A42" s="33"/>
-      <c r="P42" s="12"/>
-      <c r="Q42" s="12"/>
-      <c r="R42" s="12"/>
-      <c r="S42" s="12"/>
-      <c r="T42" s="12"/>
-      <c r="U42" s="12"/>
-      <c r="V42" s="12"/>
-      <c r="W42" s="12"/>
-      <c r="X42" s="12"/>
-      <c r="Y42" s="12"/>
-      <c r="Z42" s="12"/>
+      <c r="A42" s="32"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="X42" s="11"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="11"/>
     </row>
     <row r="43" spans="1:26" ht="18" customHeight="1">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="P43" s="12"/>
-      <c r="Q43" s="12"/>
-      <c r="R43" s="12"/>
-      <c r="S43" s="12"/>
-      <c r="T43" s="12"/>
-      <c r="U43" s="12"/>
-      <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
-      <c r="X43" s="12"/>
-      <c r="Y43" s="12"/>
-      <c r="Z43" s="12"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
     </row>
     <row r="44" spans="1:26" ht="18" customHeight="1">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="12"/>
-      <c r="Q44" s="12"/>
-      <c r="R44" s="12"/>
-      <c r="S44" s="12"/>
-      <c r="T44" s="12"/>
-      <c r="U44" s="12"/>
-      <c r="V44" s="12"/>
-      <c r="W44" s="12"/>
-      <c r="X44" s="12"/>
-      <c r="Y44" s="12"/>
-      <c r="Z44" s="12"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
     </row>
     <row r="45" spans="1:26" ht="18">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
       <c r="P45" s="8"/>
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
@@ -30003,20 +30035,29 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="50">
-    <mergeCell ref="F25:F28"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A35:O36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="J39:N39"/>
-    <mergeCell ref="J38:N38"/>
+  <mergeCells count="51">
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="A12:O12"/>
+    <mergeCell ref="A13:O13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="J6:O6"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="J41:N41"/>
@@ -30033,27 +30074,19 @@
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="B25:C28"/>
     <mergeCell ref="D25:E28"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A35:O36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="J39:N39"/>
+    <mergeCell ref="J38:N38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Fix a few bugs and implemented base changes for Asset Type functionality
</commit_message>
<xml_diff>
--- a/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
+++ b/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="Workbook_______"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Common\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Domain\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06E7FA3-575E-4F77-8736-6CAA3373E33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4915E251-4F86-4373-A629-1D3DB1155B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="FIELD_NUMBER_NAMES" localSheetId="0">Відомість!$B$20</definedName>
-    <definedName name="FIELD_RANGE_0" localSheetId="0">Відомість!$F$4</definedName>
+    <definedName name="FIELD_RANGE_0" localSheetId="0">Відомість!$C$4</definedName>
     <definedName name="FIELD_RANGE_1" localSheetId="0">Відомість!$A$3</definedName>
     <definedName name="FIELD_RANGE_10" localSheetId="0">Відомість!$J$38</definedName>
     <definedName name="FIELD_RANGE_11" localSheetId="0">Відомість!$C$39</definedName>
@@ -311,9 +311,6 @@
     <t>[COMMANDER_RANK]</t>
   </si>
   <si>
-    <t>визначення залишкової вартості майна [SERVICE_NAME] станом на ___.___.20___ року</t>
-  </si>
-  <si>
     <t>визначила залишкову вартість майна [SERVICE_NAME]</t>
   </si>
   <si>
@@ -342,6 +339,9 @@
   </si>
   <si>
     <t>[UNIT_EDRPOU]</t>
+  </si>
+  <si>
+    <t>визначення залишкової вартості майна [SERVICE_NAME] станом на [REPORT_DATE] року</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -848,11 +848,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -877,9 +903,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -993,6 +1016,9 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1055,6 +1081,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1685,7 +1717,7 @@
       <calculatedColumnFormula>Table[[#This Row],[Стовпець9]]*Table[[#This Row],[Стовпець10]]*Table[[#This Row],[Стовпець11]]*Table[[#This Row],[Стовпець12]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="14" xr3:uid="{CEDCFCC2-BC90-413B-8FB3-7840FCC05502}" name="Стовпець14" dataDxfId="1">
-      <calculatedColumnFormula>ROUND(G19*M19*Table[[#This Row],[Стовпець4]],2)</calculatedColumnFormula>
+      <calculatedColumnFormula>ROUND(G19*M19,2)*Table[[#This Row],[Стовпець4]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{DE3CE185-A73A-4CAD-A056-A4AAA7DA4D52}" name="Стовпець15" dataDxfId="0"/>
   </tableColumns>
@@ -1896,8 +1928,8 @@
   </sheetPr>
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2011,12 +2043,11 @@
         <v>0</v>
       </c>
       <c r="B4" s="72"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="10" t="s">
-        <v>61</v>
+      <c r="C4" s="75" t="s">
+        <v>60</v>
       </c>
+      <c r="D4" s="76"/>
+      <c r="E4" s="51"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2069,13 +2100,13 @@
     <row r="6" spans="1:26" ht="18" customHeight="1">
       <c r="A6" s="74"/>
       <c r="B6" s="72"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="52" t="s">
         <v>1</v>
       </c>
@@ -2084,23 +2115,23 @@
       <c r="M6" s="52"/>
       <c r="N6" s="52"/>
       <c r="O6" s="52"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="18" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
       <c r="J7" s="52" t="s">
         <v>47</v>
       </c>
@@ -2109,23 +2140,23 @@
       <c r="M7" s="52"/>
       <c r="N7" s="52"/>
       <c r="O7" s="52"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="18" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
       <c r="J8" s="53" t="s">
         <v>50</v>
       </c>
@@ -2136,23 +2167,23 @@
       </c>
       <c r="N8" s="54"/>
       <c r="O8" s="54"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="24.75" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
       <c r="J9" s="52" t="s">
         <v>2</v>
       </c>
@@ -2161,73 +2192,73 @@
       <c r="M9" s="52"/>
       <c r="N9" s="52"/>
       <c r="O9" s="52"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
     </row>
     <row r="10" spans="1:26" ht="18" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="8"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="18" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
     </row>
     <row r="12" spans="1:26" ht="18" customHeight="1">
       <c r="A12" s="61" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="61"/>
@@ -2243,7 +2274,7 @@
       <c r="M12" s="61"/>
       <c r="N12" s="61"/>
       <c r="O12" s="61"/>
-      <c r="Q12" s="12"/>
+      <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="1:26" ht="18" customHeight="1">
       <c r="A13" s="62" t="s">
@@ -2263,11 +2294,11 @@
       <c r="M13" s="62"/>
       <c r="N13" s="62"/>
       <c r="O13" s="62"/>
-      <c r="Q13" s="12"/>
+      <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="1:26" ht="18" customHeight="1">
       <c r="A14" s="69" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="69"/>
       <c r="C14" s="69"/>
@@ -2283,8 +2314,8 @@
       <c r="M14" s="69"/>
       <c r="N14" s="69"/>
       <c r="O14" s="70"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:26" ht="81.75" customHeight="1">
       <c r="A15" s="63" t="s">
@@ -2326,7 +2357,7 @@
       <c r="O15" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="P15" s="14"/>
+      <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="24" customHeight="1">
       <c r="A16" s="64"/>
@@ -2337,22 +2368,22 @@
       <c r="F16" s="65"/>
       <c r="G16" s="65"/>
       <c r="H16" s="56"/>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="14" t="s">
         <v>15</v>
       </c>
       <c r="M16" s="65"/>
       <c r="N16" s="58"/>
       <c r="O16" s="60"/>
-      <c r="P16" s="14"/>
+      <c r="P16" s="13"/>
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1">
       <c r="A17" s="4">
@@ -2379,22 +2410,22 @@
       <c r="H17" s="4">
         <v>8</v>
       </c>
-      <c r="I17" s="92">
+      <c r="I17" s="94">
         <v>9</v>
       </c>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="94"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="96"/>
       <c r="M17" s="4">
         <v>10</v>
       </c>
       <c r="N17" s="4">
         <v>11</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17" s="15">
         <v>12</v>
       </c>
-      <c r="P17" s="17"/>
+      <c r="P17" s="16"/>
     </row>
     <row r="18" spans="1:26" ht="49.5" hidden="1" customHeight="1">
       <c r="A18" s="2" t="s">
@@ -2445,8 +2476,8 @@
     </row>
     <row r="19" spans="1:26" ht="15.5">
       <c r="A19" s="2"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="41"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
       <c r="F19" s="4"/>
@@ -2464,20 +2495,20 @@
         <v>0</v>
       </c>
       <c r="N19" s="5">
-        <f>ROUND(G19*M19*Table[[#This Row],[Стовпець4]],2)</f>
+        <f>ROUND(G19*M19,2)*Table[[#This Row],[Стовпець4]]</f>
         <v>0</v>
       </c>
       <c r="O19" s="7"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
       <c r="A20" s="4"/>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="18"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
       <c r="I20" s="6"/>
@@ -2485,197 +2516,197 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="51">
+      <c r="N20" s="50">
         <f>SUM(N19:N19)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="19"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="11"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="1:26" ht="15" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="25"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="24"/>
       <c r="Q21" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="12"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="11"/>
     </row>
     <row r="24" spans="1:26" ht="18.5" thickBot="1">
-      <c r="A24" s="79"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="29"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="28"/>
       <c r="Q24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="18">
-      <c r="A25" s="89" t="s">
+      <c r="A25" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="91" t="s">
+      <c r="B25" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91" t="s">
+      <c r="C25" s="93"/>
+      <c r="D25" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91" t="s">
+      <c r="E25" s="93"/>
+      <c r="F25" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="76" t="s">
+      <c r="G25" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="29"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="28"/>
       <c r="Q25" s="8"/>
     </row>
     <row r="26" spans="1:26" ht="18">
-      <c r="A26" s="90"/>
+      <c r="A26" s="92"/>
       <c r="B26" s="59"/>
       <c r="C26" s="59"/>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
       <c r="F26" s="59"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="29"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="28"/>
       <c r="Q26" s="8"/>
     </row>
     <row r="27" spans="1:26" ht="18">
-      <c r="A27" s="90"/>
+      <c r="A27" s="92"/>
       <c r="B27" s="59"/>
       <c r="C27" s="59"/>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
       <c r="F27" s="59"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="29"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="28"/>
       <c r="Q27" s="8"/>
     </row>
     <row r="28" spans="1:26" ht="18">
-      <c r="A28" s="90"/>
+      <c r="A28" s="92"/>
       <c r="B28" s="59"/>
       <c r="C28" s="59"/>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
       <c r="F28" s="59"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="27"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="26"/>
       <c r="Q28" s="8"/>
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
-      <c r="A29" s="44"/>
-      <c r="B29" s="83" t="s">
+      <c r="A29" s="43"/>
+      <c r="B29" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="84"/>
-      <c r="D29" s="85"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
       <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
-      <c r="A30" s="46"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="87"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
@@ -2688,22 +2719,22 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A31" s="46"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="26"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
@@ -2716,27 +2747,27 @@
       <c r="Z31" s="8"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A32" s="48"/>
-      <c r="B32" s="96" t="s">
+      <c r="A32" s="47"/>
+      <c r="B32" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="97"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="50">
+      <c r="C32" s="99"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="99"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="49">
         <f>SUM(G29:G31)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
@@ -2749,22 +2780,22 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
-      <c r="A33" s="21"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
@@ -2777,22 +2808,22 @@
       <c r="Z33" s="8"/>
     </row>
     <row r="34" spans="1:26" ht="18">
-      <c r="A34" s="28"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="Q34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="Q34" s="25"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
@@ -2804,25 +2835,25 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35" spans="1:26" ht="18">
-      <c r="A35" s="95" t="str">
+      <c r="A35" s="97" t="str">
         <f>_xlfn.CONCAT("        Висновки комісії: Залишкова вартість майна [SERVICE_NAME] визначалась з урахуванням технічного зносу згідно з Методикою визначення залишкової вартості майна ЗС України та інших військових формувань, та становить ",TEXT(FIELD_SUM, "0,00")," грн.")</f>
         <v xml:space="preserve">        Висновки комісії: Залишкова вартість майна [SERVICE_NAME] визначалась з урахуванням технічного зносу згідно з Методикою визначення залишкової вартості майна ЗС України та інших військових формувань, та становить 0,00 грн.</v>
       </c>
-      <c r="B35" s="95"/>
-      <c r="C35" s="95"/>
-      <c r="D35" s="95"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="95"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="95"/>
-      <c r="K35" s="95"/>
-      <c r="L35" s="95"/>
-      <c r="M35" s="95"/>
-      <c r="N35" s="95"/>
-      <c r="O35" s="95"/>
-      <c r="P35" s="26"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="97"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="97"/>
+      <c r="F35" s="97"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="97"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="97"/>
+      <c r="K35" s="97"/>
+      <c r="L35" s="97"/>
+      <c r="M35" s="97"/>
+      <c r="N35" s="97"/>
+      <c r="O35" s="97"/>
+      <c r="P35" s="25"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
@@ -2835,22 +2866,22 @@
       <c r="Z35" s="8"/>
     </row>
     <row r="36" spans="1:26" ht="18">
-      <c r="A36" s="95"/>
-      <c r="B36" s="95"/>
-      <c r="C36" s="95"/>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="95"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95"/>
-      <c r="I36" s="95"/>
-      <c r="J36" s="95"/>
-      <c r="K36" s="95"/>
-      <c r="L36" s="95"/>
-      <c r="M36" s="95"/>
-      <c r="N36" s="95"/>
-      <c r="O36" s="95"/>
-      <c r="P36" s="26"/>
+      <c r="A36" s="97"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="97"/>
+      <c r="D36" s="97"/>
+      <c r="E36" s="97"/>
+      <c r="F36" s="97"/>
+      <c r="G36" s="97"/>
+      <c r="H36" s="97"/>
+      <c r="I36" s="97"/>
+      <c r="J36" s="97"/>
+      <c r="K36" s="97"/>
+      <c r="L36" s="97"/>
+      <c r="M36" s="97"/>
+      <c r="N36" s="97"/>
+      <c r="O36" s="97"/>
+      <c r="P36" s="25"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
@@ -2863,22 +2894,22 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37" spans="1:26" ht="15.5" customHeight="1">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="27"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="25"/>
+      <c r="O37" s="25"/>
+      <c r="P37" s="26"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
@@ -2891,28 +2922,28 @@
       <c r="Z37" s="8"/>
     </row>
     <row r="38" spans="1:26" ht="18" customHeight="1">
-      <c r="A38" s="95" t="s">
+      <c r="A38" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="95"/>
-      <c r="C38" s="95" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="95"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="95" t="s">
+      <c r="B38" s="97"/>
+      <c r="C38" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="K38" s="95"/>
-      <c r="L38" s="95"/>
-      <c r="M38" s="95"/>
-      <c r="N38" s="95"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="27"/>
+      <c r="D38" s="97"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="K38" s="97"/>
+      <c r="L38" s="97"/>
+      <c r="M38" s="97"/>
+      <c r="N38" s="97"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="26"/>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
@@ -2925,173 +2956,173 @@
       <c r="Z38" s="8"/>
     </row>
     <row r="39" spans="1:26" ht="18" customHeight="1">
-      <c r="A39" s="95" t="s">
+      <c r="A39" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="95"/>
-      <c r="C39" s="95" t="s">
+      <c r="B39" s="97"/>
+      <c r="C39" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="97"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="97" t="s">
+        <v>57</v>
+      </c>
+      <c r="K39" s="97"/>
+      <c r="L39" s="97"/>
+      <c r="M39" s="97"/>
+      <c r="N39" s="97"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+    </row>
+    <row r="40" spans="1:26" ht="18" customHeight="1">
+      <c r="A40" s="11"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="95"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="95" t="s">
+      <c r="D40" s="77"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="K39" s="95"/>
-      <c r="L39" s="95"/>
-      <c r="M39" s="95"/>
-      <c r="N39" s="95"/>
-      <c r="O39" s="26"/>
-      <c r="P39" s="26"/>
-      <c r="Q39" s="12"/>
-      <c r="R39" s="12"/>
-      <c r="S39" s="12"/>
-      <c r="T39" s="12"/>
-      <c r="U39" s="12"/>
-      <c r="V39" s="12"/>
-      <c r="W39" s="12"/>
-      <c r="X39" s="12"/>
-      <c r="Y39" s="12"/>
-      <c r="Z39" s="12"/>
-    </row>
-    <row r="40" spans="1:26" ht="18" customHeight="1">
-      <c r="A40" s="12"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="75" t="s">
+      <c r="K40" s="77"/>
+      <c r="L40" s="77"/>
+      <c r="M40" s="77"/>
+      <c r="N40" s="77"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
+    </row>
+    <row r="41" spans="1:26" ht="18" customHeight="1">
+      <c r="A41" s="11"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="75"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="75" t="s">
+      <c r="D41" s="77"/>
+      <c r="E41" s="28"/>
+      <c r="J41" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="K40" s="75"/>
-      <c r="L40" s="75"/>
-      <c r="M40" s="75"/>
-      <c r="N40" s="75"/>
-      <c r="O40" s="37"/>
-      <c r="P40" s="26"/>
-      <c r="Q40" s="12"/>
-      <c r="R40" s="12"/>
-      <c r="S40" s="12"/>
-      <c r="T40" s="12"/>
-      <c r="U40" s="12"/>
-      <c r="V40" s="12"/>
-      <c r="W40" s="12"/>
-      <c r="X40" s="12"/>
-      <c r="Y40" s="12"/>
-      <c r="Z40" s="12"/>
-    </row>
-    <row r="41" spans="1:26" ht="18" customHeight="1">
-      <c r="A41" s="12"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="75" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" s="75"/>
-      <c r="E41" s="29"/>
-      <c r="J41" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="75"/>
-      <c r="N41" s="75"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="32"/>
-      <c r="S41" s="32"/>
-      <c r="T41" s="32"/>
-      <c r="U41" s="32"/>
-      <c r="V41" s="32"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="32"/>
-      <c r="Y41" s="32"/>
-      <c r="Z41" s="32"/>
+      <c r="K41" s="77"/>
+      <c r="L41" s="77"/>
+      <c r="M41" s="77"/>
+      <c r="N41" s="77"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
     </row>
     <row r="42" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A42" s="33"/>
-      <c r="P42" s="12"/>
-      <c r="Q42" s="12"/>
-      <c r="R42" s="12"/>
-      <c r="S42" s="12"/>
-      <c r="T42" s="12"/>
-      <c r="U42" s="12"/>
-      <c r="V42" s="12"/>
-      <c r="W42" s="12"/>
-      <c r="X42" s="12"/>
-      <c r="Y42" s="12"/>
-      <c r="Z42" s="12"/>
+      <c r="A42" s="32"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="X42" s="11"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="11"/>
     </row>
     <row r="43" spans="1:26" ht="18" customHeight="1">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="P43" s="12"/>
-      <c r="Q43" s="12"/>
-      <c r="R43" s="12"/>
-      <c r="S43" s="12"/>
-      <c r="T43" s="12"/>
-      <c r="U43" s="12"/>
-      <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
-      <c r="X43" s="12"/>
-      <c r="Y43" s="12"/>
-      <c r="Z43" s="12"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
     </row>
     <row r="44" spans="1:26" ht="18" customHeight="1">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="12"/>
-      <c r="Q44" s="12"/>
-      <c r="R44" s="12"/>
-      <c r="S44" s="12"/>
-      <c r="T44" s="12"/>
-      <c r="U44" s="12"/>
-      <c r="V44" s="12"/>
-      <c r="W44" s="12"/>
-      <c r="X44" s="12"/>
-      <c r="Y44" s="12"/>
-      <c r="Z44" s="12"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
     </row>
     <row r="45" spans="1:26" ht="18">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
       <c r="P45" s="8"/>
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
@@ -30003,7 +30034,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="50">
+  <mergeCells count="51">
     <mergeCell ref="F25:F28"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="A38:B38"/>
@@ -30038,6 +30069,7 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="J7:O7"/>
     <mergeCell ref="J9:O9"/>
     <mergeCell ref="J8:L8"/>

</xml_diff>

<commit_message>
Make Residual Value report be appliable and extendable for different services; Fix small issues
</commit_message>
<xml_diff>
--- a/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
+++ b/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="Workbook_______"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Domain\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4915E251-4F86-4373-A629-1D3DB1155B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA51937-E9DA-494E-9634-C81E696B378B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,25 +16,30 @@
     <sheet name="Відомість" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="COMPLEX_MERGED_RANGE_1" localSheetId="0">Відомість!$J$6:$O$9</definedName>
+    <definedName name="COMPLEX_MERGED_RANGE_2" localSheetId="0">Відомість!$L$37:$O$40</definedName>
+    <definedName name="FIELD_HEADER_TITLE" localSheetId="0">Відомість!$A$15</definedName>
     <definedName name="FIELD_NUMBER_NAMES" localSheetId="0">Відомість!$B$20</definedName>
     <definedName name="FIELD_RANGE_0" localSheetId="0">Відомість!$C$4</definedName>
     <definedName name="FIELD_RANGE_1" localSheetId="0">Відомість!$A$3</definedName>
-    <definedName name="FIELD_RANGE_10" localSheetId="0">Відомість!$J$38</definedName>
-    <definedName name="FIELD_RANGE_11" localSheetId="0">Відомість!$C$39</definedName>
-    <definedName name="FIELD_RANGE_12" localSheetId="0">Відомість!$J$39</definedName>
-    <definedName name="FIELD_RANGE_13" localSheetId="0">Відомість!$C$40</definedName>
-    <definedName name="FIELD_RANGE_14" localSheetId="0">Відомість!$J$40</definedName>
-    <definedName name="FIELD_RANGE_15" localSheetId="0">Відомість!$C$41</definedName>
-    <definedName name="FIELD_RANGE_16" localSheetId="0">Відомість!$J$41</definedName>
-    <definedName name="FIELD_RANGE_2" localSheetId="0">Відомість!$J$7</definedName>
-    <definedName name="FIELD_RANGE_3" localSheetId="0">Відомість!$J$8</definedName>
-    <definedName name="FIELD_RANGE_4" localSheetId="0">Відомість!$M$8</definedName>
+    <definedName name="FIELD_RANGE_10" localSheetId="0">Відомість!$L$37</definedName>
+    <definedName name="FIELD_RANGE_11" localSheetId="0">Відомість!$C$38</definedName>
+    <definedName name="FIELD_RANGE_12" localSheetId="0">Відомість!$L$38</definedName>
+    <definedName name="FIELD_RANGE_13" localSheetId="0">Відомість!$C$39</definedName>
+    <definedName name="FIELD_RANGE_14" localSheetId="0">Відомість!$L$39</definedName>
+    <definedName name="FIELD_RANGE_15" localSheetId="0">Відомість!$C$40</definedName>
+    <definedName name="FIELD_RANGE_16" localSheetId="0">Відомість!$L$40</definedName>
+    <definedName name="FIELD_RANGE_2" localSheetId="0">Відомість!$K$7</definedName>
+    <definedName name="FIELD_RANGE_3" localSheetId="0">Відомість!$K$8</definedName>
+    <definedName name="FIELD_RANGE_4" localSheetId="0">Відомість!$N$8</definedName>
     <definedName name="FIELD_RANGE_5" localSheetId="0">Відомість!$A$12</definedName>
     <definedName name="FIELD_RANGE_6" localSheetId="0">Відомість!$A$13</definedName>
     <definedName name="FIELD_RANGE_7" localSheetId="0">Відомість!$A$14</definedName>
     <definedName name="FIELD_RANGE_8" localSheetId="0">Відомість!$A$35</definedName>
-    <definedName name="FIELD_RANGE_9" localSheetId="0">Відомість!$C$38</definedName>
-    <definedName name="FIELD_SUM" localSheetId="0">Відомість!$N$20</definedName>
+    <definedName name="FIELD_RANGE_9" localSheetId="0">Відомість!$C$37</definedName>
+    <definedName name="FIELD_SUM" localSheetId="0">Відомість!#REF!</definedName>
+    <definedName name="FIELD_TABLE_COLUMN_NUMBER" localSheetId="0">Відомість!$A$17</definedName>
+    <definedName name="FIELDS_TITLE" localSheetId="0">Відомість!$A$11:$O$14</definedName>
     <definedName name="HEADER_Table2_FIELD" localSheetId="0">Відомість!$A$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -55,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>ідентифікаційний код за ЄДРПОУ</t>
   </si>
@@ -82,27 +87,6 @@
   </si>
   <si>
     <t>Курс іноземної валюти, в якій визначена ціна імпортованого військового майна згідно з договором (контрактом), до нривні, встановлений Національним банком</t>
-  </si>
-  <si>
-    <t>Значення коефіцієнтів, які використовуються під час визначення сукупного крефіцієнта зносу</t>
-  </si>
-  <si>
-    <t>Сукупний коефіцієнт зносу                            (Кскз)</t>
-  </si>
-  <si>
-    <t>Посилання        на звіт про оцінку майна</t>
-  </si>
-  <si>
-    <t>Ке</t>
-  </si>
-  <si>
-    <t>Кр</t>
-  </si>
-  <si>
-    <t>Кзб</t>
-  </si>
-  <si>
-    <t>Ктс</t>
   </si>
   <si>
     <t>Всього 2 (два) найменування</t>
@@ -153,72 +137,8 @@
     <t>Стовпець8</t>
   </si>
   <si>
-    <t>Стовпець9</t>
-  </si>
-  <si>
-    <t>Стовпець10</t>
-  </si>
-  <si>
-    <t>Стовпець11</t>
-  </si>
-  <si>
-    <t>Стовпець12</t>
-  </si>
-  <si>
-    <t>Стовпець13</t>
-  </si>
-  <si>
-    <t>Стовпець14</t>
-  </si>
-  <si>
-    <t>Стовпець15</t>
-  </si>
-  <si>
     <t>Розрахунок
 вмісту дорогоцінних металів, чорних та кольорових металів</t>
-  </si>
-  <si>
-    <r>
-      <t>Ціна придбання (ціна за прейскурантом, ціна за договором, згідно з яким військове майно придбане на дату взяття на облік), дата взяття на облік</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>2023 року</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">         </t>
-    </r>
   </si>
   <si>
     <r>
@@ -265,32 +185,6 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>Залишкова вартість (графа 7 х  графу 10) (В</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>зал</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Глава комісії:</t>
   </si>
   <si>
     <t>Члени комісії:</t>
@@ -343,6 +237,78 @@
   <si>
     <t>визначення залишкової вартості майна [SERVICE_NAME] станом на [REPORT_DATE] року</t>
   </si>
+  <si>
+    <r>
+      <t>Ціна придбання (ціна за прейскурантом, ціна за договором, згідно з яким військове майно придбане на дату взяття на облік), дата взяття на облік</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+  </si>
+  <si>
+    <t>Стовпець9</t>
+  </si>
+  <si>
+    <t>Стовпець10</t>
+  </si>
+  <si>
+    <t>Стовпець11</t>
+  </si>
+  <si>
+    <t>Стовпець12</t>
+  </si>
+  <si>
+    <t>Стовпець13</t>
+  </si>
+  <si>
+    <t>Стовпець14</t>
+  </si>
+  <si>
+    <t>Стовпець15</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Висновки комісії: Залишкова вартість майна [SERVICE_NAME] визначалась з урахуванням технічного зносу згідно з Методикою визначення залишкової вартості майна ЗС України та інших військових формувань, та становить </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>[TOTAL_RESIDUAL_SUM]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> грн.</t>
+    </r>
+  </si>
+  <si>
+    <t>Голова комісії:</t>
+  </si>
 </sst>
 </file>
 
@@ -352,7 +318,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ _₽"/>
     <numFmt numFmtId="165" formatCode="#,##0.00_₴"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -433,12 +399,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -464,7 +424,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -479,7 +438,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -874,11 +833,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -909,19 +883,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -960,20 +925,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1013,37 +978,46 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1057,20 +1031,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1088,21 +1077,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1112,40 +1086,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1154,6 +1100,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -1161,234 +1120,199 @@
   <dxfs count="18">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="165" formatCode="#,##0.00_₴"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ _₽"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
@@ -1416,7 +1340,7 @@
           <color rgb="FF000000"/>
         </left>
         <right style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
           <color rgb="FF000000"/>
@@ -1665,7 +1589,9 @@
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
@@ -1676,7 +1602,9 @@
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
@@ -1709,17 +1637,13 @@
       <calculatedColumnFormula>ROUND(E19*F19,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{367C3413-BF3B-423C-A04A-2814E50C87E1}" name="Стовпець8" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{32E2D941-91C2-444C-831E-C957FDDE8FF5}" name="Стовпець9" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{C3D05F5A-ED98-4CAA-8BBF-67341037557A}" name="Стовпець10" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{B0586091-33F5-48EF-8DE5-A83060AA2B47}" name="Стовпець11" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{E791FFD9-D66B-4A3C-B133-AEAFFD58B46E}" name="Стовпець12" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{95448C30-091A-4230-B812-4DB5B62D75AC}" name="Стовпець13" dataDxfId="2">
-      <calculatedColumnFormula>Table[[#This Row],[Стовпець9]]*Table[[#This Row],[Стовпець10]]*Table[[#This Row],[Стовпець11]]*Table[[#This Row],[Стовпець12]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="14" xr3:uid="{CEDCFCC2-BC90-413B-8FB3-7840FCC05502}" name="Стовпець14" dataDxfId="1">
-      <calculatedColumnFormula>ROUND(G19*M19,2)*Table[[#This Row],[Стовпець4]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="15" xr3:uid="{DE3CE185-A73A-4CAD-A056-A4AAA7DA4D52}" name="Стовпець15" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{202BCDE3-5F48-4FA4-8C3F-A34C56881D6E}" name="Стовпець9" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{17574747-EE2A-4B01-BB04-855077C0E1EA}" name="Стовпець10" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{12AAD393-3012-4400-B19F-F964366D98C7}" name="Стовпець11" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{0107D3B1-D8D8-43D9-9D6F-679BD5947952}" name="Стовпець12" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{CE8D7C7C-C1EF-43A1-A678-379081133252}" name="Стовпець13" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{9ED438C1-E185-4C3B-A31F-A751FC28DDF0}" name="Стовпець14" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{E843A11C-28C0-4349-9D21-39647F8044A0}" name="Стовпець15" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1926,10 +1850,10 @@
   <sheetPr codeName="Worksheet_____1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="69" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2009,10 +1933,10 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A3" s="71" t="s">
-        <v>46</v>
+      <c r="A3" s="76" t="s">
+        <v>29</v>
       </c>
-      <c r="B3" s="72"/>
+      <c r="B3" s="77"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2039,15 +1963,15 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="75" t="s">
-        <v>60</v>
+      <c r="B4" s="77"/>
+      <c r="C4" s="80" t="s">
+        <v>43</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="51"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="47"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2098,33 +2022,22 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" spans="1:26" ht="18" customHeight="1">
-      <c r="A6" s="74"/>
-      <c r="B6" s="72"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="77"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="52" t="s">
+      <c r="K6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="27"/>
     </row>
     <row r="7" spans="1:26" ht="18" customHeight="1">
       <c r="A7" s="8"/>
@@ -2132,24 +2045,15 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
-      <c r="J7" s="52" t="s">
-        <v>47</v>
+      <c r="K7" s="55" t="s">
+        <v>30</v>
       </c>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="27"/>
     </row>
     <row r="8" spans="1:26" ht="18" customHeight="1">
       <c r="A8" s="8"/>
@@ -2157,26 +2061,17 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="J8" s="53" t="s">
-        <v>50</v>
+      <c r="K8" s="58" t="s">
+        <v>33</v>
       </c>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="54" t="s">
-        <v>49</v>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="56" t="s">
+        <v>32</v>
       </c>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="11"/>
     </row>
     <row r="9" spans="1:26" ht="24.75" customHeight="1">
       <c r="A9" s="8"/>
@@ -2184,24 +2079,15 @@
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="J9" s="52" t="s">
+      <c r="K9" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="27"/>
     </row>
     <row r="10" spans="1:26" ht="18" customHeight="1">
       <c r="A10" s="8"/>
@@ -2209,41 +2095,35 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="8"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="10"/>
+      <c r="P10" s="10"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="11"/>
     </row>
     <row r="11" spans="1:26" ht="18" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11" t="s">
+      <c r="A11" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
@@ -2258,7 +2138,7 @@
     </row>
     <row r="12" spans="1:26" ht="18" customHeight="1">
       <c r="A12" s="61" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="61"/>
@@ -2278,7 +2158,7 @@
     </row>
     <row r="13" spans="1:26" ht="18" customHeight="1">
       <c r="A13" s="62" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B13" s="62"/>
       <c r="C13" s="62"/>
@@ -2297,23 +2177,23 @@
       <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="1:26" ht="18" customHeight="1">
-      <c r="A14" s="69" t="s">
-        <v>51</v>
+      <c r="A14" s="66" t="s">
+        <v>34</v>
       </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="69"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="70"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="67"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="11"/>
     </row>
@@ -2331,32 +2211,24 @@
         <v>7</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F15" s="63" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="G15" s="63" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
-      <c r="H15" s="55" t="s">
+      <c r="H15" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="N15" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="O15" s="59" t="s">
-        <v>11</v>
-      </c>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
       <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="24" customHeight="1">
@@ -2367,22 +2239,14 @@
       <c r="E16" s="65"/>
       <c r="F16" s="65"/>
       <c r="G16" s="65"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="65"/>
-      <c r="N16" s="58"/>
-      <c r="O16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="12"/>
       <c r="P16" s="13"/>
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1">
@@ -2407,77 +2271,69 @@
       <c r="G17" s="4">
         <v>7</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="50">
         <v>8</v>
       </c>
-      <c r="I17" s="94">
-        <v>9</v>
-      </c>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="4">
-        <v>10</v>
-      </c>
-      <c r="N17" s="4">
-        <v>11</v>
-      </c>
-      <c r="O17" s="15">
-        <v>12</v>
-      </c>
-      <c r="P17" s="16"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="14"/>
     </row>
     <row r="18" spans="1:26" ht="49.5" hidden="1" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>25</v>
+      <c r="I18" s="52" t="s">
+        <v>46</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>26</v>
+      <c r="J18" s="52" t="s">
+        <v>47</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>27</v>
+      <c r="K18" s="52" t="s">
+        <v>48</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>28</v>
+      <c r="L18" s="52" t="s">
+        <v>49</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>29</v>
+      <c r="M18" s="52" t="s">
+        <v>50</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>30</v>
+      <c r="N18" s="52" t="s">
+        <v>51</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>38</v>
+      <c r="O18" s="52" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.5">
       <c r="A19" s="2"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="40"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
       <c r="F19" s="4"/>
@@ -2485,228 +2341,217 @@
         <f>ROUND(E19*F19,2)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4">
-        <f>Table[[#This Row],[Стовпець9]]*Table[[#This Row],[Стовпець10]]*Table[[#This Row],[Стовпець11]]*Table[[#This Row],[Стовпець12]]</f>
-        <v>0</v>
-      </c>
-      <c r="N19" s="5">
-        <f>ROUND(G19*M19,2)*Table[[#This Row],[Стовпець4]]</f>
-        <v>0</v>
-      </c>
-      <c r="O19" s="7"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="95"/>
+      <c r="N19" s="94"/>
+      <c r="O19" s="53"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="82" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C20" s="83"/>
       <c r="D20" s="83"/>
       <c r="E20" s="84"/>
-      <c r="F20" s="17"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="50">
-        <f>SUM(N19:N19)</f>
-        <v>0</v>
+      <c r="I20" s="16"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="52"/>
+    </row>
+    <row r="21" spans="1:26" ht="15" customHeight="1">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="23" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A23" s="70" t="s">
+        <v>25</v>
       </c>
-      <c r="O20" s="18"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="10"/>
-    </row>
-    <row r="21" spans="1:26" ht="15" customHeight="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="8"/>
-    </row>
-    <row r="23" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A23" s="80" t="s">
-        <v>39</v>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="11"/>
+    </row>
+    <row r="24" spans="1:26" ht="18.5" thickBot="1">
+      <c r="A24" s="71"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="1:26" ht="18">
+      <c r="A25" s="72" t="s">
+        <v>10</v>
       </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="11"/>
-    </row>
-    <row r="24" spans="1:26" ht="18.5" thickBot="1">
-      <c r="A24" s="81"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="8"/>
-    </row>
-    <row r="25" spans="1:26" ht="18">
-      <c r="A25" s="91" t="s">
-        <v>17</v>
+      <c r="B25" s="74" t="s">
+        <v>11</v>
       </c>
-      <c r="B25" s="93" t="s">
-        <v>18</v>
+      <c r="C25" s="74"/>
+      <c r="D25" s="74" t="s">
+        <v>12</v>
       </c>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93" t="s">
-        <v>19</v>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74" t="s">
+        <v>13</v>
       </c>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93" t="s">
-        <v>20</v>
+      <c r="G25" s="68" t="s">
+        <v>14</v>
       </c>
-      <c r="G25" s="78" t="s">
-        <v>21</v>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="1:26" ht="18">
+      <c r="A26" s="73"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="8"/>
+    </row>
+    <row r="27" spans="1:26" ht="18">
+      <c r="A27" s="73"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="8"/>
+    </row>
+    <row r="28" spans="1:26" ht="18">
+      <c r="A28" s="73"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="8"/>
+    </row>
+    <row r="29" spans="1:26" ht="15" customHeight="1">
+      <c r="A29" s="40"/>
+      <c r="B29" s="91" t="s">
+        <v>15</v>
       </c>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="8"/>
-    </row>
-    <row r="26" spans="1:26" ht="18">
-      <c r="A26" s="92"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="8"/>
-    </row>
-    <row r="27" spans="1:26" ht="18">
-      <c r="A27" s="92"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="8"/>
-    </row>
-    <row r="28" spans="1:26" ht="18">
-      <c r="A28" s="92"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="8"/>
-    </row>
-    <row r="29" spans="1:26" ht="15" customHeight="1">
-      <c r="A29" s="43"/>
-      <c r="B29" s="85" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="86"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="93"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
       <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
-      <c r="A30" s="45"/>
-      <c r="B30" s="88"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
@@ -2719,22 +2564,22 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A31" s="45"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="89"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
@@ -2747,27 +2592,27 @@
       <c r="Z31" s="8"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A32" s="47"/>
-      <c r="B32" s="98" t="s">
-        <v>23</v>
+      <c r="A32" s="44"/>
+      <c r="B32" s="88" t="s">
+        <v>16</v>
       </c>
-      <c r="C32" s="99"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="99"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="49">
+      <c r="C32" s="89"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="46">
         <f>SUM(G29:G31)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
@@ -2780,22 +2625,22 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="37"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="12"/>
-      <c r="D33" s="38"/>
+      <c r="D33" s="35"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
@@ -2808,22 +2653,22 @@
       <c r="Z33" s="8"/>
     </row>
     <row r="34" spans="1:26" ht="18">
-      <c r="A34" s="27"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="Q34" s="25"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="Q34" s="22"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
@@ -2835,25 +2680,24 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35" spans="1:26" ht="18">
-      <c r="A35" s="97" t="str">
-        <f>_xlfn.CONCAT("        Висновки комісії: Залишкова вартість майна [SERVICE_NAME] визначалась з урахуванням технічного зносу згідно з Методикою визначення залишкової вартості майна ЗС України та інших військових формувань, та становить ",TEXT(FIELD_SUM, "0,00")," грн.")</f>
-        <v xml:space="preserve">        Висновки комісії: Залишкова вартість майна [SERVICE_NAME] визначалась з урахуванням технічного зносу згідно з Методикою визначення залишкової вартості майна ЗС України та інших військових формувань, та становить 0,00 грн.</v>
+      <c r="A35" s="57" t="s">
+        <v>53</v>
       </c>
-      <c r="B35" s="97"/>
-      <c r="C35" s="97"/>
-      <c r="D35" s="97"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="97"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="97"/>
-      <c r="I35" s="97"/>
-      <c r="J35" s="97"/>
-      <c r="K35" s="97"/>
-      <c r="L35" s="97"/>
-      <c r="M35" s="97"/>
-      <c r="N35" s="97"/>
-      <c r="O35" s="97"/>
-      <c r="P35" s="25"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="57"/>
+      <c r="M35" s="57"/>
+      <c r="N35" s="57"/>
+      <c r="O35" s="57"/>
+      <c r="P35" s="22"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
@@ -2865,25 +2709,25 @@
       <c r="Y35" s="8"/>
       <c r="Z35" s="8"/>
     </row>
-    <row r="36" spans="1:26" ht="18">
-      <c r="A36" s="97"/>
-      <c r="B36" s="97"/>
-      <c r="C36" s="97"/>
-      <c r="D36" s="97"/>
-      <c r="E36" s="97"/>
-      <c r="F36" s="97"/>
-      <c r="G36" s="97"/>
-      <c r="H36" s="97"/>
-      <c r="I36" s="97"/>
-      <c r="J36" s="97"/>
-      <c r="K36" s="97"/>
-      <c r="L36" s="97"/>
-      <c r="M36" s="97"/>
-      <c r="N36" s="97"/>
-      <c r="O36" s="97"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
+    <row r="36" spans="1:26" ht="15.5" customHeight="1">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
@@ -2893,162 +2737,154 @@
       <c r="Y36" s="8"/>
       <c r="Z36" s="8"/>
     </row>
-    <row r="37" spans="1:26" ht="15.5" customHeight="1">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="25"/>
-      <c r="P37" s="26"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8"/>
-      <c r="W37" s="8"/>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="8"/>
-    </row>
-    <row r="38" spans="1:26" ht="18" customHeight="1">
-      <c r="A38" s="97" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="97"/>
-      <c r="C38" s="97" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="97"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="97" t="s">
-        <v>52</v>
-      </c>
-      <c r="K38" s="97"/>
-      <c r="L38" s="97"/>
-      <c r="M38" s="97"/>
-      <c r="N38" s="97"/>
-      <c r="O38" s="25"/>
-      <c r="P38" s="26"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
-      <c r="W38" s="8"/>
-      <c r="X38" s="8"/>
-      <c r="Y38" s="8"/>
-      <c r="Z38" s="8"/>
-    </row>
-    <row r="39" spans="1:26" ht="18" customHeight="1">
-      <c r="A39" s="97" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="97"/>
-      <c r="C39" s="97" t="s">
+    <row r="37" spans="1:26" ht="18" customHeight="1">
+      <c r="A37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="97"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="97" t="s">
-        <v>57</v>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57" t="s">
+        <v>36</v>
       </c>
-      <c r="K39" s="97"/>
-      <c r="L39" s="97"/>
-      <c r="M39" s="97"/>
-      <c r="N39" s="97"/>
-      <c r="O39" s="25"/>
-      <c r="P39" s="25"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="33"/>
+      <c r="L37" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="M37" s="57"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="57"/>
+      <c r="P37" s="25"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="8"/>
+      <c r="Z37" s="8"/>
+    </row>
+    <row r="38" spans="1:26" ht="18" customHeight="1">
+      <c r="A38" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="33"/>
+      <c r="L38" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
+      <c r="O38" s="57"/>
+      <c r="P38" s="25"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="Z38" s="11"/>
+    </row>
+    <row r="39" spans="1:26" ht="18" customHeight="1">
+      <c r="A39" s="11"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="L39" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="M39" s="54"/>
+      <c r="N39" s="54"/>
+      <c r="O39" s="54"/>
+      <c r="P39" s="33"/>
       <c r="Q39" s="11"/>
       <c r="R39" s="11"/>
       <c r="S39" s="11"/>
-      <c r="T39" s="11"/>
-      <c r="U39" s="11"/>
-      <c r="V39" s="11"/>
-      <c r="W39" s="11"/>
-      <c r="X39" s="11"/>
-      <c r="Y39" s="11"/>
       <c r="Z39" s="11"/>
     </row>
     <row r="40" spans="1:26" ht="18" customHeight="1">
       <c r="A40" s="11"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="77" t="s">
-        <v>55</v>
+      <c r="B40" s="27"/>
+      <c r="C40" s="54" t="s">
+        <v>39</v>
       </c>
-      <c r="D40" s="77"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="77" t="s">
-        <v>58</v>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="L40" s="54" t="s">
+        <v>42</v>
       </c>
-      <c r="K40" s="77"/>
-      <c r="L40" s="77"/>
-      <c r="M40" s="77"/>
-      <c r="N40" s="77"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="25"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-      <c r="T40" s="11"/>
-      <c r="U40" s="11"/>
-      <c r="V40" s="11"/>
-      <c r="W40" s="11"/>
-      <c r="X40" s="11"/>
-      <c r="Y40" s="11"/>
-      <c r="Z40" s="11"/>
-    </row>
-    <row r="41" spans="1:26" ht="18" customHeight="1">
-      <c r="A41" s="11"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" s="77"/>
-      <c r="E41" s="28"/>
-      <c r="J41" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="K41" s="77"/>
-      <c r="L41" s="77"/>
-      <c r="M41" s="77"/>
-      <c r="N41" s="77"/>
-      <c r="Q41" s="31"/>
-      <c r="R41" s="31"/>
-      <c r="S41" s="31"/>
-      <c r="T41" s="31"/>
-      <c r="U41" s="31"/>
-      <c r="V41" s="31"/>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
-      <c r="Z41" s="31"/>
-    </row>
-    <row r="42" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A42" s="32"/>
+      <c r="M40" s="54"/>
+      <c r="N40" s="54"/>
+      <c r="O40" s="54"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
+      <c r="S40" s="28"/>
+      <c r="Z40" s="28"/>
+    </row>
+    <row r="41" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A41" s="29"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="X41" s="11"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="11"/>
+    </row>
+    <row r="42" spans="1:26" ht="18" customHeight="1">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
+      <c r="O42" s="33"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="11"/>
       <c r="R42" s="11"/>
@@ -3067,6 +2903,16 @@
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="11"/>
       <c r="R43" s="11"/>
@@ -3079,7 +2925,7 @@
       <c r="Y43" s="11"/>
       <c r="Z43" s="11"/>
     </row>
-    <row r="44" spans="1:26" ht="18" customHeight="1">
+    <row r="44" spans="1:26" ht="18">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -3098,16 +2944,16 @@
       <c r="P44" s="11"/>
       <c r="Q44" s="11"/>
       <c r="R44" s="11"/>
-      <c r="S44" s="11"/>
-      <c r="T44" s="11"/>
-      <c r="U44" s="11"/>
-      <c r="V44" s="11"/>
-      <c r="W44" s="11"/>
-      <c r="X44" s="11"/>
-      <c r="Y44" s="11"/>
-      <c r="Z44" s="11"/>
-    </row>
-    <row r="45" spans="1:26" ht="18">
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="8"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="8"/>
+      <c r="Y44" s="8"/>
+      <c r="Z44" s="8"/>
+    </row>
+    <row r="45" spans="1:26" ht="18" customHeight="1">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -3123,9 +2969,9 @@
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
       <c r="O45" s="11"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
       <c r="S45" s="8"/>
       <c r="T45" s="8"/>
       <c r="U45" s="8"/>
@@ -3136,24 +2982,24 @@
       <c r="Z45" s="8"/>
     </row>
     <row r="46" spans="1:26" ht="18" customHeight="1">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
-      <c r="R46" s="8"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
       <c r="S46" s="8"/>
       <c r="T46" s="8"/>
       <c r="U46" s="8"/>
@@ -3164,24 +3010,24 @@
       <c r="Z46" s="8"/>
     </row>
     <row r="47" spans="1:26" ht="18" customHeight="1">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
       <c r="S47" s="8"/>
       <c r="T47" s="8"/>
       <c r="U47" s="8"/>
@@ -3192,24 +3038,24 @@
       <c r="Z47" s="8"/>
     </row>
     <row r="48" spans="1:26" ht="18" customHeight="1">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
       <c r="S48" s="8"/>
       <c r="T48" s="8"/>
       <c r="U48" s="8"/>
@@ -3220,24 +3066,24 @@
       <c r="Z48" s="8"/>
     </row>
     <row r="49" spans="1:26" ht="18" customHeight="1">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="8"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
       <c r="S49" s="8"/>
       <c r="T49" s="8"/>
       <c r="U49" s="8"/>
@@ -3248,24 +3094,24 @@
       <c r="Z49" s="8"/>
     </row>
     <row r="50" spans="1:26" ht="18" customHeight="1">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
       <c r="S50" s="8"/>
       <c r="T50" s="8"/>
       <c r="U50" s="8"/>
@@ -3276,24 +3122,24 @@
       <c r="Z50" s="8"/>
     </row>
     <row r="51" spans="1:26" ht="18" customHeight="1">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
-      <c r="R51" s="8"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
       <c r="S51" s="8"/>
       <c r="T51" s="8"/>
       <c r="U51" s="8"/>
@@ -3331,7 +3177,7 @@
       <c r="Y52" s="8"/>
       <c r="Z52" s="8"/>
     </row>
-    <row r="53" spans="1:26" ht="18" customHeight="1">
+    <row r="53" spans="1:26" ht="55.5" customHeight="1">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -3723,7 +3569,7 @@
       <c r="Y66" s="8"/>
       <c r="Z66" s="8"/>
     </row>
-    <row r="67" spans="1:26" ht="18" customHeight="1">
+    <row r="67" spans="1:26" ht="59" customHeight="1">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -3807,7 +3653,7 @@
       <c r="Y69" s="8"/>
       <c r="Z69" s="8"/>
     </row>
-    <row r="70" spans="1:26" ht="18" customHeight="1">
+    <row r="70" spans="1:26" ht="12.75" customHeight="1">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -4115,7 +3961,7 @@
       <c r="Y80" s="8"/>
       <c r="Z80" s="8"/>
     </row>
-    <row r="81" spans="1:26" ht="12.75" customHeight="1">
+    <row r="81" spans="1:26" ht="61.5" customHeight="1">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
@@ -4143,7 +3989,7 @@
       <c r="Y81" s="8"/>
       <c r="Z81" s="8"/>
     </row>
-    <row r="82" spans="1:26" ht="12.75" customHeight="1">
+    <row r="82" spans="1:26" ht="46" customHeight="1">
       <c r="A82" s="8"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
@@ -27931,8 +27777,6 @@
       <c r="M931" s="8"/>
       <c r="N931" s="8"/>
       <c r="O931" s="8"/>
-      <c r="P931" s="8"/>
-      <c r="Q931" s="8"/>
       <c r="R931" s="8"/>
       <c r="S931" s="8"/>
       <c r="T931" s="8"/>
@@ -27944,23 +27788,6 @@
       <c r="Z931" s="8"/>
     </row>
     <row r="932" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A932" s="8"/>
-      <c r="B932" s="8"/>
-      <c r="C932" s="8"/>
-      <c r="D932" s="8"/>
-      <c r="E932" s="8"/>
-      <c r="F932" s="8"/>
-      <c r="G932" s="8"/>
-      <c r="H932" s="8"/>
-      <c r="I932" s="8"/>
-      <c r="J932" s="8"/>
-      <c r="K932" s="8"/>
-      <c r="L932" s="8"/>
-      <c r="M932" s="8"/>
-      <c r="N932" s="8"/>
-      <c r="O932" s="8"/>
-      <c r="P932" s="8"/>
-      <c r="Q932" s="8"/>
       <c r="R932" s="8"/>
       <c r="S932" s="8"/>
       <c r="T932" s="8"/>
@@ -27972,23 +27799,6 @@
       <c r="Z932" s="8"/>
     </row>
     <row r="933" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A933" s="8"/>
-      <c r="B933" s="8"/>
-      <c r="C933" s="8"/>
-      <c r="D933" s="8"/>
-      <c r="E933" s="8"/>
-      <c r="F933" s="8"/>
-      <c r="G933" s="8"/>
-      <c r="H933" s="8"/>
-      <c r="I933" s="8"/>
-      <c r="J933" s="8"/>
-      <c r="K933" s="8"/>
-      <c r="L933" s="8"/>
-      <c r="M933" s="8"/>
-      <c r="N933" s="8"/>
-      <c r="O933" s="8"/>
-      <c r="P933" s="8"/>
-      <c r="Q933" s="8"/>
       <c r="R933" s="8"/>
       <c r="S933" s="8"/>
       <c r="T933" s="8"/>
@@ -28000,23 +27810,6 @@
       <c r="Z933" s="8"/>
     </row>
     <row r="934" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A934" s="8"/>
-      <c r="B934" s="8"/>
-      <c r="C934" s="8"/>
-      <c r="D934" s="8"/>
-      <c r="E934" s="8"/>
-      <c r="F934" s="8"/>
-      <c r="G934" s="8"/>
-      <c r="H934" s="8"/>
-      <c r="I934" s="8"/>
-      <c r="J934" s="8"/>
-      <c r="K934" s="8"/>
-      <c r="L934" s="8"/>
-      <c r="M934" s="8"/>
-      <c r="N934" s="8"/>
-      <c r="O934" s="8"/>
-      <c r="P934" s="8"/>
-      <c r="Q934" s="8"/>
       <c r="R934" s="8"/>
       <c r="S934" s="8"/>
       <c r="T934" s="8"/>
@@ -28028,23 +27821,6 @@
       <c r="Z934" s="8"/>
     </row>
     <row r="935" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A935" s="8"/>
-      <c r="B935" s="8"/>
-      <c r="C935" s="8"/>
-      <c r="D935" s="8"/>
-      <c r="E935" s="8"/>
-      <c r="F935" s="8"/>
-      <c r="G935" s="8"/>
-      <c r="H935" s="8"/>
-      <c r="I935" s="8"/>
-      <c r="J935" s="8"/>
-      <c r="K935" s="8"/>
-      <c r="L935" s="8"/>
-      <c r="M935" s="8"/>
-      <c r="N935" s="8"/>
-      <c r="O935" s="8"/>
-      <c r="P935" s="8"/>
-      <c r="Q935" s="8"/>
       <c r="R935" s="8"/>
       <c r="S935" s="8"/>
       <c r="T935" s="8"/>
@@ -28056,23 +27832,6 @@
       <c r="Z935" s="8"/>
     </row>
     <row r="936" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A936" s="8"/>
-      <c r="B936" s="8"/>
-      <c r="C936" s="8"/>
-      <c r="D936" s="8"/>
-      <c r="E936" s="8"/>
-      <c r="F936" s="8"/>
-      <c r="G936" s="8"/>
-      <c r="H936" s="8"/>
-      <c r="I936" s="8"/>
-      <c r="J936" s="8"/>
-      <c r="K936" s="8"/>
-      <c r="L936" s="8"/>
-      <c r="M936" s="8"/>
-      <c r="N936" s="8"/>
-      <c r="O936" s="8"/>
-      <c r="P936" s="8"/>
-      <c r="Q936" s="8"/>
       <c r="R936" s="8"/>
       <c r="S936" s="8"/>
       <c r="T936" s="8"/>
@@ -28084,23 +27843,6 @@
       <c r="Z936" s="8"/>
     </row>
     <row r="937" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A937" s="8"/>
-      <c r="B937" s="8"/>
-      <c r="C937" s="8"/>
-      <c r="D937" s="8"/>
-      <c r="E937" s="8"/>
-      <c r="F937" s="8"/>
-      <c r="G937" s="8"/>
-      <c r="H937" s="8"/>
-      <c r="I937" s="8"/>
-      <c r="J937" s="8"/>
-      <c r="K937" s="8"/>
-      <c r="L937" s="8"/>
-      <c r="M937" s="8"/>
-      <c r="N937" s="8"/>
-      <c r="O937" s="8"/>
-      <c r="P937" s="8"/>
-      <c r="Q937" s="8"/>
       <c r="R937" s="8"/>
       <c r="S937" s="8"/>
       <c r="T937" s="8"/>
@@ -28112,23 +27854,6 @@
       <c r="Z937" s="8"/>
     </row>
     <row r="938" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A938" s="8"/>
-      <c r="B938" s="8"/>
-      <c r="C938" s="8"/>
-      <c r="D938" s="8"/>
-      <c r="E938" s="8"/>
-      <c r="F938" s="8"/>
-      <c r="G938" s="8"/>
-      <c r="H938" s="8"/>
-      <c r="I938" s="8"/>
-      <c r="J938" s="8"/>
-      <c r="K938" s="8"/>
-      <c r="L938" s="8"/>
-      <c r="M938" s="8"/>
-      <c r="N938" s="8"/>
-      <c r="O938" s="8"/>
-      <c r="P938" s="8"/>
-      <c r="Q938" s="8"/>
       <c r="R938" s="8"/>
       <c r="S938" s="8"/>
       <c r="T938" s="8"/>
@@ -28140,23 +27865,6 @@
       <c r="Z938" s="8"/>
     </row>
     <row r="939" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A939" s="8"/>
-      <c r="B939" s="8"/>
-      <c r="C939" s="8"/>
-      <c r="D939" s="8"/>
-      <c r="E939" s="8"/>
-      <c r="F939" s="8"/>
-      <c r="G939" s="8"/>
-      <c r="H939" s="8"/>
-      <c r="I939" s="8"/>
-      <c r="J939" s="8"/>
-      <c r="K939" s="8"/>
-      <c r="L939" s="8"/>
-      <c r="M939" s="8"/>
-      <c r="N939" s="8"/>
-      <c r="O939" s="8"/>
-      <c r="P939" s="8"/>
-      <c r="Q939" s="8"/>
       <c r="R939" s="8"/>
       <c r="S939" s="8"/>
       <c r="T939" s="8"/>
@@ -28168,23 +27876,6 @@
       <c r="Z939" s="8"/>
     </row>
     <row r="940" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A940" s="8"/>
-      <c r="B940" s="8"/>
-      <c r="C940" s="8"/>
-      <c r="D940" s="8"/>
-      <c r="E940" s="8"/>
-      <c r="F940" s="8"/>
-      <c r="G940" s="8"/>
-      <c r="H940" s="8"/>
-      <c r="I940" s="8"/>
-      <c r="J940" s="8"/>
-      <c r="K940" s="8"/>
-      <c r="L940" s="8"/>
-      <c r="M940" s="8"/>
-      <c r="N940" s="8"/>
-      <c r="O940" s="8"/>
-      <c r="P940" s="8"/>
-      <c r="Q940" s="8"/>
       <c r="R940" s="8"/>
       <c r="S940" s="8"/>
       <c r="T940" s="8"/>
@@ -28196,23 +27887,6 @@
       <c r="Z940" s="8"/>
     </row>
     <row r="941" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A941" s="8"/>
-      <c r="B941" s="8"/>
-      <c r="C941" s="8"/>
-      <c r="D941" s="8"/>
-      <c r="E941" s="8"/>
-      <c r="F941" s="8"/>
-      <c r="G941" s="8"/>
-      <c r="H941" s="8"/>
-      <c r="I941" s="8"/>
-      <c r="J941" s="8"/>
-      <c r="K941" s="8"/>
-      <c r="L941" s="8"/>
-      <c r="M941" s="8"/>
-      <c r="N941" s="8"/>
-      <c r="O941" s="8"/>
-      <c r="P941" s="8"/>
-      <c r="Q941" s="8"/>
       <c r="R941" s="8"/>
       <c r="S941" s="8"/>
       <c r="T941" s="8"/>
@@ -28224,23 +27898,6 @@
       <c r="Z941" s="8"/>
     </row>
     <row r="942" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A942" s="8"/>
-      <c r="B942" s="8"/>
-      <c r="C942" s="8"/>
-      <c r="D942" s="8"/>
-      <c r="E942" s="8"/>
-      <c r="F942" s="8"/>
-      <c r="G942" s="8"/>
-      <c r="H942" s="8"/>
-      <c r="I942" s="8"/>
-      <c r="J942" s="8"/>
-      <c r="K942" s="8"/>
-      <c r="L942" s="8"/>
-      <c r="M942" s="8"/>
-      <c r="N942" s="8"/>
-      <c r="O942" s="8"/>
-      <c r="P942" s="8"/>
-      <c r="Q942" s="8"/>
       <c r="R942" s="8"/>
       <c r="S942" s="8"/>
       <c r="T942" s="8"/>
@@ -28252,23 +27909,6 @@
       <c r="Z942" s="8"/>
     </row>
     <row r="943" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A943" s="8"/>
-      <c r="B943" s="8"/>
-      <c r="C943" s="8"/>
-      <c r="D943" s="8"/>
-      <c r="E943" s="8"/>
-      <c r="F943" s="8"/>
-      <c r="G943" s="8"/>
-      <c r="H943" s="8"/>
-      <c r="I943" s="8"/>
-      <c r="J943" s="8"/>
-      <c r="K943" s="8"/>
-      <c r="L943" s="8"/>
-      <c r="M943" s="8"/>
-      <c r="N943" s="8"/>
-      <c r="O943" s="8"/>
-      <c r="P943" s="8"/>
-      <c r="Q943" s="8"/>
       <c r="R943" s="8"/>
       <c r="S943" s="8"/>
       <c r="T943" s="8"/>
@@ -28280,23 +27920,6 @@
       <c r="Z943" s="8"/>
     </row>
     <row r="944" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A944" s="8"/>
-      <c r="B944" s="8"/>
-      <c r="C944" s="8"/>
-      <c r="D944" s="8"/>
-      <c r="E944" s="8"/>
-      <c r="F944" s="8"/>
-      <c r="G944" s="8"/>
-      <c r="H944" s="8"/>
-      <c r="I944" s="8"/>
-      <c r="J944" s="8"/>
-      <c r="K944" s="8"/>
-      <c r="L944" s="8"/>
-      <c r="M944" s="8"/>
-      <c r="N944" s="8"/>
-      <c r="O944" s="8"/>
-      <c r="P944" s="8"/>
-      <c r="Q944" s="8"/>
       <c r="R944" s="8"/>
       <c r="S944" s="8"/>
       <c r="T944" s="8"/>
@@ -28307,24 +27930,7 @@
       <c r="Y944" s="8"/>
       <c r="Z944" s="8"/>
     </row>
-    <row r="945" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A945" s="8"/>
-      <c r="B945" s="8"/>
-      <c r="C945" s="8"/>
-      <c r="D945" s="8"/>
-      <c r="E945" s="8"/>
-      <c r="F945" s="8"/>
-      <c r="G945" s="8"/>
-      <c r="H945" s="8"/>
-      <c r="I945" s="8"/>
-      <c r="J945" s="8"/>
-      <c r="K945" s="8"/>
-      <c r="L945" s="8"/>
-      <c r="M945" s="8"/>
-      <c r="N945" s="8"/>
-      <c r="O945" s="8"/>
-      <c r="P945" s="8"/>
-      <c r="Q945" s="8"/>
+    <row r="945" spans="18:26" ht="12.75" customHeight="1">
       <c r="R945" s="8"/>
       <c r="S945" s="8"/>
       <c r="T945" s="8"/>
@@ -28335,24 +27941,7 @@
       <c r="Y945" s="8"/>
       <c r="Z945" s="8"/>
     </row>
-    <row r="946" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A946" s="8"/>
-      <c r="B946" s="8"/>
-      <c r="C946" s="8"/>
-      <c r="D946" s="8"/>
-      <c r="E946" s="8"/>
-      <c r="F946" s="8"/>
-      <c r="G946" s="8"/>
-      <c r="H946" s="8"/>
-      <c r="I946" s="8"/>
-      <c r="J946" s="8"/>
-      <c r="K946" s="8"/>
-      <c r="L946" s="8"/>
-      <c r="M946" s="8"/>
-      <c r="N946" s="8"/>
-      <c r="O946" s="8"/>
-      <c r="P946" s="8"/>
-      <c r="Q946" s="8"/>
+    <row r="946" spans="18:26" ht="12.75" customHeight="1">
       <c r="R946" s="8"/>
       <c r="S946" s="8"/>
       <c r="T946" s="8"/>
@@ -28363,24 +27952,7 @@
       <c r="Y946" s="8"/>
       <c r="Z946" s="8"/>
     </row>
-    <row r="947" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A947" s="8"/>
-      <c r="B947" s="8"/>
-      <c r="C947" s="8"/>
-      <c r="D947" s="8"/>
-      <c r="E947" s="8"/>
-      <c r="F947" s="8"/>
-      <c r="G947" s="8"/>
-      <c r="H947" s="8"/>
-      <c r="I947" s="8"/>
-      <c r="J947" s="8"/>
-      <c r="K947" s="8"/>
-      <c r="L947" s="8"/>
-      <c r="M947" s="8"/>
-      <c r="N947" s="8"/>
-      <c r="O947" s="8"/>
-      <c r="P947" s="8"/>
-      <c r="Q947" s="8"/>
+    <row r="947" spans="18:26" ht="12.75" customHeight="1">
       <c r="R947" s="8"/>
       <c r="S947" s="8"/>
       <c r="T947" s="8"/>
@@ -28391,24 +27963,7 @@
       <c r="Y947" s="8"/>
       <c r="Z947" s="8"/>
     </row>
-    <row r="948" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A948" s="8"/>
-      <c r="B948" s="8"/>
-      <c r="C948" s="8"/>
-      <c r="D948" s="8"/>
-      <c r="E948" s="8"/>
-      <c r="F948" s="8"/>
-      <c r="G948" s="8"/>
-      <c r="H948" s="8"/>
-      <c r="I948" s="8"/>
-      <c r="J948" s="8"/>
-      <c r="K948" s="8"/>
-      <c r="L948" s="8"/>
-      <c r="M948" s="8"/>
-      <c r="N948" s="8"/>
-      <c r="O948" s="8"/>
-      <c r="P948" s="8"/>
-      <c r="Q948" s="8"/>
+    <row r="948" spans="18:26" ht="12.75" customHeight="1">
       <c r="R948" s="8"/>
       <c r="S948" s="8"/>
       <c r="T948" s="8"/>
@@ -28419,24 +27974,7 @@
       <c r="Y948" s="8"/>
       <c r="Z948" s="8"/>
     </row>
-    <row r="949" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A949" s="8"/>
-      <c r="B949" s="8"/>
-      <c r="C949" s="8"/>
-      <c r="D949" s="8"/>
-      <c r="E949" s="8"/>
-      <c r="F949" s="8"/>
-      <c r="G949" s="8"/>
-      <c r="H949" s="8"/>
-      <c r="I949" s="8"/>
-      <c r="J949" s="8"/>
-      <c r="K949" s="8"/>
-      <c r="L949" s="8"/>
-      <c r="M949" s="8"/>
-      <c r="N949" s="8"/>
-      <c r="O949" s="8"/>
-      <c r="P949" s="8"/>
-      <c r="Q949" s="8"/>
+    <row r="949" spans="18:26" ht="12.75" customHeight="1">
       <c r="R949" s="8"/>
       <c r="S949" s="8"/>
       <c r="T949" s="8"/>
@@ -28447,24 +27985,7 @@
       <c r="Y949" s="8"/>
       <c r="Z949" s="8"/>
     </row>
-    <row r="950" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A950" s="8"/>
-      <c r="B950" s="8"/>
-      <c r="C950" s="8"/>
-      <c r="D950" s="8"/>
-      <c r="E950" s="8"/>
-      <c r="F950" s="8"/>
-      <c r="G950" s="8"/>
-      <c r="H950" s="8"/>
-      <c r="I950" s="8"/>
-      <c r="J950" s="8"/>
-      <c r="K950" s="8"/>
-      <c r="L950" s="8"/>
-      <c r="M950" s="8"/>
-      <c r="N950" s="8"/>
-      <c r="O950" s="8"/>
-      <c r="P950" s="8"/>
-      <c r="Q950" s="8"/>
+    <row r="950" spans="18:26" ht="12.75" customHeight="1">
       <c r="R950" s="8"/>
       <c r="S950" s="8"/>
       <c r="T950" s="8"/>
@@ -28475,24 +27996,7 @@
       <c r="Y950" s="8"/>
       <c r="Z950" s="8"/>
     </row>
-    <row r="951" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A951" s="8"/>
-      <c r="B951" s="8"/>
-      <c r="C951" s="8"/>
-      <c r="D951" s="8"/>
-      <c r="E951" s="8"/>
-      <c r="F951" s="8"/>
-      <c r="G951" s="8"/>
-      <c r="H951" s="8"/>
-      <c r="I951" s="8"/>
-      <c r="J951" s="8"/>
-      <c r="K951" s="8"/>
-      <c r="L951" s="8"/>
-      <c r="M951" s="8"/>
-      <c r="N951" s="8"/>
-      <c r="O951" s="8"/>
-      <c r="P951" s="8"/>
-      <c r="Q951" s="8"/>
+    <row r="951" spans="18:26" ht="12.75" customHeight="1">
       <c r="R951" s="8"/>
       <c r="S951" s="8"/>
       <c r="T951" s="8"/>
@@ -28503,24 +28007,7 @@
       <c r="Y951" s="8"/>
       <c r="Z951" s="8"/>
     </row>
-    <row r="952" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A952" s="8"/>
-      <c r="B952" s="8"/>
-      <c r="C952" s="8"/>
-      <c r="D952" s="8"/>
-      <c r="E952" s="8"/>
-      <c r="F952" s="8"/>
-      <c r="G952" s="8"/>
-      <c r="H952" s="8"/>
-      <c r="I952" s="8"/>
-      <c r="J952" s="8"/>
-      <c r="K952" s="8"/>
-      <c r="L952" s="8"/>
-      <c r="M952" s="8"/>
-      <c r="N952" s="8"/>
-      <c r="O952" s="8"/>
-      <c r="P952" s="8"/>
-      <c r="Q952" s="8"/>
+    <row r="952" spans="18:26" ht="12.75" customHeight="1">
       <c r="R952" s="8"/>
       <c r="S952" s="8"/>
       <c r="T952" s="8"/>
@@ -28531,24 +28018,7 @@
       <c r="Y952" s="8"/>
       <c r="Z952" s="8"/>
     </row>
-    <row r="953" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A953" s="8"/>
-      <c r="B953" s="8"/>
-      <c r="C953" s="8"/>
-      <c r="D953" s="8"/>
-      <c r="E953" s="8"/>
-      <c r="F953" s="8"/>
-      <c r="G953" s="8"/>
-      <c r="H953" s="8"/>
-      <c r="I953" s="8"/>
-      <c r="J953" s="8"/>
-      <c r="K953" s="8"/>
-      <c r="L953" s="8"/>
-      <c r="M953" s="8"/>
-      <c r="N953" s="8"/>
-      <c r="O953" s="8"/>
-      <c r="P953" s="8"/>
-      <c r="Q953" s="8"/>
+    <row r="953" spans="18:26" ht="12.75" customHeight="1">
       <c r="R953" s="8"/>
       <c r="S953" s="8"/>
       <c r="T953" s="8"/>
@@ -28559,24 +28029,7 @@
       <c r="Y953" s="8"/>
       <c r="Z953" s="8"/>
     </row>
-    <row r="954" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A954" s="8"/>
-      <c r="B954" s="8"/>
-      <c r="C954" s="8"/>
-      <c r="D954" s="8"/>
-      <c r="E954" s="8"/>
-      <c r="F954" s="8"/>
-      <c r="G954" s="8"/>
-      <c r="H954" s="8"/>
-      <c r="I954" s="8"/>
-      <c r="J954" s="8"/>
-      <c r="K954" s="8"/>
-      <c r="L954" s="8"/>
-      <c r="M954" s="8"/>
-      <c r="N954" s="8"/>
-      <c r="O954" s="8"/>
-      <c r="P954" s="8"/>
-      <c r="Q954" s="8"/>
+    <row r="954" spans="18:26" ht="12.75" customHeight="1">
       <c r="R954" s="8"/>
       <c r="S954" s="8"/>
       <c r="T954" s="8"/>
@@ -28587,24 +28040,7 @@
       <c r="Y954" s="8"/>
       <c r="Z954" s="8"/>
     </row>
-    <row r="955" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A955" s="8"/>
-      <c r="B955" s="8"/>
-      <c r="C955" s="8"/>
-      <c r="D955" s="8"/>
-      <c r="E955" s="8"/>
-      <c r="F955" s="8"/>
-      <c r="G955" s="8"/>
-      <c r="H955" s="8"/>
-      <c r="I955" s="8"/>
-      <c r="J955" s="8"/>
-      <c r="K955" s="8"/>
-      <c r="L955" s="8"/>
-      <c r="M955" s="8"/>
-      <c r="N955" s="8"/>
-      <c r="O955" s="8"/>
-      <c r="P955" s="8"/>
-      <c r="Q955" s="8"/>
+    <row r="955" spans="18:26" ht="12.75" customHeight="1">
       <c r="R955" s="8"/>
       <c r="S955" s="8"/>
       <c r="T955" s="8"/>
@@ -28615,24 +28051,7 @@
       <c r="Y955" s="8"/>
       <c r="Z955" s="8"/>
     </row>
-    <row r="956" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A956" s="8"/>
-      <c r="B956" s="8"/>
-      <c r="C956" s="8"/>
-      <c r="D956" s="8"/>
-      <c r="E956" s="8"/>
-      <c r="F956" s="8"/>
-      <c r="G956" s="8"/>
-      <c r="H956" s="8"/>
-      <c r="I956" s="8"/>
-      <c r="J956" s="8"/>
-      <c r="K956" s="8"/>
-      <c r="L956" s="8"/>
-      <c r="M956" s="8"/>
-      <c r="N956" s="8"/>
-      <c r="O956" s="8"/>
-      <c r="P956" s="8"/>
-      <c r="Q956" s="8"/>
+    <row r="956" spans="18:26" ht="12.75" customHeight="1">
       <c r="R956" s="8"/>
       <c r="S956" s="8"/>
       <c r="T956" s="8"/>
@@ -28643,24 +28062,7 @@
       <c r="Y956" s="8"/>
       <c r="Z956" s="8"/>
     </row>
-    <row r="957" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A957" s="8"/>
-      <c r="B957" s="8"/>
-      <c r="C957" s="8"/>
-      <c r="D957" s="8"/>
-      <c r="E957" s="8"/>
-      <c r="F957" s="8"/>
-      <c r="G957" s="8"/>
-      <c r="H957" s="8"/>
-      <c r="I957" s="8"/>
-      <c r="J957" s="8"/>
-      <c r="K957" s="8"/>
-      <c r="L957" s="8"/>
-      <c r="M957" s="8"/>
-      <c r="N957" s="8"/>
-      <c r="O957" s="8"/>
-      <c r="P957" s="8"/>
-      <c r="Q957" s="8"/>
+    <row r="957" spans="18:26" ht="12.75" customHeight="1">
       <c r="R957" s="8"/>
       <c r="S957" s="8"/>
       <c r="T957" s="8"/>
@@ -28671,24 +28073,7 @@
       <c r="Y957" s="8"/>
       <c r="Z957" s="8"/>
     </row>
-    <row r="958" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A958" s="8"/>
-      <c r="B958" s="8"/>
-      <c r="C958" s="8"/>
-      <c r="D958" s="8"/>
-      <c r="E958" s="8"/>
-      <c r="F958" s="8"/>
-      <c r="G958" s="8"/>
-      <c r="H958" s="8"/>
-      <c r="I958" s="8"/>
-      <c r="J958" s="8"/>
-      <c r="K958" s="8"/>
-      <c r="L958" s="8"/>
-      <c r="M958" s="8"/>
-      <c r="N958" s="8"/>
-      <c r="O958" s="8"/>
-      <c r="P958" s="8"/>
-      <c r="Q958" s="8"/>
+    <row r="958" spans="18:26" ht="12.75" customHeight="1">
       <c r="R958" s="8"/>
       <c r="S958" s="8"/>
       <c r="T958" s="8"/>
@@ -28699,24 +28084,7 @@
       <c r="Y958" s="8"/>
       <c r="Z958" s="8"/>
     </row>
-    <row r="959" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A959" s="8"/>
-      <c r="B959" s="8"/>
-      <c r="C959" s="8"/>
-      <c r="D959" s="8"/>
-      <c r="E959" s="8"/>
-      <c r="F959" s="8"/>
-      <c r="G959" s="8"/>
-      <c r="H959" s="8"/>
-      <c r="I959" s="8"/>
-      <c r="J959" s="8"/>
-      <c r="K959" s="8"/>
-      <c r="L959" s="8"/>
-      <c r="M959" s="8"/>
-      <c r="N959" s="8"/>
-      <c r="O959" s="8"/>
-      <c r="P959" s="8"/>
-      <c r="Q959" s="8"/>
+    <row r="959" spans="18:26" ht="12.75" customHeight="1">
       <c r="R959" s="8"/>
       <c r="S959" s="8"/>
       <c r="T959" s="8"/>
@@ -28727,24 +28095,7 @@
       <c r="Y959" s="8"/>
       <c r="Z959" s="8"/>
     </row>
-    <row r="960" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A960" s="8"/>
-      <c r="B960" s="8"/>
-      <c r="C960" s="8"/>
-      <c r="D960" s="8"/>
-      <c r="E960" s="8"/>
-      <c r="F960" s="8"/>
-      <c r="G960" s="8"/>
-      <c r="H960" s="8"/>
-      <c r="I960" s="8"/>
-      <c r="J960" s="8"/>
-      <c r="K960" s="8"/>
-      <c r="L960" s="8"/>
-      <c r="M960" s="8"/>
-      <c r="N960" s="8"/>
-      <c r="O960" s="8"/>
-      <c r="P960" s="8"/>
-      <c r="Q960" s="8"/>
+    <row r="960" spans="18:26" ht="12.75" customHeight="1">
       <c r="R960" s="8"/>
       <c r="S960" s="8"/>
       <c r="T960" s="8"/>
@@ -28755,24 +28106,7 @@
       <c r="Y960" s="8"/>
       <c r="Z960" s="8"/>
     </row>
-    <row r="961" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A961" s="8"/>
-      <c r="B961" s="8"/>
-      <c r="C961" s="8"/>
-      <c r="D961" s="8"/>
-      <c r="E961" s="8"/>
-      <c r="F961" s="8"/>
-      <c r="G961" s="8"/>
-      <c r="H961" s="8"/>
-      <c r="I961" s="8"/>
-      <c r="J961" s="8"/>
-      <c r="K961" s="8"/>
-      <c r="L961" s="8"/>
-      <c r="M961" s="8"/>
-      <c r="N961" s="8"/>
-      <c r="O961" s="8"/>
-      <c r="P961" s="8"/>
-      <c r="Q961" s="8"/>
+    <row r="961" spans="18:26" ht="12.75" customHeight="1">
       <c r="R961" s="8"/>
       <c r="S961" s="8"/>
       <c r="T961" s="8"/>
@@ -28783,24 +28117,7 @@
       <c r="Y961" s="8"/>
       <c r="Z961" s="8"/>
     </row>
-    <row r="962" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A962" s="8"/>
-      <c r="B962" s="8"/>
-      <c r="C962" s="8"/>
-      <c r="D962" s="8"/>
-      <c r="E962" s="8"/>
-      <c r="F962" s="8"/>
-      <c r="G962" s="8"/>
-      <c r="H962" s="8"/>
-      <c r="I962" s="8"/>
-      <c r="J962" s="8"/>
-      <c r="K962" s="8"/>
-      <c r="L962" s="8"/>
-      <c r="M962" s="8"/>
-      <c r="N962" s="8"/>
-      <c r="O962" s="8"/>
-      <c r="P962" s="8"/>
-      <c r="Q962" s="8"/>
+    <row r="962" spans="18:26" ht="12.75" customHeight="1">
       <c r="R962" s="8"/>
       <c r="S962" s="8"/>
       <c r="T962" s="8"/>
@@ -28811,24 +28128,7 @@
       <c r="Y962" s="8"/>
       <c r="Z962" s="8"/>
     </row>
-    <row r="963" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A963" s="8"/>
-      <c r="B963" s="8"/>
-      <c r="C963" s="8"/>
-      <c r="D963" s="8"/>
-      <c r="E963" s="8"/>
-      <c r="F963" s="8"/>
-      <c r="G963" s="8"/>
-      <c r="H963" s="8"/>
-      <c r="I963" s="8"/>
-      <c r="J963" s="8"/>
-      <c r="K963" s="8"/>
-      <c r="L963" s="8"/>
-      <c r="M963" s="8"/>
-      <c r="N963" s="8"/>
-      <c r="O963" s="8"/>
-      <c r="P963" s="8"/>
-      <c r="Q963" s="8"/>
+    <row r="963" spans="18:26" ht="12.75" customHeight="1">
       <c r="R963" s="8"/>
       <c r="S963" s="8"/>
       <c r="T963" s="8"/>
@@ -28839,24 +28139,7 @@
       <c r="Y963" s="8"/>
       <c r="Z963" s="8"/>
     </row>
-    <row r="964" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A964" s="8"/>
-      <c r="B964" s="8"/>
-      <c r="C964" s="8"/>
-      <c r="D964" s="8"/>
-      <c r="E964" s="8"/>
-      <c r="F964" s="8"/>
-      <c r="G964" s="8"/>
-      <c r="H964" s="8"/>
-      <c r="I964" s="8"/>
-      <c r="J964" s="8"/>
-      <c r="K964" s="8"/>
-      <c r="L964" s="8"/>
-      <c r="M964" s="8"/>
-      <c r="N964" s="8"/>
-      <c r="O964" s="8"/>
-      <c r="P964" s="8"/>
-      <c r="Q964" s="8"/>
+    <row r="964" spans="18:26" ht="12.75" customHeight="1">
       <c r="R964" s="8"/>
       <c r="S964" s="8"/>
       <c r="T964" s="8"/>
@@ -28867,24 +28150,7 @@
       <c r="Y964" s="8"/>
       <c r="Z964" s="8"/>
     </row>
-    <row r="965" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A965" s="8"/>
-      <c r="B965" s="8"/>
-      <c r="C965" s="8"/>
-      <c r="D965" s="8"/>
-      <c r="E965" s="8"/>
-      <c r="F965" s="8"/>
-      <c r="G965" s="8"/>
-      <c r="H965" s="8"/>
-      <c r="I965" s="8"/>
-      <c r="J965" s="8"/>
-      <c r="K965" s="8"/>
-      <c r="L965" s="8"/>
-      <c r="M965" s="8"/>
-      <c r="N965" s="8"/>
-      <c r="O965" s="8"/>
-      <c r="P965" s="8"/>
-      <c r="Q965" s="8"/>
+    <row r="965" spans="18:26" ht="12.75" customHeight="1">
       <c r="R965" s="8"/>
       <c r="S965" s="8"/>
       <c r="T965" s="8"/>
@@ -28895,24 +28161,7 @@
       <c r="Y965" s="8"/>
       <c r="Z965" s="8"/>
     </row>
-    <row r="966" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A966" s="8"/>
-      <c r="B966" s="8"/>
-      <c r="C966" s="8"/>
-      <c r="D966" s="8"/>
-      <c r="E966" s="8"/>
-      <c r="F966" s="8"/>
-      <c r="G966" s="8"/>
-      <c r="H966" s="8"/>
-      <c r="I966" s="8"/>
-      <c r="J966" s="8"/>
-      <c r="K966" s="8"/>
-      <c r="L966" s="8"/>
-      <c r="M966" s="8"/>
-      <c r="N966" s="8"/>
-      <c r="O966" s="8"/>
-      <c r="P966" s="8"/>
-      <c r="Q966" s="8"/>
+    <row r="966" spans="18:26" ht="12.75" customHeight="1">
       <c r="R966" s="8"/>
       <c r="S966" s="8"/>
       <c r="T966" s="8"/>
@@ -28923,24 +28172,7 @@
       <c r="Y966" s="8"/>
       <c r="Z966" s="8"/>
     </row>
-    <row r="967" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A967" s="8"/>
-      <c r="B967" s="8"/>
-      <c r="C967" s="8"/>
-      <c r="D967" s="8"/>
-      <c r="E967" s="8"/>
-      <c r="F967" s="8"/>
-      <c r="G967" s="8"/>
-      <c r="H967" s="8"/>
-      <c r="I967" s="8"/>
-      <c r="J967" s="8"/>
-      <c r="K967" s="8"/>
-      <c r="L967" s="8"/>
-      <c r="M967" s="8"/>
-      <c r="N967" s="8"/>
-      <c r="O967" s="8"/>
-      <c r="P967" s="8"/>
-      <c r="Q967" s="8"/>
+    <row r="967" spans="18:26" ht="12.75" customHeight="1">
       <c r="R967" s="8"/>
       <c r="S967" s="8"/>
       <c r="T967" s="8"/>
@@ -28951,24 +28183,7 @@
       <c r="Y967" s="8"/>
       <c r="Z967" s="8"/>
     </row>
-    <row r="968" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A968" s="8"/>
-      <c r="B968" s="8"/>
-      <c r="C968" s="8"/>
-      <c r="D968" s="8"/>
-      <c r="E968" s="8"/>
-      <c r="F968" s="8"/>
-      <c r="G968" s="8"/>
-      <c r="H968" s="8"/>
-      <c r="I968" s="8"/>
-      <c r="J968" s="8"/>
-      <c r="K968" s="8"/>
-      <c r="L968" s="8"/>
-      <c r="M968" s="8"/>
-      <c r="N968" s="8"/>
-      <c r="O968" s="8"/>
-      <c r="P968" s="8"/>
-      <c r="Q968" s="8"/>
+    <row r="968" spans="18:26" ht="12.75" customHeight="1">
       <c r="R968" s="8"/>
       <c r="S968" s="8"/>
       <c r="T968" s="8"/>
@@ -28979,24 +28194,7 @@
       <c r="Y968" s="8"/>
       <c r="Z968" s="8"/>
     </row>
-    <row r="969" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A969" s="8"/>
-      <c r="B969" s="8"/>
-      <c r="C969" s="8"/>
-      <c r="D969" s="8"/>
-      <c r="E969" s="8"/>
-      <c r="F969" s="8"/>
-      <c r="G969" s="8"/>
-      <c r="H969" s="8"/>
-      <c r="I969" s="8"/>
-      <c r="J969" s="8"/>
-      <c r="K969" s="8"/>
-      <c r="L969" s="8"/>
-      <c r="M969" s="8"/>
-      <c r="N969" s="8"/>
-      <c r="O969" s="8"/>
-      <c r="P969" s="8"/>
-      <c r="Q969" s="8"/>
+    <row r="969" spans="18:26" ht="12.75" customHeight="1">
       <c r="R969" s="8"/>
       <c r="S969" s="8"/>
       <c r="T969" s="8"/>
@@ -29007,24 +28205,7 @@
       <c r="Y969" s="8"/>
       <c r="Z969" s="8"/>
     </row>
-    <row r="970" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A970" s="8"/>
-      <c r="B970" s="8"/>
-      <c r="C970" s="8"/>
-      <c r="D970" s="8"/>
-      <c r="E970" s="8"/>
-      <c r="F970" s="8"/>
-      <c r="G970" s="8"/>
-      <c r="H970" s="8"/>
-      <c r="I970" s="8"/>
-      <c r="J970" s="8"/>
-      <c r="K970" s="8"/>
-      <c r="L970" s="8"/>
-      <c r="M970" s="8"/>
-      <c r="N970" s="8"/>
-      <c r="O970" s="8"/>
-      <c r="P970" s="8"/>
-      <c r="Q970" s="8"/>
+    <row r="970" spans="18:26" ht="12.75" customHeight="1">
       <c r="R970" s="8"/>
       <c r="S970" s="8"/>
       <c r="T970" s="8"/>
@@ -29035,24 +28216,7 @@
       <c r="Y970" s="8"/>
       <c r="Z970" s="8"/>
     </row>
-    <row r="971" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A971" s="8"/>
-      <c r="B971" s="8"/>
-      <c r="C971" s="8"/>
-      <c r="D971" s="8"/>
-      <c r="E971" s="8"/>
-      <c r="F971" s="8"/>
-      <c r="G971" s="8"/>
-      <c r="H971" s="8"/>
-      <c r="I971" s="8"/>
-      <c r="J971" s="8"/>
-      <c r="K971" s="8"/>
-      <c r="L971" s="8"/>
-      <c r="M971" s="8"/>
-      <c r="N971" s="8"/>
-      <c r="O971" s="8"/>
-      <c r="P971" s="8"/>
-      <c r="Q971" s="8"/>
+    <row r="971" spans="18:26" ht="12.75" customHeight="1">
       <c r="R971" s="8"/>
       <c r="S971" s="8"/>
       <c r="T971" s="8"/>
@@ -29063,24 +28227,7 @@
       <c r="Y971" s="8"/>
       <c r="Z971" s="8"/>
     </row>
-    <row r="972" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A972" s="8"/>
-      <c r="B972" s="8"/>
-      <c r="C972" s="8"/>
-      <c r="D972" s="8"/>
-      <c r="E972" s="8"/>
-      <c r="F972" s="8"/>
-      <c r="G972" s="8"/>
-      <c r="H972" s="8"/>
-      <c r="I972" s="8"/>
-      <c r="J972" s="8"/>
-      <c r="K972" s="8"/>
-      <c r="L972" s="8"/>
-      <c r="M972" s="8"/>
-      <c r="N972" s="8"/>
-      <c r="O972" s="8"/>
-      <c r="P972" s="8"/>
-      <c r="Q972" s="8"/>
+    <row r="972" spans="18:26" ht="12.75" customHeight="1">
       <c r="R972" s="8"/>
       <c r="S972" s="8"/>
       <c r="T972" s="8"/>
@@ -29091,24 +28238,7 @@
       <c r="Y972" s="8"/>
       <c r="Z972" s="8"/>
     </row>
-    <row r="973" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A973" s="8"/>
-      <c r="B973" s="8"/>
-      <c r="C973" s="8"/>
-      <c r="D973" s="8"/>
-      <c r="E973" s="8"/>
-      <c r="F973" s="8"/>
-      <c r="G973" s="8"/>
-      <c r="H973" s="8"/>
-      <c r="I973" s="8"/>
-      <c r="J973" s="8"/>
-      <c r="K973" s="8"/>
-      <c r="L973" s="8"/>
-      <c r="M973" s="8"/>
-      <c r="N973" s="8"/>
-      <c r="O973" s="8"/>
-      <c r="P973" s="8"/>
-      <c r="Q973" s="8"/>
+    <row r="973" spans="18:26" ht="12.75" customHeight="1">
       <c r="R973" s="8"/>
       <c r="S973" s="8"/>
       <c r="T973" s="8"/>
@@ -29119,24 +28249,7 @@
       <c r="Y973" s="8"/>
       <c r="Z973" s="8"/>
     </row>
-    <row r="974" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A974" s="8"/>
-      <c r="B974" s="8"/>
-      <c r="C974" s="8"/>
-      <c r="D974" s="8"/>
-      <c r="E974" s="8"/>
-      <c r="F974" s="8"/>
-      <c r="G974" s="8"/>
-      <c r="H974" s="8"/>
-      <c r="I974" s="8"/>
-      <c r="J974" s="8"/>
-      <c r="K974" s="8"/>
-      <c r="L974" s="8"/>
-      <c r="M974" s="8"/>
-      <c r="N974" s="8"/>
-      <c r="O974" s="8"/>
-      <c r="P974" s="8"/>
-      <c r="Q974" s="8"/>
+    <row r="974" spans="18:26" ht="12.75" customHeight="1">
       <c r="R974" s="8"/>
       <c r="S974" s="8"/>
       <c r="T974" s="8"/>
@@ -29147,24 +28260,7 @@
       <c r="Y974" s="8"/>
       <c r="Z974" s="8"/>
     </row>
-    <row r="975" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A975" s="8"/>
-      <c r="B975" s="8"/>
-      <c r="C975" s="8"/>
-      <c r="D975" s="8"/>
-      <c r="E975" s="8"/>
-      <c r="F975" s="8"/>
-      <c r="G975" s="8"/>
-      <c r="H975" s="8"/>
-      <c r="I975" s="8"/>
-      <c r="J975" s="8"/>
-      <c r="K975" s="8"/>
-      <c r="L975" s="8"/>
-      <c r="M975" s="8"/>
-      <c r="N975" s="8"/>
-      <c r="O975" s="8"/>
-      <c r="P975" s="8"/>
-      <c r="Q975" s="8"/>
+    <row r="975" spans="18:26" ht="12.75" customHeight="1">
       <c r="R975" s="8"/>
       <c r="S975" s="8"/>
       <c r="T975" s="8"/>
@@ -29175,24 +28271,7 @@
       <c r="Y975" s="8"/>
       <c r="Z975" s="8"/>
     </row>
-    <row r="976" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A976" s="8"/>
-      <c r="B976" s="8"/>
-      <c r="C976" s="8"/>
-      <c r="D976" s="8"/>
-      <c r="E976" s="8"/>
-      <c r="F976" s="8"/>
-      <c r="G976" s="8"/>
-      <c r="H976" s="8"/>
-      <c r="I976" s="8"/>
-      <c r="J976" s="8"/>
-      <c r="K976" s="8"/>
-      <c r="L976" s="8"/>
-      <c r="M976" s="8"/>
-      <c r="N976" s="8"/>
-      <c r="O976" s="8"/>
-      <c r="P976" s="8"/>
-      <c r="Q976" s="8"/>
+    <row r="976" spans="18:26" ht="12.75" customHeight="1">
       <c r="R976" s="8"/>
       <c r="S976" s="8"/>
       <c r="T976" s="8"/>
@@ -29203,24 +28282,7 @@
       <c r="Y976" s="8"/>
       <c r="Z976" s="8"/>
     </row>
-    <row r="977" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A977" s="8"/>
-      <c r="B977" s="8"/>
-      <c r="C977" s="8"/>
-      <c r="D977" s="8"/>
-      <c r="E977" s="8"/>
-      <c r="F977" s="8"/>
-      <c r="G977" s="8"/>
-      <c r="H977" s="8"/>
-      <c r="I977" s="8"/>
-      <c r="J977" s="8"/>
-      <c r="K977" s="8"/>
-      <c r="L977" s="8"/>
-      <c r="M977" s="8"/>
-      <c r="N977" s="8"/>
-      <c r="O977" s="8"/>
-      <c r="P977" s="8"/>
-      <c r="Q977" s="8"/>
+    <row r="977" spans="18:26" ht="12.75" customHeight="1">
       <c r="R977" s="8"/>
       <c r="S977" s="8"/>
       <c r="T977" s="8"/>
@@ -29231,24 +28293,7 @@
       <c r="Y977" s="8"/>
       <c r="Z977" s="8"/>
     </row>
-    <row r="978" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A978" s="8"/>
-      <c r="B978" s="8"/>
-      <c r="C978" s="8"/>
-      <c r="D978" s="8"/>
-      <c r="E978" s="8"/>
-      <c r="F978" s="8"/>
-      <c r="G978" s="8"/>
-      <c r="H978" s="8"/>
-      <c r="I978" s="8"/>
-      <c r="J978" s="8"/>
-      <c r="K978" s="8"/>
-      <c r="L978" s="8"/>
-      <c r="M978" s="8"/>
-      <c r="N978" s="8"/>
-      <c r="O978" s="8"/>
-      <c r="P978" s="8"/>
-      <c r="Q978" s="8"/>
+    <row r="978" spans="18:26" ht="12.75" customHeight="1">
       <c r="R978" s="8"/>
       <c r="S978" s="8"/>
       <c r="T978" s="8"/>
@@ -29259,24 +28304,7 @@
       <c r="Y978" s="8"/>
       <c r="Z978" s="8"/>
     </row>
-    <row r="979" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A979" s="8"/>
-      <c r="B979" s="8"/>
-      <c r="C979" s="8"/>
-      <c r="D979" s="8"/>
-      <c r="E979" s="8"/>
-      <c r="F979" s="8"/>
-      <c r="G979" s="8"/>
-      <c r="H979" s="8"/>
-      <c r="I979" s="8"/>
-      <c r="J979" s="8"/>
-      <c r="K979" s="8"/>
-      <c r="L979" s="8"/>
-      <c r="M979" s="8"/>
-      <c r="N979" s="8"/>
-      <c r="O979" s="8"/>
-      <c r="P979" s="8"/>
-      <c r="Q979" s="8"/>
+    <row r="979" spans="18:26" ht="12.75" customHeight="1">
       <c r="R979" s="8"/>
       <c r="S979" s="8"/>
       <c r="T979" s="8"/>
@@ -29287,24 +28315,7 @@
       <c r="Y979" s="8"/>
       <c r="Z979" s="8"/>
     </row>
-    <row r="980" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A980" s="8"/>
-      <c r="B980" s="8"/>
-      <c r="C980" s="8"/>
-      <c r="D980" s="8"/>
-      <c r="E980" s="8"/>
-      <c r="F980" s="8"/>
-      <c r="G980" s="8"/>
-      <c r="H980" s="8"/>
-      <c r="I980" s="8"/>
-      <c r="J980" s="8"/>
-      <c r="K980" s="8"/>
-      <c r="L980" s="8"/>
-      <c r="M980" s="8"/>
-      <c r="N980" s="8"/>
-      <c r="O980" s="8"/>
-      <c r="P980" s="8"/>
-      <c r="Q980" s="8"/>
+    <row r="980" spans="18:26" ht="12.75" customHeight="1">
       <c r="R980" s="8"/>
       <c r="S980" s="8"/>
       <c r="T980" s="8"/>
@@ -29315,24 +28326,7 @@
       <c r="Y980" s="8"/>
       <c r="Z980" s="8"/>
     </row>
-    <row r="981" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A981" s="8"/>
-      <c r="B981" s="8"/>
-      <c r="C981" s="8"/>
-      <c r="D981" s="8"/>
-      <c r="E981" s="8"/>
-      <c r="F981" s="8"/>
-      <c r="G981" s="8"/>
-      <c r="H981" s="8"/>
-      <c r="I981" s="8"/>
-      <c r="J981" s="8"/>
-      <c r="K981" s="8"/>
-      <c r="L981" s="8"/>
-      <c r="M981" s="8"/>
-      <c r="N981" s="8"/>
-      <c r="O981" s="8"/>
-      <c r="P981" s="8"/>
-      <c r="Q981" s="8"/>
+    <row r="981" spans="18:26" ht="12.75" customHeight="1">
       <c r="R981" s="8"/>
       <c r="S981" s="8"/>
       <c r="T981" s="8"/>
@@ -29343,24 +28337,7 @@
       <c r="Y981" s="8"/>
       <c r="Z981" s="8"/>
     </row>
-    <row r="982" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A982" s="8"/>
-      <c r="B982" s="8"/>
-      <c r="C982" s="8"/>
-      <c r="D982" s="8"/>
-      <c r="E982" s="8"/>
-      <c r="F982" s="8"/>
-      <c r="G982" s="8"/>
-      <c r="H982" s="8"/>
-      <c r="I982" s="8"/>
-      <c r="J982" s="8"/>
-      <c r="K982" s="8"/>
-      <c r="L982" s="8"/>
-      <c r="M982" s="8"/>
-      <c r="N982" s="8"/>
-      <c r="O982" s="8"/>
-      <c r="P982" s="8"/>
-      <c r="Q982" s="8"/>
+    <row r="982" spans="18:26" ht="12.75" customHeight="1">
       <c r="R982" s="8"/>
       <c r="S982" s="8"/>
       <c r="T982" s="8"/>
@@ -29371,24 +28348,7 @@
       <c r="Y982" s="8"/>
       <c r="Z982" s="8"/>
     </row>
-    <row r="983" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A983" s="8"/>
-      <c r="B983" s="8"/>
-      <c r="C983" s="8"/>
-      <c r="D983" s="8"/>
-      <c r="E983" s="8"/>
-      <c r="F983" s="8"/>
-      <c r="G983" s="8"/>
-      <c r="H983" s="8"/>
-      <c r="I983" s="8"/>
-      <c r="J983" s="8"/>
-      <c r="K983" s="8"/>
-      <c r="L983" s="8"/>
-      <c r="M983" s="8"/>
-      <c r="N983" s="8"/>
-      <c r="O983" s="8"/>
-      <c r="P983" s="8"/>
-      <c r="Q983" s="8"/>
+    <row r="983" spans="18:26" ht="12.75" customHeight="1">
       <c r="R983" s="8"/>
       <c r="S983" s="8"/>
       <c r="T983" s="8"/>
@@ -29399,24 +28359,7 @@
       <c r="Y983" s="8"/>
       <c r="Z983" s="8"/>
     </row>
-    <row r="984" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A984" s="8"/>
-      <c r="B984" s="8"/>
-      <c r="C984" s="8"/>
-      <c r="D984" s="8"/>
-      <c r="E984" s="8"/>
-      <c r="F984" s="8"/>
-      <c r="G984" s="8"/>
-      <c r="H984" s="8"/>
-      <c r="I984" s="8"/>
-      <c r="J984" s="8"/>
-      <c r="K984" s="8"/>
-      <c r="L984" s="8"/>
-      <c r="M984" s="8"/>
-      <c r="N984" s="8"/>
-      <c r="O984" s="8"/>
-      <c r="P984" s="8"/>
-      <c r="Q984" s="8"/>
+    <row r="984" spans="18:26" ht="12.75" customHeight="1">
       <c r="R984" s="8"/>
       <c r="S984" s="8"/>
       <c r="T984" s="8"/>
@@ -29427,24 +28370,7 @@
       <c r="Y984" s="8"/>
       <c r="Z984" s="8"/>
     </row>
-    <row r="985" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A985" s="8"/>
-      <c r="B985" s="8"/>
-      <c r="C985" s="8"/>
-      <c r="D985" s="8"/>
-      <c r="E985" s="8"/>
-      <c r="F985" s="8"/>
-      <c r="G985" s="8"/>
-      <c r="H985" s="8"/>
-      <c r="I985" s="8"/>
-      <c r="J985" s="8"/>
-      <c r="K985" s="8"/>
-      <c r="L985" s="8"/>
-      <c r="M985" s="8"/>
-      <c r="N985" s="8"/>
-      <c r="O985" s="8"/>
-      <c r="P985" s="8"/>
-      <c r="Q985" s="8"/>
+    <row r="985" spans="18:26" ht="12.75" customHeight="1">
       <c r="R985" s="8"/>
       <c r="S985" s="8"/>
       <c r="T985" s="8"/>
@@ -29455,24 +28381,7 @@
       <c r="Y985" s="8"/>
       <c r="Z985" s="8"/>
     </row>
-    <row r="986" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A986" s="8"/>
-      <c r="B986" s="8"/>
-      <c r="C986" s="8"/>
-      <c r="D986" s="8"/>
-      <c r="E986" s="8"/>
-      <c r="F986" s="8"/>
-      <c r="G986" s="8"/>
-      <c r="H986" s="8"/>
-      <c r="I986" s="8"/>
-      <c r="J986" s="8"/>
-      <c r="K986" s="8"/>
-      <c r="L986" s="8"/>
-      <c r="M986" s="8"/>
-      <c r="N986" s="8"/>
-      <c r="O986" s="8"/>
-      <c r="P986" s="8"/>
-      <c r="Q986" s="8"/>
+    <row r="986" spans="18:26" ht="12.75" customHeight="1">
       <c r="R986" s="8"/>
       <c r="S986" s="8"/>
       <c r="T986" s="8"/>
@@ -29483,24 +28392,7 @@
       <c r="Y986" s="8"/>
       <c r="Z986" s="8"/>
     </row>
-    <row r="987" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A987" s="8"/>
-      <c r="B987" s="8"/>
-      <c r="C987" s="8"/>
-      <c r="D987" s="8"/>
-      <c r="E987" s="8"/>
-      <c r="F987" s="8"/>
-      <c r="G987" s="8"/>
-      <c r="H987" s="8"/>
-      <c r="I987" s="8"/>
-      <c r="J987" s="8"/>
-      <c r="K987" s="8"/>
-      <c r="L987" s="8"/>
-      <c r="M987" s="8"/>
-      <c r="N987" s="8"/>
-      <c r="O987" s="8"/>
-      <c r="P987" s="8"/>
-      <c r="Q987" s="8"/>
+    <row r="987" spans="18:26" ht="12.75" customHeight="1">
       <c r="R987" s="8"/>
       <c r="S987" s="8"/>
       <c r="T987" s="8"/>
@@ -29511,24 +28403,7 @@
       <c r="Y987" s="8"/>
       <c r="Z987" s="8"/>
     </row>
-    <row r="988" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A988" s="8"/>
-      <c r="B988" s="8"/>
-      <c r="C988" s="8"/>
-      <c r="D988" s="8"/>
-      <c r="E988" s="8"/>
-      <c r="F988" s="8"/>
-      <c r="G988" s="8"/>
-      <c r="H988" s="8"/>
-      <c r="I988" s="8"/>
-      <c r="J988" s="8"/>
-      <c r="K988" s="8"/>
-      <c r="L988" s="8"/>
-      <c r="M988" s="8"/>
-      <c r="N988" s="8"/>
-      <c r="O988" s="8"/>
-      <c r="P988" s="8"/>
-      <c r="Q988" s="8"/>
+    <row r="988" spans="18:26" ht="12.75" customHeight="1">
       <c r="R988" s="8"/>
       <c r="S988" s="8"/>
       <c r="T988" s="8"/>
@@ -29539,24 +28414,7 @@
       <c r="Y988" s="8"/>
       <c r="Z988" s="8"/>
     </row>
-    <row r="989" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A989" s="8"/>
-      <c r="B989" s="8"/>
-      <c r="C989" s="8"/>
-      <c r="D989" s="8"/>
-      <c r="E989" s="8"/>
-      <c r="F989" s="8"/>
-      <c r="G989" s="8"/>
-      <c r="H989" s="8"/>
-      <c r="I989" s="8"/>
-      <c r="J989" s="8"/>
-      <c r="K989" s="8"/>
-      <c r="L989" s="8"/>
-      <c r="M989" s="8"/>
-      <c r="N989" s="8"/>
-      <c r="O989" s="8"/>
-      <c r="P989" s="8"/>
-      <c r="Q989" s="8"/>
+    <row r="989" spans="18:26" ht="12.75" customHeight="1">
       <c r="R989" s="8"/>
       <c r="S989" s="8"/>
       <c r="T989" s="8"/>
@@ -29567,24 +28425,7 @@
       <c r="Y989" s="8"/>
       <c r="Z989" s="8"/>
     </row>
-    <row r="990" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A990" s="8"/>
-      <c r="B990" s="8"/>
-      <c r="C990" s="8"/>
-      <c r="D990" s="8"/>
-      <c r="E990" s="8"/>
-      <c r="F990" s="8"/>
-      <c r="G990" s="8"/>
-      <c r="H990" s="8"/>
-      <c r="I990" s="8"/>
-      <c r="J990" s="8"/>
-      <c r="K990" s="8"/>
-      <c r="L990" s="8"/>
-      <c r="M990" s="8"/>
-      <c r="N990" s="8"/>
-      <c r="O990" s="8"/>
-      <c r="P990" s="8"/>
-      <c r="Q990" s="8"/>
+    <row r="990" spans="18:26" ht="12.75" customHeight="1">
       <c r="R990" s="8"/>
       <c r="S990" s="8"/>
       <c r="T990" s="8"/>
@@ -29595,24 +28436,7 @@
       <c r="Y990" s="8"/>
       <c r="Z990" s="8"/>
     </row>
-    <row r="991" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A991" s="8"/>
-      <c r="B991" s="8"/>
-      <c r="C991" s="8"/>
-      <c r="D991" s="8"/>
-      <c r="E991" s="8"/>
-      <c r="F991" s="8"/>
-      <c r="G991" s="8"/>
-      <c r="H991" s="8"/>
-      <c r="I991" s="8"/>
-      <c r="J991" s="8"/>
-      <c r="K991" s="8"/>
-      <c r="L991" s="8"/>
-      <c r="M991" s="8"/>
-      <c r="N991" s="8"/>
-      <c r="O991" s="8"/>
-      <c r="P991" s="8"/>
-      <c r="Q991" s="8"/>
+    <row r="991" spans="18:26" ht="12.75" customHeight="1">
       <c r="R991" s="8"/>
       <c r="S991" s="8"/>
       <c r="T991" s="8"/>
@@ -29623,24 +28447,7 @@
       <c r="Y991" s="8"/>
       <c r="Z991" s="8"/>
     </row>
-    <row r="992" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A992" s="8"/>
-      <c r="B992" s="8"/>
-      <c r="C992" s="8"/>
-      <c r="D992" s="8"/>
-      <c r="E992" s="8"/>
-      <c r="F992" s="8"/>
-      <c r="G992" s="8"/>
-      <c r="H992" s="8"/>
-      <c r="I992" s="8"/>
-      <c r="J992" s="8"/>
-      <c r="K992" s="8"/>
-      <c r="L992" s="8"/>
-      <c r="M992" s="8"/>
-      <c r="N992" s="8"/>
-      <c r="O992" s="8"/>
-      <c r="P992" s="8"/>
-      <c r="Q992" s="8"/>
+    <row r="992" spans="18:26" ht="12.75" customHeight="1">
       <c r="R992" s="8"/>
       <c r="S992" s="8"/>
       <c r="T992" s="8"/>
@@ -29651,24 +28458,7 @@
       <c r="Y992" s="8"/>
       <c r="Z992" s="8"/>
     </row>
-    <row r="993" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A993" s="8"/>
-      <c r="B993" s="8"/>
-      <c r="C993" s="8"/>
-      <c r="D993" s="8"/>
-      <c r="E993" s="8"/>
-      <c r="F993" s="8"/>
-      <c r="G993" s="8"/>
-      <c r="H993" s="8"/>
-      <c r="I993" s="8"/>
-      <c r="J993" s="8"/>
-      <c r="K993" s="8"/>
-      <c r="L993" s="8"/>
-      <c r="M993" s="8"/>
-      <c r="N993" s="8"/>
-      <c r="O993" s="8"/>
-      <c r="P993" s="8"/>
-      <c r="Q993" s="8"/>
+    <row r="993" spans="18:26" ht="12.75" customHeight="1">
       <c r="R993" s="8"/>
       <c r="S993" s="8"/>
       <c r="T993" s="8"/>
@@ -29679,24 +28469,7 @@
       <c r="Y993" s="8"/>
       <c r="Z993" s="8"/>
     </row>
-    <row r="994" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A994" s="8"/>
-      <c r="B994" s="8"/>
-      <c r="C994" s="8"/>
-      <c r="D994" s="8"/>
-      <c r="E994" s="8"/>
-      <c r="F994" s="8"/>
-      <c r="G994" s="8"/>
-      <c r="H994" s="8"/>
-      <c r="I994" s="8"/>
-      <c r="J994" s="8"/>
-      <c r="K994" s="8"/>
-      <c r="L994" s="8"/>
-      <c r="M994" s="8"/>
-      <c r="N994" s="8"/>
-      <c r="O994" s="8"/>
-      <c r="P994" s="8"/>
-      <c r="Q994" s="8"/>
+    <row r="994" spans="18:26" ht="12.75" customHeight="1">
       <c r="R994" s="8"/>
       <c r="S994" s="8"/>
       <c r="T994" s="8"/>
@@ -29707,24 +28480,7 @@
       <c r="Y994" s="8"/>
       <c r="Z994" s="8"/>
     </row>
-    <row r="995" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A995" s="8"/>
-      <c r="B995" s="8"/>
-      <c r="C995" s="8"/>
-      <c r="D995" s="8"/>
-      <c r="E995" s="8"/>
-      <c r="F995" s="8"/>
-      <c r="G995" s="8"/>
-      <c r="H995" s="8"/>
-      <c r="I995" s="8"/>
-      <c r="J995" s="8"/>
-      <c r="K995" s="8"/>
-      <c r="L995" s="8"/>
-      <c r="M995" s="8"/>
-      <c r="N995" s="8"/>
-      <c r="O995" s="8"/>
-      <c r="P995" s="8"/>
-      <c r="Q995" s="8"/>
+    <row r="995" spans="18:26" ht="12.75" customHeight="1">
       <c r="R995" s="8"/>
       <c r="S995" s="8"/>
       <c r="T995" s="8"/>
@@ -29735,24 +28491,7 @@
       <c r="Y995" s="8"/>
       <c r="Z995" s="8"/>
     </row>
-    <row r="996" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A996" s="8"/>
-      <c r="B996" s="8"/>
-      <c r="C996" s="8"/>
-      <c r="D996" s="8"/>
-      <c r="E996" s="8"/>
-      <c r="F996" s="8"/>
-      <c r="G996" s="8"/>
-      <c r="H996" s="8"/>
-      <c r="I996" s="8"/>
-      <c r="J996" s="8"/>
-      <c r="K996" s="8"/>
-      <c r="L996" s="8"/>
-      <c r="M996" s="8"/>
-      <c r="N996" s="8"/>
-      <c r="O996" s="8"/>
-      <c r="P996" s="8"/>
-      <c r="Q996" s="8"/>
+    <row r="996" spans="18:26" ht="12.75" customHeight="1">
       <c r="R996" s="8"/>
       <c r="S996" s="8"/>
       <c r="T996" s="8"/>
@@ -29763,24 +28502,7 @@
       <c r="Y996" s="8"/>
       <c r="Z996" s="8"/>
     </row>
-    <row r="997" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A997" s="8"/>
-      <c r="B997" s="8"/>
-      <c r="C997" s="8"/>
-      <c r="D997" s="8"/>
-      <c r="E997" s="8"/>
-      <c r="F997" s="8"/>
-      <c r="G997" s="8"/>
-      <c r="H997" s="8"/>
-      <c r="I997" s="8"/>
-      <c r="J997" s="8"/>
-      <c r="K997" s="8"/>
-      <c r="L997" s="8"/>
-      <c r="M997" s="8"/>
-      <c r="N997" s="8"/>
-      <c r="O997" s="8"/>
-      <c r="P997" s="8"/>
-      <c r="Q997" s="8"/>
+    <row r="997" spans="18:26" ht="12.75" customHeight="1">
       <c r="R997" s="8"/>
       <c r="S997" s="8"/>
       <c r="T997" s="8"/>
@@ -29791,24 +28513,7 @@
       <c r="Y997" s="8"/>
       <c r="Z997" s="8"/>
     </row>
-    <row r="998" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A998" s="8"/>
-      <c r="B998" s="8"/>
-      <c r="C998" s="8"/>
-      <c r="D998" s="8"/>
-      <c r="E998" s="8"/>
-      <c r="F998" s="8"/>
-      <c r="G998" s="8"/>
-      <c r="H998" s="8"/>
-      <c r="I998" s="8"/>
-      <c r="J998" s="8"/>
-      <c r="K998" s="8"/>
-      <c r="L998" s="8"/>
-      <c r="M998" s="8"/>
-      <c r="N998" s="8"/>
-      <c r="O998" s="8"/>
-      <c r="P998" s="8"/>
-      <c r="Q998" s="8"/>
+    <row r="998" spans="18:26" ht="12.75" customHeight="1">
       <c r="R998" s="8"/>
       <c r="S998" s="8"/>
       <c r="T998" s="8"/>
@@ -29819,24 +28524,7 @@
       <c r="Y998" s="8"/>
       <c r="Z998" s="8"/>
     </row>
-    <row r="999" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A999" s="8"/>
-      <c r="B999" s="8"/>
-      <c r="C999" s="8"/>
-      <c r="D999" s="8"/>
-      <c r="E999" s="8"/>
-      <c r="F999" s="8"/>
-      <c r="G999" s="8"/>
-      <c r="H999" s="8"/>
-      <c r="I999" s="8"/>
-      <c r="J999" s="8"/>
-      <c r="K999" s="8"/>
-      <c r="L999" s="8"/>
-      <c r="M999" s="8"/>
-      <c r="N999" s="8"/>
-      <c r="O999" s="8"/>
-      <c r="P999" s="8"/>
-      <c r="Q999" s="8"/>
+    <row r="999" spans="18:26" ht="12.75" customHeight="1">
       <c r="R999" s="8"/>
       <c r="S999" s="8"/>
       <c r="T999" s="8"/>
@@ -29847,24 +28535,7 @@
       <c r="Y999" s="8"/>
       <c r="Z999" s="8"/>
     </row>
-    <row r="1000" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1000" s="8"/>
-      <c r="B1000" s="8"/>
-      <c r="C1000" s="8"/>
-      <c r="D1000" s="8"/>
-      <c r="E1000" s="8"/>
-      <c r="F1000" s="8"/>
-      <c r="G1000" s="8"/>
-      <c r="H1000" s="8"/>
-      <c r="I1000" s="8"/>
-      <c r="J1000" s="8"/>
-      <c r="K1000" s="8"/>
-      <c r="L1000" s="8"/>
-      <c r="M1000" s="8"/>
-      <c r="N1000" s="8"/>
-      <c r="O1000" s="8"/>
-      <c r="P1000" s="8"/>
-      <c r="Q1000" s="8"/>
+    <row r="1000" spans="18:26" ht="12.75" customHeight="1">
       <c r="R1000" s="8"/>
       <c r="S1000" s="8"/>
       <c r="T1000" s="8"/>
@@ -29875,24 +28546,7 @@
       <c r="Y1000" s="8"/>
       <c r="Z1000" s="8"/>
     </row>
-    <row r="1001" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1001" s="8"/>
-      <c r="B1001" s="8"/>
-      <c r="C1001" s="8"/>
-      <c r="D1001" s="8"/>
-      <c r="E1001" s="8"/>
-      <c r="F1001" s="8"/>
-      <c r="G1001" s="8"/>
-      <c r="H1001" s="8"/>
-      <c r="I1001" s="8"/>
-      <c r="J1001" s="8"/>
-      <c r="K1001" s="8"/>
-      <c r="L1001" s="8"/>
-      <c r="M1001" s="8"/>
-      <c r="N1001" s="8"/>
-      <c r="O1001" s="8"/>
-      <c r="P1001" s="8"/>
-      <c r="Q1001" s="8"/>
+    <row r="1001" spans="18:26" ht="12.75" customHeight="1">
       <c r="R1001" s="8"/>
       <c r="S1001" s="8"/>
       <c r="T1001" s="8"/>
@@ -29903,24 +28557,7 @@
       <c r="Y1001" s="8"/>
       <c r="Z1001" s="8"/>
     </row>
-    <row r="1002" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1002" s="8"/>
-      <c r="B1002" s="8"/>
-      <c r="C1002" s="8"/>
-      <c r="D1002" s="8"/>
-      <c r="E1002" s="8"/>
-      <c r="F1002" s="8"/>
-      <c r="G1002" s="8"/>
-      <c r="H1002" s="8"/>
-      <c r="I1002" s="8"/>
-      <c r="J1002" s="8"/>
-      <c r="K1002" s="8"/>
-      <c r="L1002" s="8"/>
-      <c r="M1002" s="8"/>
-      <c r="N1002" s="8"/>
-      <c r="O1002" s="8"/>
-      <c r="P1002" s="8"/>
-      <c r="Q1002" s="8"/>
+    <row r="1002" spans="18:26" ht="12.75" customHeight="1">
       <c r="R1002" s="8"/>
       <c r="S1002" s="8"/>
       <c r="T1002" s="8"/>
@@ -29931,24 +28568,7 @@
       <c r="Y1002" s="8"/>
       <c r="Z1002" s="8"/>
     </row>
-    <row r="1003" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1003" s="8"/>
-      <c r="B1003" s="8"/>
-      <c r="C1003" s="8"/>
-      <c r="D1003" s="8"/>
-      <c r="E1003" s="8"/>
-      <c r="F1003" s="8"/>
-      <c r="G1003" s="8"/>
-      <c r="H1003" s="8"/>
-      <c r="I1003" s="8"/>
-      <c r="J1003" s="8"/>
-      <c r="K1003" s="8"/>
-      <c r="L1003" s="8"/>
-      <c r="M1003" s="8"/>
-      <c r="N1003" s="8"/>
-      <c r="O1003" s="8"/>
-      <c r="P1003" s="8"/>
-      <c r="Q1003" s="8"/>
+    <row r="1003" spans="18:26" ht="12.75" customHeight="1">
       <c r="R1003" s="8"/>
       <c r="S1003" s="8"/>
       <c r="T1003" s="8"/>
@@ -29959,24 +28579,7 @@
       <c r="Y1003" s="8"/>
       <c r="Z1003" s="8"/>
     </row>
-    <row r="1004" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1004" s="8"/>
-      <c r="B1004" s="8"/>
-      <c r="C1004" s="8"/>
-      <c r="D1004" s="8"/>
-      <c r="E1004" s="8"/>
-      <c r="F1004" s="8"/>
-      <c r="G1004" s="8"/>
-      <c r="H1004" s="8"/>
-      <c r="I1004" s="8"/>
-      <c r="J1004" s="8"/>
-      <c r="K1004" s="8"/>
-      <c r="L1004" s="8"/>
-      <c r="M1004" s="8"/>
-      <c r="N1004" s="8"/>
-      <c r="O1004" s="8"/>
-      <c r="P1004" s="8"/>
-      <c r="Q1004" s="8"/>
+    <row r="1004" spans="18:26" ht="12.75" customHeight="1">
       <c r="R1004" s="8"/>
       <c r="S1004" s="8"/>
       <c r="T1004" s="8"/>
@@ -29987,76 +28590,21 @@
       <c r="Y1004" s="8"/>
       <c r="Z1004" s="8"/>
     </row>
-    <row r="1005" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A1005" s="8"/>
-      <c r="B1005" s="8"/>
-      <c r="C1005" s="8"/>
-      <c r="D1005" s="8"/>
-      <c r="E1005" s="8"/>
-      <c r="F1005" s="8"/>
-      <c r="G1005" s="8"/>
-      <c r="H1005" s="8"/>
-      <c r="I1005" s="8"/>
-      <c r="J1005" s="8"/>
-      <c r="K1005" s="8"/>
-      <c r="L1005" s="8"/>
-      <c r="M1005" s="8"/>
-      <c r="N1005" s="8"/>
-      <c r="O1005" s="8"/>
-      <c r="P1005" s="8"/>
-      <c r="Q1005" s="8"/>
-      <c r="R1005" s="8"/>
-      <c r="S1005" s="8"/>
-      <c r="T1005" s="8"/>
-      <c r="U1005" s="8"/>
-      <c r="V1005" s="8"/>
-      <c r="W1005" s="8"/>
-      <c r="X1005" s="8"/>
-      <c r="Y1005" s="8"/>
-      <c r="Z1005" s="8"/>
-    </row>
-    <row r="1006" spans="1:26" ht="15" customHeight="1">
-      <c r="A1006" s="8"/>
-      <c r="B1006" s="8"/>
-      <c r="C1006" s="8"/>
-      <c r="D1006" s="8"/>
-      <c r="E1006" s="8"/>
-      <c r="F1006" s="8"/>
-      <c r="G1006" s="8"/>
-      <c r="H1006" s="8"/>
-      <c r="I1006" s="8"/>
-      <c r="J1006" s="8"/>
-      <c r="K1006" s="8"/>
-      <c r="L1006" s="8"/>
-      <c r="M1006" s="8"/>
-      <c r="N1006" s="8"/>
-      <c r="O1006" s="8"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="51">
+  <mergeCells count="47">
     <mergeCell ref="F25:F28"/>
-    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A35:O36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="J39:N39"/>
-    <mergeCell ref="J38:N38"/>
-    <mergeCell ref="J6:O6"/>
     <mergeCell ref="G15:G16"/>
-    <mergeCell ref="J41:N41"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="J40:N40"/>
-    <mergeCell ref="G25:G28"/>
-    <mergeCell ref="A23:G24"/>
-    <mergeCell ref="B20:E20"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="B30:C30"/>
@@ -30064,28 +28612,34 @@
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="B25:C28"/>
     <mergeCell ref="D25:E28"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="F15:F16"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="K6:O6"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="K8:M8"/>
     <mergeCell ref="H15:H16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
     <mergeCell ref="A12:O12"/>
     <mergeCell ref="A13:O13"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="E15:E16"/>
-    <mergeCell ref="I15:L15"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="A14:O14"/>
-    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A35:O35"/>
+    <mergeCell ref="G25:G28"/>
+    <mergeCell ref="A23:G24"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="L40:O40"/>
+    <mergeCell ref="K7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="K9:O9"/>
+    <mergeCell ref="L37:O37"/>
+    <mergeCell ref="L38:O38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Adjust templates, add settings tab
</commit_message>
<xml_diff>
--- a/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
+++ b/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Domain\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA51937-E9DA-494E-9634-C81E696B378B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBDEE02-69B7-4088-B884-54277530777D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,22 +16,22 @@
     <sheet name="Відомість" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="COMPLEX_MERGED_RANGE_1" localSheetId="0">Відомість!$J$6:$O$9</definedName>
-    <definedName name="COMPLEX_MERGED_RANGE_2" localSheetId="0">Відомість!$L$37:$O$40</definedName>
+    <definedName name="COMPLEX_MERGED_RANGE_1" localSheetId="0">Відомість!$L$6:$P$9</definedName>
+    <definedName name="COMPLEX_MERGED_RANGE_2" localSheetId="0">Відомість!$M$37:$P$40</definedName>
     <definedName name="FIELD_HEADER_TITLE" localSheetId="0">Відомість!$A$15</definedName>
     <definedName name="FIELD_NUMBER_NAMES" localSheetId="0">Відомість!$B$20</definedName>
     <definedName name="FIELD_RANGE_0" localSheetId="0">Відомість!$C$4</definedName>
     <definedName name="FIELD_RANGE_1" localSheetId="0">Відомість!$A$3</definedName>
-    <definedName name="FIELD_RANGE_10" localSheetId="0">Відомість!$L$37</definedName>
+    <definedName name="FIELD_RANGE_10" localSheetId="0">Відомість!$M$37</definedName>
     <definedName name="FIELD_RANGE_11" localSheetId="0">Відомість!$C$38</definedName>
-    <definedName name="FIELD_RANGE_12" localSheetId="0">Відомість!$L$38</definedName>
+    <definedName name="FIELD_RANGE_12" localSheetId="0">Відомість!$M$38</definedName>
     <definedName name="FIELD_RANGE_13" localSheetId="0">Відомість!$C$39</definedName>
-    <definedName name="FIELD_RANGE_14" localSheetId="0">Відомість!$L$39</definedName>
+    <definedName name="FIELD_RANGE_14" localSheetId="0">Відомість!$M$39</definedName>
     <definedName name="FIELD_RANGE_15" localSheetId="0">Відомість!$C$40</definedName>
-    <definedName name="FIELD_RANGE_16" localSheetId="0">Відомість!$L$40</definedName>
-    <definedName name="FIELD_RANGE_2" localSheetId="0">Відомість!$K$7</definedName>
-    <definedName name="FIELD_RANGE_3" localSheetId="0">Відомість!$K$8</definedName>
-    <definedName name="FIELD_RANGE_4" localSheetId="0">Відомість!$N$8</definedName>
+    <definedName name="FIELD_RANGE_16" localSheetId="0">Відомість!$M$40</definedName>
+    <definedName name="FIELD_RANGE_2" localSheetId="0">Відомість!$L$7</definedName>
+    <definedName name="FIELD_RANGE_3" localSheetId="0">Відомість!$L$8</definedName>
+    <definedName name="FIELD_RANGE_4" localSheetId="0">Відомість!$O$8</definedName>
     <definedName name="FIELD_RANGE_5" localSheetId="0">Відомість!$A$12</definedName>
     <definedName name="FIELD_RANGE_6" localSheetId="0">Відомість!$A$13</definedName>
     <definedName name="FIELD_RANGE_7" localSheetId="0">Відомість!$A$14</definedName>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>ідентифікаційний код за ЄДРПОУ</t>
   </si>
@@ -309,6 +309,9 @@
   <si>
     <t>Голова комісії:</t>
   </si>
+  <si>
+    <t>Стовпець52</t>
+  </si>
 </sst>
 </file>
 
@@ -438,7 +441,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -462,15 +465,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -487,17 +481,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -848,16 +831,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -885,9 +901,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -919,7 +932,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -948,13 +961,13 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -966,16 +979,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -987,78 +994,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1071,53 +1065,200 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ _₽"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1130,7 +1271,6 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1188,6 +1328,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1341,73 +1482,6 @@
         </left>
         <right style="thin">
           <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ _₽"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
         </right>
         <top style="thin">
           <color rgb="FF000000"/>
@@ -1624,25 +1698,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{48DE2C05-180A-4702-9C30-1CFABF4F8FAC}" name="Table" displayName="Table" ref="A18:O19" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
-  <autoFilter ref="A18:O19" xr:uid="{48DE2C05-180A-4702-9C30-1CFABF4F8FAC}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{66111BEB-9378-4A74-A18F-4AF1F7610B8A}" name="Стовпець1" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{7F02335C-6B7B-481B-AA66-A99D53295D48}" name="Стовпець2" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{AC958478-2380-4462-ADB7-810E91AE2702}" name="Стовпець3" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{4D8DF304-E376-491E-9F7D-7A03F13DBB99}" name="Стовпець4" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{5D79FBC9-1D68-44B0-BD0A-A2F59263FD62}" name="Стовпець5" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{64873108-ECB2-491F-96B4-07CE2637EE51}" name="Стовпець6" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{28BA7FB3-3224-4141-BA1B-28B92F3BBD84}" name="Стовпець7" dataDxfId="8">
-      <calculatedColumnFormula>ROUND(E19*F19,2)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{48DE2C05-180A-4702-9C30-1CFABF4F8FAC}" name="Table" displayName="Table" ref="A18:P19" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A18:P19" xr:uid="{48DE2C05-180A-4702-9C30-1CFABF4F8FAC}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{66111BEB-9378-4A74-A18F-4AF1F7610B8A}" name="Стовпець1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7F02335C-6B7B-481B-AA66-A99D53295D48}" name="Стовпець2" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{AC958478-2380-4462-ADB7-810E91AE2702}" name="Стовпець3" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{4D8DF304-E376-491E-9F7D-7A03F13DBB99}" name="Стовпець4" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{5D79FBC9-1D68-44B0-BD0A-A2F59263FD62}" name="Стовпець5" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{0F061852-471E-46A7-9A27-17017CF4C250}" name="Стовпець52" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{64873108-ECB2-491F-96B4-07CE2637EE51}" name="Стовпець6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{28BA7FB3-3224-4141-BA1B-28B92F3BBD84}" name="Стовпець7" dataDxfId="11">
+      <calculatedColumnFormula>ROUND(E19*G19,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{367C3413-BF3B-423C-A04A-2814E50C87E1}" name="Стовпець8" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{202BCDE3-5F48-4FA4-8C3F-A34C56881D6E}" name="Стовпець9" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{17574747-EE2A-4B01-BB04-855077C0E1EA}" name="Стовпець10" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{12AAD393-3012-4400-B19F-F964366D98C7}" name="Стовпець11" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{0107D3B1-D8D8-43D9-9D6F-679BD5947952}" name="Стовпець12" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{CE8D7C7C-C1EF-43A1-A678-379081133252}" name="Стовпець13" dataDxfId="0"/>
-    <tableColumn id="14" xr3:uid="{9ED438C1-E185-4C3B-A31F-A751FC28DDF0}" name="Стовпець14" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{367C3413-BF3B-423C-A04A-2814E50C87E1}" name="Стовпець8" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{202BCDE3-5F48-4FA4-8C3F-A34C56881D6E}" name="Стовпець9" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{17574747-EE2A-4B01-BB04-855077C0E1EA}" name="Стовпець10" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{12AAD393-3012-4400-B19F-F964366D98C7}" name="Стовпець11" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{0107D3B1-D8D8-43D9-9D6F-679BD5947952}" name="Стовпець12" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{CE8D7C7C-C1EF-43A1-A678-379081133252}" name="Стовпець13" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{9ED438C1-E185-4C3B-A31F-A751FC28DDF0}" name="Стовпець14" dataDxfId="4"/>
     <tableColumn id="15" xr3:uid="{E843A11C-28C0-4349-9D21-39647F8044A0}" name="Стовпець15" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1852,8 +1927,8 @@
   </sheetPr>
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="69" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="69" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1862,11 +1937,11 @@
     <col min="2" max="2" width="24.26953125" style="9" customWidth="1"/>
     <col min="3" max="3" width="8.6328125" style="9" customWidth="1"/>
     <col min="4" max="4" width="8.26953125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="22.90625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" style="9" customWidth="1"/>
+    <col min="5" max="6" width="12.6328125" style="9" customWidth="1"/>
     <col min="7" max="7" width="13.36328125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="9" customWidth="1"/>
-    <col min="9" max="12" width="7.7265625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" style="9" customWidth="1"/>
+    <col min="10" max="12" width="7.7265625" style="9" customWidth="1"/>
     <col min="13" max="14" width="14.453125" style="9" customWidth="1"/>
     <col min="15" max="15" width="14.54296875" style="9" customWidth="1"/>
     <col min="16" max="16" width="14.453125" style="9" customWidth="1"/>
@@ -1933,10 +2008,10 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="77"/>
+      <c r="B3" s="71"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1963,15 +2038,15 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="80" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="47"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="44"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2022,22 +2097,21 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" spans="1:26" ht="18" customHeight="1">
-      <c r="A6" s="79"/>
-      <c r="B6" s="77"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="K6" s="55" t="s">
+      <c r="L6" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="27"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="26"/>
     </row>
     <row r="7" spans="1:26" ht="18" customHeight="1">
       <c r="A7" s="8"/>
@@ -2045,15 +2119,14 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
-      <c r="K7" s="55" t="s">
+      <c r="L7" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="27"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="26"/>
     </row>
     <row r="8" spans="1:26" ht="18" customHeight="1">
       <c r="A8" s="8"/>
@@ -2061,16 +2134,15 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="K8" s="58" t="s">
+      <c r="L8" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="56" t="s">
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="56"/>
-      <c r="P8" s="10"/>
+      <c r="P8" s="87"/>
       <c r="Q8" s="11"/>
     </row>
     <row r="9" spans="1:26" ht="24.75" customHeight="1">
@@ -2079,15 +2151,14 @@
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="K9" s="55" t="s">
+      <c r="L9" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="27"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="26"/>
     </row>
     <row r="10" spans="1:26" ht="18" customHeight="1">
       <c r="A10" s="8"/>
@@ -2107,24 +2178,24 @@
       <c r="Z10" s="11"/>
     </row>
     <row r="11" spans="1:26" ht="18" customHeight="1">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="67"/>
-      <c r="P11" s="8"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
@@ -2137,64 +2208,66 @@
       <c r="Z11" s="11"/>
     </row>
     <row r="12" spans="1:26" ht="18" customHeight="1">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
       <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="1:26" ht="18" customHeight="1">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+      <c r="P13" s="81"/>
       <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="1:26" ht="18" customHeight="1">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="67"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="67"/>
-      <c r="P14" s="12"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
+      <c r="P14" s="102"/>
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:26" ht="81.75" customHeight="1">
@@ -2207,45 +2280,39 @@
       <c r="C15" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="63" t="s">
+      <c r="F15" s="53"/>
+      <c r="G15" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="63" t="s">
+      <c r="H15" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="59" t="s">
+      <c r="I15" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
+      <c r="J15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
       <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="24" customHeight="1">
-      <c r="A16" s="64"/>
+      <c r="A16" s="82"/>
       <c r="B16" s="64"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="20"/>
+      <c r="N16" s="45"/>
       <c r="O16" s="12"/>
       <c r="P16" s="13"/>
     </row>
@@ -2259,28 +2326,25 @@
       <c r="C17" s="4">
         <v>3</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="88">
         <v>4</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="90">
         <v>5</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="90"/>
+      <c r="G17" s="2">
         <v>6</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="4">
         <v>7</v>
       </c>
-      <c r="H17" s="50">
+      <c r="I17" s="47">
         <v>8</v>
       </c>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
+      <c r="J17" s="46"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
       <c r="P17" s="14"/>
     </row>
     <row r="18" spans="1:26" ht="49.5" hidden="1" customHeight="1">
@@ -2296,262 +2360,270 @@
       <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="52" t="s">
+      <c r="J18" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="J18" s="52" t="s">
+      <c r="K18" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="K18" s="52" t="s">
+      <c r="L18" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="L18" s="52" t="s">
+      <c r="M18" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="M18" s="52" t="s">
+      <c r="N18" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="N18" s="52" t="s">
+      <c r="O18" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="O18" s="52" t="s">
+      <c r="P18" s="49" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.5">
       <c r="A19" s="2"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="5">
-        <f>ROUND(E19*F19,2)</f>
+      <c r="B19" s="96"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="95">
+        <v>100000</v>
+      </c>
+      <c r="F19" s="103">
+        <v>46012</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="5">
+        <f>ROUND(E19*G19,2)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="51"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="95"/>
-      <c r="N19" s="94"/>
-      <c r="O19" s="53"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="50"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="82" t="s">
+      <c r="A20" s="88"/>
+      <c r="B20" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="4"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="2"/>
       <c r="H20" s="7"/>
-      <c r="I20" s="16"/>
+      <c r="I20" s="7"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="52"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
     </row>
     <row r="21" spans="1:26" ht="15" customHeight="1">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="21"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="20"/>
       <c r="Q21" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
       <c r="Q23" s="11"/>
     </row>
     <row r="24" spans="1:26" ht="18.5" thickBot="1">
-      <c r="A24" s="71"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="25"/>
+      <c r="A24" s="86"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="24"/>
       <c r="Q24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="18">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74" t="s">
+      <c r="C25" s="52"/>
+      <c r="D25" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74" t="s">
+      <c r="E25" s="52"/>
+      <c r="F25" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="68" t="s">
+      <c r="G25" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="25"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="24"/>
       <c r="Q25" s="8"/>
     </row>
     <row r="26" spans="1:26" ht="18">
-      <c r="A26" s="73"/>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="25"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="24"/>
       <c r="Q26" s="8"/>
     </row>
     <row r="27" spans="1:26" ht="18">
-      <c r="A27" s="73"/>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="25"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="24"/>
       <c r="Q27" s="8"/>
     </row>
     <row r="28" spans="1:26" ht="18">
-      <c r="A28" s="73"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="23"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="22"/>
       <c r="Q28" s="8"/>
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
-      <c r="A29" s="40"/>
-      <c r="B29" s="91" t="s">
+      <c r="A29" s="37"/>
+      <c r="B29" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="92"/>
-      <c r="D29" s="93"/>
-      <c r="E29" s="92"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
       <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
-      <c r="A30" s="42"/>
-      <c r="B30" s="85"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
@@ -2564,22 +2636,22 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A31" s="42"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
@@ -2592,27 +2664,27 @@
       <c r="Z31" s="8"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A32" s="44"/>
-      <c r="B32" s="88" t="s">
+      <c r="A32" s="41"/>
+      <c r="B32" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="89"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="46">
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43">
         <f>SUM(G29:G31)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
@@ -2625,22 +2697,22 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
-      <c r="A33" s="17"/>
-      <c r="B33" s="34"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="12"/>
-      <c r="D33" s="35"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
@@ -2653,22 +2725,22 @@
       <c r="Z33" s="8"/>
     </row>
     <row r="34" spans="1:26" ht="18">
-      <c r="A34" s="24"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="Q34" s="22"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="Q34" s="21"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
@@ -2679,25 +2751,25 @@
       <c r="Y34" s="8"/>
       <c r="Z34" s="8"/>
     </row>
-    <row r="35" spans="1:26" ht="18">
-      <c r="A35" s="57" t="s">
+    <row r="35" spans="1:26" ht="18" customHeight="1">
+      <c r="A35" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="57"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="57"/>
-      <c r="N35" s="57"/>
-      <c r="O35" s="57"/>
-      <c r="P35" s="22"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="85"/>
+      <c r="J35" s="85"/>
+      <c r="K35" s="85"/>
+      <c r="L35" s="85"/>
+      <c r="M35" s="85"/>
+      <c r="N35" s="85"/>
+      <c r="O35" s="85"/>
+      <c r="P35" s="85"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
@@ -2710,22 +2782,22 @@
       <c r="Z35" s="8"/>
     </row>
     <row r="36" spans="1:26" ht="15.5" customHeight="1">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
       <c r="Q36" s="11"/>
       <c r="R36" s="11"/>
       <c r="S36" s="8"/>
@@ -2738,54 +2810,52 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37" spans="1:26" ht="18" customHeight="1">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57" t="s">
+      <c r="B37" s="54"/>
+      <c r="C37" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="33"/>
-      <c r="L37" s="57" t="s">
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="32"/>
+      <c r="M37" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="M37" s="57"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="57"/>
-      <c r="P37" s="25"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="54"/>
+      <c r="P37" s="54"/>
       <c r="Q37" s="11"/>
       <c r="R37" s="11"/>
       <c r="S37" s="8"/>
       <c r="Z37" s="8"/>
     </row>
     <row r="38" spans="1:26" ht="18" customHeight="1">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57" t="s">
+      <c r="B38" s="54"/>
+      <c r="C38" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="33"/>
-      <c r="L38" s="57" t="s">
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="32"/>
+      <c r="M38" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="M38" s="57"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="25"/>
+      <c r="N38" s="54"/>
+      <c r="O38" s="54"/>
+      <c r="P38" s="54"/>
       <c r="Q38" s="11"/>
       <c r="R38" s="11"/>
       <c r="S38" s="11"/>
@@ -2793,24 +2863,23 @@
     </row>
     <row r="39" spans="1:26" ht="18" customHeight="1">
       <c r="A39" s="11"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="54" t="s">
+      <c r="B39" s="26"/>
+      <c r="C39" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="33"/>
-      <c r="L39" s="54" t="s">
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="M39" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="M39" s="54"/>
-      <c r="N39" s="54"/>
-      <c r="O39" s="54"/>
-      <c r="P39" s="33"/>
+      <c r="N39" s="55"/>
+      <c r="O39" s="55"/>
+      <c r="P39" s="55"/>
       <c r="Q39" s="11"/>
       <c r="R39" s="11"/>
       <c r="S39" s="11"/>
@@ -2818,45 +2887,44 @@
     </row>
     <row r="40" spans="1:26" ht="18" customHeight="1">
       <c r="A40" s="11"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="54" t="s">
+      <c r="B40" s="26"/>
+      <c r="C40" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="L40" s="54" t="s">
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="M40" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="M40" s="54"/>
-      <c r="N40" s="54"/>
-      <c r="O40" s="54"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="28"/>
-      <c r="S40" s="28"/>
-      <c r="Z40" s="28"/>
+      <c r="N40" s="55"/>
+      <c r="O40" s="55"/>
+      <c r="P40" s="55"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
+      <c r="Z40" s="27"/>
     </row>
     <row r="41" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A41" s="29"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
+      <c r="A41" s="28"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
       <c r="P41" s="11"/>
       <c r="Q41" s="11"/>
       <c r="R41" s="11"/>
@@ -2875,16 +2943,16 @@
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="33"/>
-      <c r="L42" s="33"/>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
-      <c r="O42" s="33"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="32"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="32"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="11"/>
       <c r="R42" s="11"/>
@@ -28592,23 +28660,30 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="47">
-    <mergeCell ref="F25:F28"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
+  <mergeCells count="48">
+    <mergeCell ref="M39:P39"/>
+    <mergeCell ref="M40:P40"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="M37:P37"/>
+    <mergeCell ref="M38:P38"/>
+    <mergeCell ref="A11:P11"/>
+    <mergeCell ref="A12:P12"/>
+    <mergeCell ref="A13:P13"/>
+    <mergeCell ref="A14:P14"/>
+    <mergeCell ref="A35:P35"/>
+    <mergeCell ref="L6:P6"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C15:C16"/>
     <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G25:G28"/>
+    <mergeCell ref="A23:G24"/>
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="B25:C28"/>
     <mergeCell ref="D25:E28"/>
@@ -28616,30 +28691,24 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="K6:O6"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
     <mergeCell ref="H15:H16"/>
-    <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A13:O13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A35:O35"/>
-    <mergeCell ref="G25:G28"/>
-    <mergeCell ref="A23:G24"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="L40:O40"/>
-    <mergeCell ref="K7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="K9:O9"/>
-    <mergeCell ref="L37:O37"/>
-    <mergeCell ref="L38:O38"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Introduce ProductSelectionViewModel to avoid code duplication
</commit_message>
<xml_diff>
--- a/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
+++ b/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Domain\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBDEE02-69B7-4088-B884-54277530777D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A209D6-5720-420E-8081-55618A6A50F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -868,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1007,52 +1007,98 @@
     <xf numFmtId="165" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1071,71 +1117,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1147,10 +1129,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1158,107 +1155,6 @@
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ _₽"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1544,6 +1440,107 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ _₽"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color rgb="FF000000"/>
@@ -1705,20 +1702,20 @@
     <tableColumn id="2" xr3:uid="{7F02335C-6B7B-481B-AA66-A99D53295D48}" name="Стовпець2" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{AC958478-2380-4462-ADB7-810E91AE2702}" name="Стовпець3" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{4D8DF304-E376-491E-9F7D-7A03F13DBB99}" name="Стовпець4" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{5D79FBC9-1D68-44B0-BD0A-A2F59263FD62}" name="Стовпець5" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{0F061852-471E-46A7-9A27-17017CF4C250}" name="Стовпець52" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{64873108-ECB2-491F-96B4-07CE2637EE51}" name="Стовпець6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{28BA7FB3-3224-4141-BA1B-28B92F3BBD84}" name="Стовпець7" dataDxfId="11">
+    <tableColumn id="5" xr3:uid="{5D79FBC9-1D68-44B0-BD0A-A2F59263FD62}" name="Стовпець5" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{0F061852-471E-46A7-9A27-17017CF4C250}" name="Стовпець52" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{64873108-ECB2-491F-96B4-07CE2637EE51}" name="Стовпець6" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{28BA7FB3-3224-4141-BA1B-28B92F3BBD84}" name="Стовпець7" dataDxfId="8">
       <calculatedColumnFormula>ROUND(E19*G19,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{367C3413-BF3B-423C-A04A-2814E50C87E1}" name="Стовпець8" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{202BCDE3-5F48-4FA4-8C3F-A34C56881D6E}" name="Стовпець9" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{17574747-EE2A-4B01-BB04-855077C0E1EA}" name="Стовпець10" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{12AAD393-3012-4400-B19F-F964366D98C7}" name="Стовпець11" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{0107D3B1-D8D8-43D9-9D6F-679BD5947952}" name="Стовпець12" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{CE8D7C7C-C1EF-43A1-A678-379081133252}" name="Стовпець13" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{9ED438C1-E185-4C3B-A31F-A751FC28DDF0}" name="Стовпець14" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{E843A11C-28C0-4349-9D21-39647F8044A0}" name="Стовпець15" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{367C3413-BF3B-423C-A04A-2814E50C87E1}" name="Стовпець8" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{202BCDE3-5F48-4FA4-8C3F-A34C56881D6E}" name="Стовпець9" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{17574747-EE2A-4B01-BB04-855077C0E1EA}" name="Стовпець10" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{12AAD393-3012-4400-B19F-F964366D98C7}" name="Стовпець11" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{0107D3B1-D8D8-43D9-9D6F-679BD5947952}" name="Стовпець12" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{CE8D7C7C-C1EF-43A1-A678-379081133252}" name="Стовпець13" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{9ED438C1-E185-4C3B-A31F-A751FC28DDF0}" name="Стовпець14" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{E843A11C-28C0-4349-9D21-39647F8044A0}" name="Стовпець15" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1928,7 +1925,7 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="69" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2008,10 +2005,10 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="71"/>
+      <c r="B3" s="85"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2038,14 +2035,14 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="74" t="s">
+      <c r="B4" s="85"/>
+      <c r="C4" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="75"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="44"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -2097,20 +2094,20 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" spans="1:26" ht="18" customHeight="1">
-      <c r="A6" s="73"/>
-      <c r="B6" s="71"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="L6" s="76" t="s">
+      <c r="L6" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
       <c r="Q6" s="26"/>
     </row>
     <row r="7" spans="1:26" ht="18" customHeight="1">
@@ -2119,13 +2116,13 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
-      <c r="L7" s="76" t="s">
+      <c r="L7" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="76"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="60"/>
       <c r="Q7" s="26"/>
     </row>
     <row r="8" spans="1:26" ht="18" customHeight="1">
@@ -2134,15 +2131,15 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="L8" s="77" t="s">
+      <c r="L8" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="87" t="s">
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="87"/>
+      <c r="P8" s="61"/>
       <c r="Q8" s="11"/>
     </row>
     <row r="9" spans="1:26" ht="24.75" customHeight="1">
@@ -2151,13 +2148,13 @@
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="L9" s="76" t="s">
+      <c r="L9" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
       <c r="Q9" s="26"/>
     </row>
     <row r="10" spans="1:26" ht="18" customHeight="1">
@@ -2178,24 +2175,24 @@
       <c r="Z10" s="11"/>
     </row>
     <row r="11" spans="1:26" ht="18" customHeight="1">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="56"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
@@ -2208,92 +2205,92 @@
       <c r="Z11" s="11"/>
     </row>
     <row r="12" spans="1:26" ht="18" customHeight="1">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="80"/>
-      <c r="P12" s="80"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
       <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="1:26" ht="18" customHeight="1">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="81"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="81"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="65"/>
+      <c r="P13" s="65"/>
       <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="1:26" ht="18" customHeight="1">
-      <c r="A14" s="102" t="s">
+      <c r="A14" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="102"/>
-      <c r="C14" s="102"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="102"/>
-      <c r="L14" s="102"/>
-      <c r="M14" s="102"/>
-      <c r="N14" s="102"/>
-      <c r="O14" s="102"/>
-      <c r="P14" s="102"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:26" ht="81.75" customHeight="1">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="93" t="s">
+      <c r="D15" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="53"/>
-      <c r="G15" s="94" t="s">
+      <c r="F15" s="83"/>
+      <c r="G15" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="63" t="s">
+      <c r="H15" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="78" t="s">
+      <c r="I15" s="68" t="s">
         <v>8</v>
       </c>
       <c r="J15" s="45"/>
@@ -2302,15 +2299,15 @@
       <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="24" customHeight="1">
-      <c r="A16" s="82"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="79"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="69"/>
       <c r="J16" s="20"/>
       <c r="N16" s="45"/>
       <c r="O16" s="12"/>
@@ -2326,7 +2323,7 @@
       <c r="C17" s="4">
         <v>3</v>
       </c>
-      <c r="D17" s="88">
+      <c r="D17" s="52">
         <v>4</v>
       </c>
       <c r="E17" s="90">
@@ -2360,10 +2357,10 @@
       <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="89" t="s">
+      <c r="E18" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="89" t="s">
+      <c r="F18" s="53" t="s">
         <v>55</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -2399,13 +2396,13 @@
     </row>
     <row r="19" spans="1:26" ht="15.5">
       <c r="A19" s="2"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="95">
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="54">
         <v>100000</v>
       </c>
-      <c r="F19" s="103">
+      <c r="F19" s="58">
         <v>46012</v>
       </c>
       <c r="G19" s="4"/>
@@ -2423,14 +2420,14 @@
       <c r="P19" s="50"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A20" s="88"/>
-      <c r="B20" s="99" t="s">
+      <c r="A20" s="52"/>
+      <c r="B20" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="101"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="93"/>
       <c r="G20" s="2"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -2461,15 +2458,15 @@
       <c r="Q21" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A23" s="85" t="s">
+      <c r="A23" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="85"/>
-      <c r="C23" s="85"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
@@ -2482,13 +2479,13 @@
       <c r="Q23" s="11"/>
     </row>
     <row r="24" spans="1:26" ht="18.5" thickBot="1">
-      <c r="A24" s="86"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
+      <c r="A24" s="79"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
       <c r="J24" s="21"/>
@@ -2501,21 +2498,21 @@
       <c r="Q24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="18">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52" t="s">
+      <c r="C25" s="82"/>
+      <c r="D25" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52" t="s">
+      <c r="E25" s="82"/>
+      <c r="F25" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="83" t="s">
+      <c r="G25" s="77" t="s">
         <v>14</v>
       </c>
       <c r="H25" s="21"/>
@@ -2530,13 +2527,13 @@
       <c r="Q25" s="8"/>
     </row>
     <row r="26" spans="1:26" ht="18">
-      <c r="A26" s="69"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="84"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="78"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
@@ -2549,13 +2546,13 @@
       <c r="Q26" s="8"/>
     </row>
     <row r="27" spans="1:26" ht="18">
-      <c r="A27" s="69"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="84"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="83"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="78"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
@@ -2568,13 +2565,13 @@
       <c r="Q27" s="8"/>
     </row>
     <row r="28" spans="1:26" ht="18">
-      <c r="A28" s="69"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="84"/>
+      <c r="A28" s="81"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="78"/>
       <c r="H28" s="22"/>
       <c r="I28" s="24"/>
       <c r="J28" s="24"/>
@@ -2588,12 +2585,12 @@
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
       <c r="A29" s="37"/>
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="66"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="66"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="101"/>
       <c r="F29" s="36"/>
       <c r="G29" s="38"/>
       <c r="H29" s="22"/>
@@ -2609,10 +2606,10 @@
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
       <c r="A30" s="39"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="58"/>
+      <c r="B30" s="94"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="95"/>
       <c r="F30" s="25"/>
       <c r="G30" s="40"/>
       <c r="H30" s="22"/>
@@ -2637,10 +2634,10 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="39"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="58"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="95"/>
       <c r="F31" s="25"/>
       <c r="G31" s="40"/>
       <c r="H31" s="22"/>
@@ -2665,12 +2662,12 @@
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A32" s="41"/>
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="61"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="99"/>
+      <c r="E32" s="98"/>
       <c r="F32" s="42"/>
       <c r="G32" s="43">
         <f>SUM(G29:G31)</f>
@@ -2751,25 +2748,25 @@
       <c r="Y34" s="8"/>
       <c r="Z34" s="8"/>
     </row>
-    <row r="35" spans="1:26" ht="18" customHeight="1">
-      <c r="A35" s="85" t="s">
+    <row r="35" spans="1:26" ht="39" customHeight="1">
+      <c r="A35" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="85"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="85"/>
-      <c r="I35" s="85"/>
-      <c r="J35" s="85"/>
-      <c r="K35" s="85"/>
-      <c r="L35" s="85"/>
-      <c r="M35" s="85"/>
-      <c r="N35" s="85"/>
-      <c r="O35" s="85"/>
-      <c r="P35" s="85"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="62"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="62"/>
+      <c r="N35" s="62"/>
+      <c r="O35" s="62"/>
+      <c r="P35" s="62"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
@@ -2810,52 +2807,52 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37" spans="1:26" ht="18" customHeight="1">
-      <c r="A37" s="54" t="s">
+      <c r="A37" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="54"/>
-      <c r="C37" s="54" t="s">
+      <c r="B37" s="62"/>
+      <c r="C37" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="I37" s="21"/>
       <c r="J37" s="32"/>
-      <c r="M37" s="54" t="s">
+      <c r="M37" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="N37" s="54"/>
-      <c r="O37" s="54"/>
-      <c r="P37" s="54"/>
+      <c r="N37" s="62"/>
+      <c r="O37" s="62"/>
+      <c r="P37" s="62"/>
       <c r="Q37" s="11"/>
       <c r="R37" s="11"/>
       <c r="S37" s="8"/>
       <c r="Z37" s="8"/>
     </row>
     <row r="38" spans="1:26" ht="18" customHeight="1">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54" t="s">
+      <c r="B38" s="62"/>
+      <c r="C38" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="21"/>
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="I38" s="21"/>
       <c r="J38" s="32"/>
-      <c r="M38" s="54" t="s">
+      <c r="M38" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="N38" s="54"/>
-      <c r="O38" s="54"/>
-      <c r="P38" s="54"/>
+      <c r="N38" s="62"/>
+      <c r="O38" s="62"/>
+      <c r="P38" s="62"/>
       <c r="Q38" s="11"/>
       <c r="R38" s="11"/>
       <c r="S38" s="11"/>
@@ -2864,22 +2861,22 @@
     <row r="39" spans="1:26" ht="18" customHeight="1">
       <c r="A39" s="11"/>
       <c r="B39" s="26"/>
-      <c r="C39" s="55" t="s">
+      <c r="C39" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
       <c r="F39" s="32"/>
       <c r="G39" s="32"/>
       <c r="H39" s="32"/>
       <c r="I39" s="32"/>
       <c r="J39" s="32"/>
-      <c r="M39" s="55" t="s">
+      <c r="M39" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="N39" s="55"/>
-      <c r="O39" s="55"/>
-      <c r="P39" s="55"/>
+      <c r="N39" s="59"/>
+      <c r="O39" s="59"/>
+      <c r="P39" s="59"/>
       <c r="Q39" s="11"/>
       <c r="R39" s="11"/>
       <c r="S39" s="11"/>
@@ -2888,22 +2885,22 @@
     <row r="40" spans="1:26" ht="18" customHeight="1">
       <c r="A40" s="11"/>
       <c r="B40" s="26"/>
-      <c r="C40" s="55" t="s">
+      <c r="C40" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="55"/>
-      <c r="E40" s="55"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
       <c r="F40" s="32"/>
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="32"/>
       <c r="J40" s="32"/>
-      <c r="M40" s="55" t="s">
+      <c r="M40" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="N40" s="55"/>
-      <c r="O40" s="55"/>
-      <c r="P40" s="55"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="59"/>
+      <c r="P40" s="59"/>
       <c r="Q40" s="27"/>
       <c r="R40" s="27"/>
       <c r="S40" s="27"/>
@@ -28661,18 +28658,22 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="48">
-    <mergeCell ref="M39:P39"/>
-    <mergeCell ref="M40:P40"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="M37:P37"/>
-    <mergeCell ref="M38:P38"/>
-    <mergeCell ref="A11:P11"/>
-    <mergeCell ref="A12:P12"/>
-    <mergeCell ref="A13:P13"/>
-    <mergeCell ref="A14:P14"/>
-    <mergeCell ref="A35:P35"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E15:F16"/>
     <mergeCell ref="L6:P6"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="L8:N8"/>
@@ -28687,28 +28688,24 @@
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="B25:C28"/>
     <mergeCell ref="D25:E28"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E15:F16"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="F25:F28"/>
+    <mergeCell ref="M39:P39"/>
+    <mergeCell ref="M40:P40"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="M37:P37"/>
+    <mergeCell ref="M38:P38"/>
+    <mergeCell ref="A11:P11"/>
+    <mergeCell ref="A12:P12"/>
+    <mergeCell ref="A13:P13"/>
+    <mergeCell ref="A14:P14"/>
+    <mergeCell ref="A35:P35"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Fix Residual Value Report inconsistencies
</commit_message>
<xml_diff>
--- a/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
+++ b/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Domain\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C18E57-CA35-4257-B44B-DF28E182BC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F98286-E374-4198-8D98-39E9ADEB042B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,29 +141,6 @@
         <family val="1"/>
       </rPr>
       <t>і</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Первісна вартість (графа 5 х  графу 6)      (В</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>п</t>
     </r>
     <r>
       <rPr>
@@ -323,6 +300,9 @@
   </si>
   <si>
     <t>[ASSEMBLY_YEAR] року виготовлення станом на [REPORT_DATE] року</t>
+  </si>
+  <si>
+    <t>Первісна вартість (графа 5 х  графу 6)                     (Вп)</t>
   </si>
 </sst>
 </file>
@@ -1108,6 +1088,36 @@
     <xf numFmtId="4" fontId="16" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1116,6 +1126,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1154,12 +1170,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1191,188 +1201,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ _₽"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1657,6 +1490,153 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ _₽"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -1721,22 +1701,22 @@
   <autoFilter ref="A18:O19" xr:uid="{48DE2C05-180A-4702-9C30-1CFABF4F8FAC}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{66111BEB-9378-4A74-A18F-4AF1F7610B8A}" name="Стовпець1" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{7F02335C-6B7B-481B-AA66-A99D53295D48}" name="Стовпець2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{AC958478-2380-4462-ADB7-810E91AE2702}" name="Стовпець3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{4D8DF304-E376-491E-9F7D-7A03F13DBB99}" name="Стовпець4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{5D79FBC9-1D68-44B0-BD0A-A2F59263FD62}" name="Стовпець5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{64873108-ECB2-491F-96B4-07CE2637EE51}" name="Стовпець6" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{28BA7FB3-3224-4141-BA1B-28B92F3BBD84}" name="Стовпець7" dataDxfId="13">
+    <tableColumn id="2" xr3:uid="{7F02335C-6B7B-481B-AA66-A99D53295D48}" name="Стовпець2" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{AC958478-2380-4462-ADB7-810E91AE2702}" name="Стовпець3" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{4D8DF304-E376-491E-9F7D-7A03F13DBB99}" name="Стовпець4" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{5D79FBC9-1D68-44B0-BD0A-A2F59263FD62}" name="Стовпець5" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{64873108-ECB2-491F-96B4-07CE2637EE51}" name="Стовпець6" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{28BA7FB3-3224-4141-BA1B-28B92F3BBD84}" name="Стовпець7" dataDxfId="8">
       <calculatedColumnFormula>ROUND(E19*F19,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{367C3413-BF3B-423C-A04A-2814E50C87E1}" name="Стовпець8" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{202BCDE3-5F48-4FA4-8C3F-A34C56881D6E}" name="Стовпець9" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{17574747-EE2A-4B01-BB04-855077C0E1EA}" name="Стовпець10" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{12AAD393-3012-4400-B19F-F964366D98C7}" name="Стовпець11" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{0107D3B1-D8D8-43D9-9D6F-679BD5947952}" name="Стовпець12" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{CE8D7C7C-C1EF-43A1-A678-379081133252}" name="Стовпець13" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{9ED438C1-E185-4C3B-A31F-A751FC28DDF0}" name="Стовпець14" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{E843A11C-28C0-4349-9D21-39647F8044A0}" name="Стовпець15" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{367C3413-BF3B-423C-A04A-2814E50C87E1}" name="Стовпець8" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{202BCDE3-5F48-4FA4-8C3F-A34C56881D6E}" name="Стовпець9" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{17574747-EE2A-4B01-BB04-855077C0E1EA}" name="Стовпець10" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{12AAD393-3012-4400-B19F-F964366D98C7}" name="Стовпець11" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{0107D3B1-D8D8-43D9-9D6F-679BD5947952}" name="Стовпець12" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{CE8D7C7C-C1EF-43A1-A678-379081133252}" name="Стовпець13" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{9ED438C1-E185-4C3B-A31F-A751FC28DDF0}" name="Стовпець14" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{E843A11C-28C0-4349-9D21-39647F8044A0}" name="Стовпець15" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1945,14 +1925,14 @@
   </sheetPr>
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="69" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.54296875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="6" customWidth="1"/>
     <col min="3" max="3" width="8.6328125" style="6" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" style="6" customWidth="1"/>
     <col min="5" max="5" width="24.36328125" style="6" customWidth="1"/>
@@ -2024,10 +2004,10 @@
       <c r="Y2" s="5"/>
     </row>
     <row r="3" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A3" s="83" t="s">
-        <v>25</v>
+      <c r="A3" s="93" t="s">
+        <v>24</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="94"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2053,14 +2033,14 @@
       <c r="Y3" s="5"/>
     </row>
     <row r="4" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="87" t="s">
-        <v>37</v>
+      <c r="B4" s="94"/>
+      <c r="C4" s="97" t="s">
+        <v>36</v>
       </c>
-      <c r="D4" s="88"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="27"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -2111,19 +2091,19 @@
       <c r="Y5" s="5"/>
     </row>
     <row r="6" spans="1:25" ht="18" customHeight="1">
-      <c r="A6" s="86"/>
-      <c r="B6" s="84"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="K6" s="82" t="s">
+      <c r="K6" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="92"/>
+      <c r="O6" s="92"/>
       <c r="P6" s="20"/>
     </row>
     <row r="7" spans="1:25" ht="18" customHeight="1">
@@ -2132,13 +2112,13 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="K7" s="82" t="s">
-        <v>26</v>
+      <c r="K7" s="92" t="s">
+        <v>25</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="92"/>
+      <c r="O7" s="92"/>
       <c r="P7" s="20"/>
     </row>
     <row r="8" spans="1:25" ht="18" customHeight="1">
@@ -2147,15 +2127,15 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="K8" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="81" t="s">
+      <c r="K8" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="O8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="91"/>
       <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:25" ht="24.75" customHeight="1">
@@ -2164,13 +2144,13 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="K9" s="82" t="s">
+      <c r="K9" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="92"/>
+      <c r="O9" s="92"/>
       <c r="P9" s="20"/>
     </row>
     <row r="10" spans="1:25" ht="18" customHeight="1">
@@ -2191,23 +2171,23 @@
       <c r="Y10" s="8"/>
     </row>
     <row r="11" spans="1:25" ht="18" customHeight="1">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="91"/>
-      <c r="D11" s="91"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="91"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="91"/>
-      <c r="I11" s="91"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="91"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="91"/>
-      <c r="N11" s="91"/>
-      <c r="O11" s="91"/>
+      <c r="B11" s="101"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="101"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="101"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="101"/>
+      <c r="J11" s="101"/>
+      <c r="K11" s="101"/>
+      <c r="L11" s="101"/>
+      <c r="M11" s="101"/>
+      <c r="N11" s="101"/>
+      <c r="O11" s="101"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -2220,86 +2200,86 @@
       <c r="Y11" s="8"/>
     </row>
     <row r="12" spans="1:25" ht="18" customHeight="1">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="100" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="100"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="100"/>
+      <c r="O12" s="100"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" spans="1:25" s="37" customFormat="1" ht="18" customHeight="1">
+      <c r="A13" s="100" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="100"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="100"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" spans="1:25" ht="18" customHeight="1">
+      <c r="A14" s="101"/>
+      <c r="B14" s="101"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="101"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="101"/>
+      <c r="N14" s="101"/>
+      <c r="O14" s="101"/>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" spans="1:25" ht="68" customHeight="1">
+      <c r="A15" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="87" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="90"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" spans="1:25" s="37" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="90" t="s">
+      <c r="F15" s="89" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:25" ht="18" customHeight="1">
-      <c r="A14" s="91"/>
-      <c r="B14" s="91"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
-      <c r="L14" s="91"/>
-      <c r="M14" s="91"/>
-      <c r="N14" s="91"/>
-      <c r="O14" s="91"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="1:25" ht="81.75" customHeight="1">
-      <c r="A15" s="72" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="72" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="72" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="75" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="89" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="77" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="72" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="70" t="s">
+      <c r="H15" s="82" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="28"/>
@@ -2308,14 +2288,14 @@
       <c r="O15" s="10"/>
     </row>
     <row r="16" spans="1:25" ht="24" customHeight="1">
-      <c r="A16" s="73"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="71"/>
+      <c r="A16" s="85"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="99"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="83"/>
       <c r="I16" s="16"/>
       <c r="M16" s="28"/>
       <c r="N16" s="9"/>
@@ -2355,16 +2335,16 @@
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="94" t="s">
+      <c r="B18" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="95" t="s">
+      <c r="C18" s="66" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="96" t="s">
+      <c r="E18" s="67" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="36" t="s">
@@ -2377,37 +2357,37 @@
         <v>21</v>
       </c>
       <c r="I18" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="32" t="s">
+      <c r="K18" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="L18" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="L18" s="32" t="s">
+      <c r="M18" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="M18" s="32" t="s">
+      <c r="N18" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="N18" s="32" t="s">
+      <c r="O18" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="O18" s="32" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="19" spans="1:25" ht="15.5">
-      <c r="A19" s="92"/>
-      <c r="B19" s="97"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="100">
+      <c r="A19" s="63"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="71">
         <v>100000</v>
       </c>
-      <c r="F19" s="101"/>
-      <c r="G19" s="93">
+      <c r="F19" s="72"/>
+      <c r="G19" s="64">
         <f>ROUND(E19*F19,2)</f>
         <v>0</v>
       </c>
@@ -2439,14 +2419,14 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:25" s="37" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="63" t="s">
-        <v>65</v>
+      <c r="A21" s="73" t="s">
+        <v>64</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
       <c r="G21" s="12"/>
       <c r="H21" s="15"/>
       <c r="I21" s="13"/>
@@ -2459,14 +2439,14 @@
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:25" ht="18.5" thickBot="1">
-      <c r="A22" s="79" t="s">
-        <v>57</v>
+      <c r="A22" s="76" t="s">
+        <v>56</v>
       </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
       <c r="G22" s="53"/>
       <c r="H22" s="53"/>
       <c r="I22" s="53"/>
@@ -2485,10 +2465,10 @@
         <v>10</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="39" t="s">
         <v>11</v>
@@ -2497,24 +2477,24 @@
         <v>12</v>
       </c>
       <c r="G23" s="56"/>
-      <c r="H23" s="67" t="s">
-        <v>71</v>
+      <c r="H23" s="79" t="s">
+        <v>70</v>
       </c>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="67"/>
-      <c r="N23" s="67"/>
-      <c r="O23" s="67"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="79"/>
       <c r="P23" s="8"/>
     </row>
     <row r="24" spans="1:25" ht="15.5" customHeight="1">
       <c r="A24" s="57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="43"/>
       <c r="D24" s="44">
@@ -2529,24 +2509,24 @@
         <v>0</v>
       </c>
       <c r="G24" s="56"/>
-      <c r="H24" s="68" t="s">
-        <v>70</v>
+      <c r="H24" s="80" t="s">
+        <v>69</v>
       </c>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="68"/>
-      <c r="O24" s="68"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:25" ht="18" customHeight="1">
       <c r="A25" s="57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="43"/>
       <c r="D25" s="44">
@@ -2561,22 +2541,22 @@
         <v>0</v>
       </c>
       <c r="G25" s="56"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="68"/>
-      <c r="L25" s="68"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="68"/>
-      <c r="O25" s="68"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="80"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="80"/>
+      <c r="O25" s="80"/>
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:25" ht="15.5" customHeight="1">
       <c r="A26" s="57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="43"/>
       <c r="D26" s="44">
@@ -2591,22 +2571,22 @@
         <v>0</v>
       </c>
       <c r="G26" s="56"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
-      <c r="M26" s="68"/>
-      <c r="N26" s="68"/>
-      <c r="O26" s="68"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="80"/>
+      <c r="K26" s="80"/>
+      <c r="L26" s="80"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="80"/>
+      <c r="O26" s="80"/>
       <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:25" ht="15.5" customHeight="1">
       <c r="A27" s="57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="43"/>
       <c r="D27" s="44">
@@ -2621,22 +2601,22 @@
         <v>0</v>
       </c>
       <c r="G27" s="56"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="68"/>
-      <c r="N27" s="68"/>
-      <c r="O27" s="68"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="80"/>
+      <c r="K27" s="80"/>
+      <c r="L27" s="80"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="80"/>
+      <c r="O27" s="80"/>
       <c r="P27" s="5"/>
     </row>
     <row r="28" spans="1:25" ht="15.5" customHeight="1">
       <c r="A28" s="57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="44">
@@ -2651,22 +2631,22 @@
         <v>0</v>
       </c>
       <c r="G28" s="56"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="68"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="68"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="80"/>
+      <c r="M28" s="80"/>
+      <c r="N28" s="80"/>
+      <c r="O28" s="80"/>
       <c r="P28" s="5"/>
     </row>
     <row r="29" spans="1:25" ht="15" customHeight="1">
       <c r="A29" s="58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="47"/>
       <c r="D29" s="44">
@@ -2693,10 +2673,10 @@
     </row>
     <row r="30" spans="1:25" ht="15" customHeight="1">
       <c r="A30" s="58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="44">
@@ -2790,23 +2770,23 @@
       <c r="Y32" s="5"/>
     </row>
     <row r="33" spans="1:25" ht="18">
-      <c r="A33" s="64" t="s">
-        <v>69</v>
+      <c r="A33" s="74" t="s">
+        <v>68</v>
       </c>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="64"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="74"/>
+      <c r="O33" s="74"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
@@ -2819,18 +2799,18 @@
       <c r="Y33" s="5"/>
     </row>
     <row r="34" spans="1:25" ht="18" customHeight="1">
-      <c r="A34" s="65" t="s">
-        <v>66</v>
+      <c r="A34" s="75" t="s">
+        <v>65</v>
       </c>
-      <c r="B34" s="65"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
       <c r="F34" s="61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
@@ -2879,50 +2859,50 @@
       <c r="Y35" s="5"/>
     </row>
     <row r="36" spans="1:25" ht="18" customHeight="1">
-      <c r="A36" s="65" t="s">
-        <v>45</v>
+      <c r="A36" s="75" t="s">
+        <v>44</v>
       </c>
-      <c r="B36" s="65"/>
-      <c r="C36" s="65" t="s">
-        <v>30</v>
+      <c r="B36" s="75"/>
+      <c r="C36" s="75" t="s">
+        <v>29</v>
       </c>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
       <c r="I36" s="23"/>
-      <c r="L36" s="65" t="s">
-        <v>29</v>
+      <c r="L36" s="75" t="s">
+        <v>28</v>
       </c>
-      <c r="M36" s="65"/>
-      <c r="N36" s="65"/>
-      <c r="O36" s="65"/>
+      <c r="M36" s="75"/>
+      <c r="N36" s="75"/>
+      <c r="O36" s="75"/>
       <c r="P36" s="8"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="5"/>
       <c r="Y36" s="5"/>
     </row>
     <row r="37" spans="1:25" ht="18" customHeight="1">
-      <c r="A37" s="65" t="s">
-        <v>24</v>
+      <c r="A37" s="75" t="s">
+        <v>23</v>
       </c>
-      <c r="B37" s="65"/>
-      <c r="C37" s="65" t="s">
-        <v>31</v>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75" t="s">
+        <v>30</v>
       </c>
-      <c r="D37" s="65"/>
-      <c r="E37" s="65"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
       <c r="H37" s="17"/>
       <c r="I37" s="23"/>
-      <c r="L37" s="65" t="s">
-        <v>34</v>
+      <c r="L37" s="75" t="s">
+        <v>33</v>
       </c>
-      <c r="M37" s="65"/>
-      <c r="N37" s="65"/>
-      <c r="O37" s="65"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="75"/>
+      <c r="O37" s="75"/>
       <c r="P37" s="8"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
@@ -2931,21 +2911,21 @@
     <row r="38" spans="1:25" ht="18" customHeight="1">
       <c r="A38" s="8"/>
       <c r="B38" s="20"/>
-      <c r="C38" s="66" t="s">
-        <v>32</v>
+      <c r="C38" s="78" t="s">
+        <v>31</v>
       </c>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="78"/>
       <c r="F38" s="23"/>
       <c r="G38" s="23"/>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
-      <c r="L38" s="66" t="s">
-        <v>35</v>
+      <c r="L38" s="78" t="s">
+        <v>34</v>
       </c>
-      <c r="M38" s="66"/>
-      <c r="N38" s="66"/>
-      <c r="O38" s="66"/>
+      <c r="M38" s="78"/>
+      <c r="N38" s="78"/>
+      <c r="O38" s="78"/>
       <c r="P38" s="8"/>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
@@ -2954,21 +2934,21 @@
     <row r="39" spans="1:25" ht="18" customHeight="1">
       <c r="A39" s="8"/>
       <c r="B39" s="20"/>
-      <c r="C39" s="66" t="s">
-        <v>33</v>
+      <c r="C39" s="78" t="s">
+        <v>32</v>
       </c>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
-      <c r="L39" s="66" t="s">
-        <v>36</v>
+      <c r="L39" s="78" t="s">
+        <v>35</v>
       </c>
-      <c r="M39" s="66"/>
-      <c r="N39" s="66"/>
-      <c r="O39" s="66"/>
+      <c r="M39" s="78"/>
+      <c r="N39" s="78"/>
+      <c r="O39" s="78"/>
       <c r="P39" s="21"/>
       <c r="Q39" s="21"/>
       <c r="R39" s="21"/>
@@ -27875,7 +27855,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Make adjustments in the Report Configuration file. Separate Commissions from the Reports. Separate common Unit data as well. Fix the templates.
</commit_message>
<xml_diff>
--- a/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
+++ b/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Domain\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F98286-E374-4198-8D98-39E9ADEB042B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6848EC73-F779-4C55-BDB2-D44427A1000A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,42 +156,6 @@
     <t>Члени комісії:</t>
   </si>
   <si>
-    <t>військова частина [MILITARY_UNIT]</t>
-  </si>
-  <si>
-    <t>Командир військової частини [MILITARY_UNIT]</t>
-  </si>
-  <si>
-    <t>[UNIT_COMMANDER]</t>
-  </si>
-  <si>
-    <t>[COMMANDER_RANK]</t>
-  </si>
-  <si>
-    <t>[COMMISION_HEAD_NAME]</t>
-  </si>
-  <si>
-    <t>[COMMISION_HEAD_RANK]</t>
-  </si>
-  <si>
-    <t>[COMMISION_PERSON1_RANK]</t>
-  </si>
-  <si>
-    <t>[COMMISION_PERSON2_RANK]</t>
-  </si>
-  <si>
-    <t>[COMMISION_PERSON3_RANK]</t>
-  </si>
-  <si>
-    <t>[COMMISION_PERSON1_NAME]</t>
-  </si>
-  <si>
-    <t>[COMMISION_PERSON2_NAME]</t>
-  </si>
-  <si>
-    <t>[COMMISION_PERSON3_NAME]</t>
-  </si>
-  <si>
     <t>[UNIT_EDRPOU]</t>
   </si>
   <si>
@@ -303,6 +267,43 @@
   </si>
   <si>
     <t>Первісна вартість (графа 5 х  графу 6)                     (Вп)</t>
+  </si>
+  <si>
+    <t>Тимчасово виконуючий обов'язки 
+командира військової частини [MIL_UNIT]</t>
+  </si>
+  <si>
+    <t>[COMM_RANK]</t>
+  </si>
+  <si>
+    <t>[UNIT_COMM]</t>
+  </si>
+  <si>
+    <t>військова частина [MIL_UNIT]</t>
+  </si>
+  <si>
+    <t>[COMMISSION_PERSON1_RANK]</t>
+  </si>
+  <si>
+    <t>[COMMISSION_HEAD_RANK]</t>
+  </si>
+  <si>
+    <t>[COMMISSION_PERSON2_RANK]</t>
+  </si>
+  <si>
+    <t>[COMMISSION_PERSON3_RANK]</t>
+  </si>
+  <si>
+    <t>[COMMISSION_HEAD_NAME]</t>
+  </si>
+  <si>
+    <t>[COMMISSION_PERSON1_NAME]</t>
+  </si>
+  <si>
+    <t>[COMMISSION_PERSON2_NAME]</t>
+  </si>
+  <si>
+    <t>[COMMISSION_PERSON3_NAME]</t>
   </si>
 </sst>
 </file>
@@ -1925,8 +1926,8 @@
   </sheetPr>
   <dimension ref="A1:Y1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="69" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2005,7 +2006,7 @@
     </row>
     <row r="3" spans="1:25" ht="12.75" customHeight="1">
       <c r="A3" s="93" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B3" s="94"/>
       <c r="C3" s="5"/>
@@ -2038,7 +2039,7 @@
       </c>
       <c r="B4" s="94"/>
       <c r="C4" s="97" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D4" s="98"/>
       <c r="E4" s="27"/>
@@ -2106,14 +2107,14 @@
       <c r="O6" s="92"/>
       <c r="P6" s="20"/>
     </row>
-    <row r="7" spans="1:25" ht="18" customHeight="1">
+    <row r="7" spans="1:25" ht="34" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="K7" s="92" t="s">
-        <v>25</v>
+      <c r="K7" s="75" t="s">
+        <v>61</v>
       </c>
       <c r="L7" s="92"/>
       <c r="M7" s="92"/>
@@ -2128,12 +2129,12 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="K8" s="81" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="L8" s="81"/>
       <c r="M8" s="81"/>
       <c r="N8" s="91" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="O8" s="91"/>
       <c r="P8" s="8"/>
@@ -2201,7 +2202,7 @@
     </row>
     <row r="12" spans="1:25" ht="18" customHeight="1">
       <c r="A12" s="100" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B12" s="100"/>
       <c r="C12" s="100"/>
@@ -2221,7 +2222,7 @@
     </row>
     <row r="13" spans="1:25" s="37" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="100" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B13" s="100"/>
       <c r="C13" s="100"/>
@@ -2271,13 +2272,13 @@
         <v>7</v>
       </c>
       <c r="E15" s="99" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F15" s="89" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="84" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="H15" s="82" t="s">
         <v>8</v>
@@ -2357,25 +2358,25 @@
         <v>21</v>
       </c>
       <c r="I18" s="32" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="K18" s="32" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L18" s="32" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="M18" s="32" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="N18" s="32" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="O18" s="32" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="15.5">
@@ -2420,7 +2421,7 @@
     </row>
     <row r="21" spans="1:25" s="37" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="73" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B21" s="73"/>
       <c r="C21" s="73"/>
@@ -2440,7 +2441,7 @@
     </row>
     <row r="22" spans="1:25" ht="18.5" thickBot="1">
       <c r="A22" s="76" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B22" s="77"/>
       <c r="C22" s="77"/>
@@ -2465,10 +2466,10 @@
         <v>10</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E23" s="39" t="s">
         <v>11</v>
@@ -2478,7 +2479,7 @@
       </c>
       <c r="G23" s="56"/>
       <c r="H23" s="79" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="I23" s="79"/>
       <c r="J23" s="79"/>
@@ -2491,10 +2492,10 @@
     </row>
     <row r="24" spans="1:25" ht="15.5" customHeight="1">
       <c r="A24" s="57" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C24" s="43"/>
       <c r="D24" s="44">
@@ -2510,7 +2511,7 @@
       </c>
       <c r="G24" s="56"/>
       <c r="H24" s="80" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="I24" s="80"/>
       <c r="J24" s="80"/>
@@ -2523,10 +2524,10 @@
     </row>
     <row r="25" spans="1:25" ht="18" customHeight="1">
       <c r="A25" s="57" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C25" s="43"/>
       <c r="D25" s="44">
@@ -2553,10 +2554,10 @@
     </row>
     <row r="26" spans="1:25" ht="15.5" customHeight="1">
       <c r="A26" s="57" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C26" s="43"/>
       <c r="D26" s="44">
@@ -2583,10 +2584,10 @@
     </row>
     <row r="27" spans="1:25" ht="15.5" customHeight="1">
       <c r="A27" s="57" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C27" s="43"/>
       <c r="D27" s="44">
@@ -2613,10 +2614,10 @@
     </row>
     <row r="28" spans="1:25" ht="15.5" customHeight="1">
       <c r="A28" s="57" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="44">
@@ -2643,10 +2644,10 @@
     </row>
     <row r="29" spans="1:25" ht="15" customHeight="1">
       <c r="A29" s="58" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C29" s="47"/>
       <c r="D29" s="44">
@@ -2673,10 +2674,10 @@
     </row>
     <row r="30" spans="1:25" ht="15" customHeight="1">
       <c r="A30" s="58" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="44">
@@ -2771,7 +2772,7 @@
     </row>
     <row r="33" spans="1:25" ht="18">
       <c r="A33" s="74" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B33" s="74"/>
       <c r="C33" s="74"/>
@@ -2800,17 +2801,17 @@
     </row>
     <row r="34" spans="1:25" ht="18" customHeight="1">
       <c r="A34" s="75" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B34" s="75"/>
       <c r="C34" s="75"/>
       <c r="D34" s="75"/>
       <c r="E34" s="75"/>
       <c r="F34" s="61" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
@@ -2860,11 +2861,11 @@
     </row>
     <row r="36" spans="1:25" ht="18" customHeight="1">
       <c r="A36" s="75" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B36" s="75"/>
       <c r="C36" s="75" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D36" s="75"/>
       <c r="E36" s="75"/>
@@ -2873,7 +2874,7 @@
       <c r="H36" s="17"/>
       <c r="I36" s="23"/>
       <c r="L36" s="75" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="M36" s="75"/>
       <c r="N36" s="75"/>
@@ -2889,7 +2890,7 @@
       </c>
       <c r="B37" s="75"/>
       <c r="C37" s="75" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D37" s="75"/>
       <c r="E37" s="75"/>
@@ -2898,7 +2899,7 @@
       <c r="H37" s="17"/>
       <c r="I37" s="23"/>
       <c r="L37" s="75" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="M37" s="75"/>
       <c r="N37" s="75"/>
@@ -2912,7 +2913,7 @@
       <c r="A38" s="8"/>
       <c r="B38" s="20"/>
       <c r="C38" s="78" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="D38" s="78"/>
       <c r="E38" s="78"/>
@@ -2921,7 +2922,7 @@
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
       <c r="L38" s="78" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="M38" s="78"/>
       <c r="N38" s="78"/>
@@ -2935,7 +2936,7 @@
       <c r="A39" s="8"/>
       <c r="B39" s="20"/>
       <c r="C39" s="78" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="D39" s="78"/>
       <c r="E39" s="78"/>
@@ -2944,7 +2945,7 @@
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
       <c r="L39" s="78" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="M39" s="78"/>
       <c r="N39" s="78"/>

</xml_diff>

<commit_message>
Add new Services Configuration Section to be able to switch between a few services and keep the data organized
</commit_message>
<xml_diff>
--- a/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
+++ b/Mil.Paperwork.Domain/Templates/ResidualValueReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Mil.Paperwork.WriteOff\Mil.Paperwork.Domain\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6848EC73-F779-4C55-BDB2-D44427A1000A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E1B699-A6AB-4C5E-B963-C8CF80867B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,10 +269,6 @@
     <t>Первісна вартість (графа 5 х  графу 6)                     (Вп)</t>
   </si>
   <si>
-    <t>Тимчасово виконуючий обов'язки 
-командира військової частини [MIL_UNIT]</t>
-  </si>
-  <si>
     <t>[COMM_RANK]</t>
   </si>
   <si>
@@ -304,6 +300,9 @@
   </si>
   <si>
     <t>[COMMISSION_PERSON3_NAME]</t>
+  </si>
+  <si>
+    <t>Командир військової частини [MIL_UNIT]</t>
   </si>
 </sst>
 </file>
@@ -1120,62 +1119,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1199,8 +1149,57 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1927,7 +1926,7 @@
   <dimension ref="A1:Y1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K8" sqref="K8:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2005,10 +2004,10 @@
       <c r="Y2" s="5"/>
     </row>
     <row r="3" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A3" s="93" t="s">
-        <v>64</v>
+      <c r="A3" s="76" t="s">
+        <v>63</v>
       </c>
-      <c r="B3" s="94"/>
+      <c r="B3" s="77"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2034,14 +2033,14 @@
       <c r="Y3" s="5"/>
     </row>
     <row r="4" spans="1:25" ht="12.75" customHeight="1">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="97" t="s">
+      <c r="B4" s="77"/>
+      <c r="C4" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="98"/>
+      <c r="D4" s="81"/>
       <c r="E4" s="27"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -2092,34 +2091,34 @@
       <c r="Y5" s="5"/>
     </row>
     <row r="6" spans="1:25" ht="18" customHeight="1">
-      <c r="A6" s="96"/>
-      <c r="B6" s="94"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="77"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="K6" s="92" t="s">
+      <c r="K6" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
       <c r="P6" s="20"/>
     </row>
-    <row r="7" spans="1:25" ht="34" customHeight="1">
+    <row r="7" spans="1:25" ht="18">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="K7" s="75" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
-      <c r="L7" s="92"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="92"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
       <c r="P7" s="20"/>
     </row>
     <row r="8" spans="1:25" ht="18" customHeight="1">
@@ -2128,15 +2127,15 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="K8" s="81" t="s">
+      <c r="K8" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="91" t="s">
-        <v>63</v>
-      </c>
-      <c r="O8" s="91"/>
+      <c r="O8" s="73"/>
       <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:25" ht="24.75" customHeight="1">
@@ -2145,13 +2144,13 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="K9" s="92" t="s">
+      <c r="K9" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="92"/>
-      <c r="M9" s="92"/>
-      <c r="N9" s="92"/>
-      <c r="O9" s="92"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
       <c r="P9" s="20"/>
     </row>
     <row r="10" spans="1:25" ht="18" customHeight="1">
@@ -2172,23 +2171,23 @@
       <c r="Y10" s="8"/>
     </row>
     <row r="11" spans="1:25" ht="18" customHeight="1">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="101"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="101"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="101"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -2201,61 +2200,61 @@
       <c r="Y11" s="8"/>
     </row>
     <row r="12" spans="1:25" ht="18" customHeight="1">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="100"/>
-      <c r="L12" s="100"/>
-      <c r="M12" s="100"/>
-      <c r="N12" s="100"/>
-      <c r="O12" s="100"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
       <c r="P12" s="8"/>
     </row>
     <row r="13" spans="1:25" s="37" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
-      <c r="O13" s="100"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="83"/>
+      <c r="N13" s="83"/>
+      <c r="O13" s="83"/>
       <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:25" ht="18" customHeight="1">
-      <c r="A14" s="101"/>
-      <c r="B14" s="101"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="101"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:25" ht="68" customHeight="1">
@@ -2268,19 +2267,19 @@
       <c r="C15" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="87" t="s">
+      <c r="D15" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="99" t="s">
+      <c r="E15" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="89" t="s">
+      <c r="F15" s="93" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="82" t="s">
+      <c r="H15" s="88" t="s">
         <v>8</v>
       </c>
       <c r="I15" s="28"/>
@@ -2289,14 +2288,14 @@
       <c r="O15" s="10"/>
     </row>
     <row r="16" spans="1:25" ht="24" customHeight="1">
-      <c r="A16" s="85"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="83"/>
+      <c r="A16" s="90"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="89"/>
       <c r="I16" s="16"/>
       <c r="M16" s="28"/>
       <c r="N16" s="9"/>
@@ -2420,14 +2419,14 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:25" s="37" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
       <c r="G21" s="12"/>
       <c r="H21" s="15"/>
       <c r="I21" s="13"/>
@@ -2440,14 +2439,14 @@
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:25" ht="18.5" thickBot="1">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="101"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="101"/>
       <c r="G22" s="53"/>
       <c r="H22" s="53"/>
       <c r="I22" s="53"/>
@@ -2478,16 +2477,16 @@
         <v>12</v>
       </c>
       <c r="G23" s="56"/>
-      <c r="H23" s="79" t="s">
+      <c r="H23" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="79"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="79"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
       <c r="P23" s="8"/>
     </row>
     <row r="24" spans="1:25" ht="15.5" customHeight="1">
@@ -2510,16 +2509,16 @@
         <v>0</v>
       </c>
       <c r="G24" s="56"/>
-      <c r="H24" s="80" t="s">
+      <c r="H24" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="80"/>
-      <c r="M24" s="80"/>
-      <c r="N24" s="80"/>
-      <c r="O24" s="80"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="97"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="97"/>
+      <c r="O24" s="97"/>
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:25" ht="18" customHeight="1">
@@ -2542,14 +2541,14 @@
         <v>0</v>
       </c>
       <c r="G25" s="56"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="80"/>
-      <c r="M25" s="80"/>
-      <c r="N25" s="80"/>
-      <c r="O25" s="80"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="97"/>
+      <c r="J25" s="97"/>
+      <c r="K25" s="97"/>
+      <c r="L25" s="97"/>
+      <c r="M25" s="97"/>
+      <c r="N25" s="97"/>
+      <c r="O25" s="97"/>
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:25" ht="15.5" customHeight="1">
@@ -2572,14 +2571,14 @@
         <v>0</v>
       </c>
       <c r="G26" s="56"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="80"/>
-      <c r="M26" s="80"/>
-      <c r="N26" s="80"/>
-      <c r="O26" s="80"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="97"/>
+      <c r="J26" s="97"/>
+      <c r="K26" s="97"/>
+      <c r="L26" s="97"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="97"/>
+      <c r="O26" s="97"/>
       <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:25" ht="15.5" customHeight="1">
@@ -2602,14 +2601,14 @@
         <v>0</v>
       </c>
       <c r="G27" s="56"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="80"/>
-      <c r="M27" s="80"/>
-      <c r="N27" s="80"/>
-      <c r="O27" s="80"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="97"/>
+      <c r="N27" s="97"/>
+      <c r="O27" s="97"/>
       <c r="P27" s="5"/>
     </row>
     <row r="28" spans="1:25" ht="15.5" customHeight="1">
@@ -2632,14 +2631,14 @@
         <v>0</v>
       </c>
       <c r="G28" s="56"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="80"/>
-      <c r="L28" s="80"/>
-      <c r="M28" s="80"/>
-      <c r="N28" s="80"/>
-      <c r="O28" s="80"/>
+      <c r="H28" s="97"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="97"/>
+      <c r="L28" s="97"/>
+      <c r="M28" s="97"/>
+      <c r="N28" s="97"/>
+      <c r="O28" s="97"/>
       <c r="P28" s="5"/>
     </row>
     <row r="29" spans="1:25" ht="15" customHeight="1">
@@ -2771,23 +2770,23 @@
       <c r="Y32" s="5"/>
     </row>
     <row r="33" spans="1:25" ht="18">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="74"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="99"/>
+      <c r="E33" s="99"/>
+      <c r="F33" s="99"/>
+      <c r="G33" s="99"/>
+      <c r="H33" s="99"/>
+      <c r="I33" s="99"/>
+      <c r="J33" s="99"/>
+      <c r="K33" s="99"/>
+      <c r="L33" s="99"/>
+      <c r="M33" s="99"/>
+      <c r="N33" s="99"/>
+      <c r="O33" s="99"/>
       <c r="P33" s="17"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
@@ -2865,7 +2864,7 @@
       </c>
       <c r="B36" s="75"/>
       <c r="C36" s="75" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="75"/>
       <c r="E36" s="75"/>
@@ -2874,7 +2873,7 @@
       <c r="H36" s="17"/>
       <c r="I36" s="23"/>
       <c r="L36" s="75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M36" s="75"/>
       <c r="N36" s="75"/>
@@ -2890,7 +2889,7 @@
       </c>
       <c r="B37" s="75"/>
       <c r="C37" s="75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="75"/>
       <c r="E37" s="75"/>
@@ -2899,7 +2898,7 @@
       <c r="H37" s="17"/>
       <c r="I37" s="23"/>
       <c r="L37" s="75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M37" s="75"/>
       <c r="N37" s="75"/>
@@ -2912,21 +2911,21 @@
     <row r="38" spans="1:25" ht="18" customHeight="1">
       <c r="A38" s="8"/>
       <c r="B38" s="20"/>
-      <c r="C38" s="78" t="s">
-        <v>67</v>
+      <c r="C38" s="95" t="s">
+        <v>66</v>
       </c>
-      <c r="D38" s="78"/>
-      <c r="E38" s="78"/>
+      <c r="D38" s="95"/>
+      <c r="E38" s="95"/>
       <c r="F38" s="23"/>
       <c r="G38" s="23"/>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
-      <c r="L38" s="78" t="s">
-        <v>71</v>
+      <c r="L38" s="95" t="s">
+        <v>70</v>
       </c>
-      <c r="M38" s="78"/>
-      <c r="N38" s="78"/>
-      <c r="O38" s="78"/>
+      <c r="M38" s="95"/>
+      <c r="N38" s="95"/>
+      <c r="O38" s="95"/>
       <c r="P38" s="8"/>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
@@ -2935,21 +2934,21 @@
     <row r="39" spans="1:25" ht="18" customHeight="1">
       <c r="A39" s="8"/>
       <c r="B39" s="20"/>
-      <c r="C39" s="78" t="s">
-        <v>68</v>
+      <c r="C39" s="95" t="s">
+        <v>67</v>
       </c>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="95"/>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
-      <c r="L39" s="78" t="s">
-        <v>72</v>
+      <c r="L39" s="95" t="s">
+        <v>71</v>
       </c>
-      <c r="M39" s="78"/>
-      <c r="N39" s="78"/>
-      <c r="O39" s="78"/>
+      <c r="M39" s="95"/>
+      <c r="N39" s="95"/>
+      <c r="O39" s="95"/>
       <c r="P39" s="21"/>
       <c r="Q39" s="21"/>
       <c r="R39" s="21"/>
@@ -27816,6 +27815,27 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="37">
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A33:O33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="H23:O23"/>
+    <mergeCell ref="H24:O28"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="L38:O38"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="F15:F16"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="K9:O9"/>
     <mergeCell ref="L36:O36"/>
@@ -27832,27 +27852,6 @@
     <mergeCell ref="A11:O11"/>
     <mergeCell ref="A12:O12"/>
     <mergeCell ref="A14:O14"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="H23:O23"/>
-    <mergeCell ref="H24:O28"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="L38:O38"/>
-    <mergeCell ref="L39:O39"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A33:O33"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A22:F22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>